<commit_message>
241021, oxford 10/28 09:40
</commit_message>
<xml_diff>
--- a/R/data/oxford_241021.xlsx
+++ b/R/data/oxford_241021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005824C3-0A42-174B-A822-DE1E03CB6992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3248354-BEF0-5641-B8BD-E361AA5DA069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="56280" yWindow="1360" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="846">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2491,6 +2491,76 @@
   </si>
   <si>
     <t>지소영</t>
+  </si>
+  <si>
+    <t>sehyeon0330@naver.com</t>
+  </si>
+  <si>
+    <t>김세현</t>
+  </si>
+  <si>
+    <t>withhowon@gmail.com</t>
+  </si>
+  <si>
+    <t>서호원</t>
+  </si>
+  <si>
+    <t>kter0506@naver.com</t>
+  </si>
+  <si>
+    <t>김태은</t>
+  </si>
+  <si>
+    <t>ksong1210@icloud.com</t>
+  </si>
+  <si>
+    <t>곽송</t>
+  </si>
+  <si>
+    <t>ujs4198@navre.com</t>
+  </si>
+  <si>
+    <t>엄준식</t>
+  </si>
+  <si>
+    <t>erang051216@naver.com</t>
+  </si>
+  <si>
+    <t>박이랑</t>
+  </si>
+  <si>
+    <t>ydchufd@naver.com</t>
+  </si>
+  <si>
+    <t>정유민</t>
+  </si>
+  <si>
+    <t>minuhwang16@gmail.com</t>
+  </si>
+  <si>
+    <t>황민우</t>
+  </si>
+  <si>
+    <t>gchans0524@gmail.com</t>
+  </si>
+  <si>
+    <t>한기찬</t>
+  </si>
+  <si>
+    <t>ella2005710@gmail.com</t>
+  </si>
+  <si>
+    <t>김송이</t>
+  </si>
+  <si>
+    <t>mmin121420@naver.com</t>
+  </si>
+  <si>
+    <t>김승민</t>
+  </si>
+  <si>
+    <t>언어청각학부</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2792,7 +2862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2864,6 +2934,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2913,7 +2986,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM342">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM353">
   <tableColumns count="65">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -3186,11 +3259,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM342"/>
+  <dimension ref="A1:BM353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D346" sqref="D346"/>
+      <pane ySplit="1" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D350" sqref="D350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -41801,35 +41874,1245 @@
       <c r="AJ342" s="16">
         <v>4</v>
       </c>
-      <c r="AK342" s="24"/>
-      <c r="AL342" s="24"/>
-      <c r="AM342" s="24"/>
-      <c r="AN342" s="24"/>
-      <c r="AO342" s="24"/>
-      <c r="AP342" s="24"/>
-      <c r="AQ342" s="24"/>
-      <c r="AR342" s="24"/>
-      <c r="AS342" s="24"/>
-      <c r="AT342" s="24"/>
-      <c r="AU342" s="24"/>
-      <c r="AV342" s="24"/>
-      <c r="AW342" s="24"/>
-      <c r="AX342" s="24"/>
-      <c r="AY342" s="24"/>
-      <c r="AZ342" s="24"/>
-      <c r="BA342" s="24"/>
-      <c r="BB342" s="24"/>
-      <c r="BC342" s="24"/>
-      <c r="BD342" s="24"/>
-      <c r="BE342" s="24"/>
-      <c r="BF342" s="24"/>
-      <c r="BG342" s="24"/>
-      <c r="BH342" s="24"/>
-      <c r="BI342" s="24"/>
-      <c r="BJ342" s="24"/>
-      <c r="BK342" s="24"/>
-      <c r="BL342" s="24"/>
-      <c r="BM342" s="24"/>
+    </row>
+    <row r="343" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A343" s="8">
+        <v>45593.005040219912</v>
+      </c>
+      <c r="B343" s="9" t="s">
+        <v>823</v>
+      </c>
+      <c r="C343" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D343" s="9">
+        <v>20212609</v>
+      </c>
+      <c r="E343" s="9" t="s">
+        <v>824</v>
+      </c>
+      <c r="F343" s="10">
+        <v>0</v>
+      </c>
+      <c r="G343" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H343" s="9">
+        <v>1</v>
+      </c>
+      <c r="I343" s="9">
+        <v>6</v>
+      </c>
+      <c r="J343" s="9">
+        <v>4</v>
+      </c>
+      <c r="K343" s="9">
+        <v>2</v>
+      </c>
+      <c r="L343" s="9">
+        <v>3</v>
+      </c>
+      <c r="M343" s="9">
+        <v>4</v>
+      </c>
+      <c r="N343" s="9">
+        <v>4</v>
+      </c>
+      <c r="O343" s="9">
+        <v>3</v>
+      </c>
+      <c r="P343" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q343" s="9">
+        <v>2</v>
+      </c>
+      <c r="R343" s="9">
+        <v>3</v>
+      </c>
+      <c r="S343" s="9">
+        <v>3</v>
+      </c>
+      <c r="T343" s="9">
+        <v>2</v>
+      </c>
+      <c r="U343" s="9">
+        <v>1</v>
+      </c>
+      <c r="V343" s="9">
+        <v>3</v>
+      </c>
+      <c r="W343" s="9">
+        <v>5</v>
+      </c>
+      <c r="X343" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y343" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z343" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA343" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB343" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC343" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD343" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE343" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF343" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG343" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH343" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI343" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ343" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="344" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A344" s="4">
+        <v>45593.006314988423</v>
+      </c>
+      <c r="B344" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="C344" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D344" s="5">
+        <v>20246245</v>
+      </c>
+      <c r="E344" s="5" t="s">
+        <v>826</v>
+      </c>
+      <c r="F344" s="6">
+        <v>4.8611111124046147E-3</v>
+      </c>
+      <c r="G344" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK344" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL344" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM344" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN344" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO344" s="5">
+        <v>3</v>
+      </c>
+      <c r="AP344" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ344" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR344" s="5">
+        <v>6</v>
+      </c>
+      <c r="AS344" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT344" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU344" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV344" s="5">
+        <v>6</v>
+      </c>
+      <c r="AW344" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX344" s="5">
+        <v>2</v>
+      </c>
+      <c r="AY344" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ344" s="5">
+        <v>6</v>
+      </c>
+      <c r="BA344" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB344" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC344" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD344" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE344" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF344" s="5">
+        <v>6</v>
+      </c>
+      <c r="BG344" s="5">
+        <v>2</v>
+      </c>
+      <c r="BH344" s="5">
+        <v>3</v>
+      </c>
+      <c r="BI344" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ344" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK344" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL344" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM344" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A345" s="8">
+        <v>45593.065451446761</v>
+      </c>
+      <c r="B345" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="C345" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D345" s="9">
+        <v>20243813</v>
+      </c>
+      <c r="E345" s="9" t="s">
+        <v>828</v>
+      </c>
+      <c r="F345" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G345" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK345" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL345" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM345" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN345" s="9">
+        <v>6</v>
+      </c>
+      <c r="AO345" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP345" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ345" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR345" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS345" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT345" s="9">
+        <v>4</v>
+      </c>
+      <c r="AU345" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV345" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW345" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX345" s="9">
+        <v>4</v>
+      </c>
+      <c r="AY345" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ345" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA345" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB345" s="9">
+        <v>5</v>
+      </c>
+      <c r="BC345" s="9">
+        <v>4</v>
+      </c>
+      <c r="BD345" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE345" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF345" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG345" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH345" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI345" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ345" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK345" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL345" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM345" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A346" s="4">
+        <v>45593.083512650468</v>
+      </c>
+      <c r="B346" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="C346" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D346" s="5">
+        <v>20242304</v>
+      </c>
+      <c r="E346" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="F346" s="6">
+        <v>8.1250000002910383E-2</v>
+      </c>
+      <c r="G346" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H346" s="5">
+        <v>4</v>
+      </c>
+      <c r="I346" s="5">
+        <v>5</v>
+      </c>
+      <c r="J346" s="5">
+        <v>3</v>
+      </c>
+      <c r="K346" s="5">
+        <v>4</v>
+      </c>
+      <c r="L346" s="5">
+        <v>2</v>
+      </c>
+      <c r="M346" s="5">
+        <v>5</v>
+      </c>
+      <c r="N346" s="5">
+        <v>4</v>
+      </c>
+      <c r="O346" s="5">
+        <v>3</v>
+      </c>
+      <c r="P346" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q346" s="5">
+        <v>2</v>
+      </c>
+      <c r="R346" s="5">
+        <v>5</v>
+      </c>
+      <c r="S346" s="5">
+        <v>5</v>
+      </c>
+      <c r="T346" s="5">
+        <v>4</v>
+      </c>
+      <c r="U346" s="5">
+        <v>5</v>
+      </c>
+      <c r="V346" s="5">
+        <v>4</v>
+      </c>
+      <c r="W346" s="5">
+        <v>5</v>
+      </c>
+      <c r="X346" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y346" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z346" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA346" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB346" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC346" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD346" s="5">
+        <v>6</v>
+      </c>
+      <c r="AE346" s="5">
+        <v>5</v>
+      </c>
+      <c r="AF346" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG346" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH346" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI346" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ346" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="347" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A347" s="8">
+        <v>45593.103460914353</v>
+      </c>
+      <c r="B347" s="9" t="s">
+        <v>831</v>
+      </c>
+      <c r="C347" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D347" s="9">
+        <v>20197118</v>
+      </c>
+      <c r="E347" s="9" t="s">
+        <v>832</v>
+      </c>
+      <c r="F347" s="10">
+        <v>0.101388888884685</v>
+      </c>
+      <c r="G347" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK347" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL347" s="9">
+        <v>4</v>
+      </c>
+      <c r="AM347" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN347" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO347" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP347" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ347" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR347" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS347" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT347" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU347" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV347" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW347" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX347" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY347" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ347" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA347" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB347" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC347" s="9">
+        <v>4</v>
+      </c>
+      <c r="BD347" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE347" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF347" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG347" s="9">
+        <v>4</v>
+      </c>
+      <c r="BH347" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI347" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ347" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK347" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL347" s="9">
+        <v>4</v>
+      </c>
+      <c r="BM347" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="348" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A348" s="4">
+        <v>45593.107033773151</v>
+      </c>
+      <c r="B348" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="C348" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D348" s="5">
+        <v>20243223</v>
+      </c>
+      <c r="E348" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="F348" s="6">
+        <v>9.9999999998544808E-2</v>
+      </c>
+      <c r="G348" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK348" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL348" s="5">
+        <v>2</v>
+      </c>
+      <c r="AM348" s="5">
+        <v>2</v>
+      </c>
+      <c r="AN348" s="5">
+        <v>2</v>
+      </c>
+      <c r="AO348" s="5">
+        <v>1</v>
+      </c>
+      <c r="AP348" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ348" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR348" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS348" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT348" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU348" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV348" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW348" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX348" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY348" s="5">
+        <v>2</v>
+      </c>
+      <c r="AZ348" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA348" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB348" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC348" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD348" s="5">
+        <v>2</v>
+      </c>
+      <c r="BE348" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF348" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG348" s="5">
+        <v>3</v>
+      </c>
+      <c r="BH348" s="5">
+        <v>5</v>
+      </c>
+      <c r="BI348" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ348" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK348" s="5">
+        <v>3</v>
+      </c>
+      <c r="BL348" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM348" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A349" s="8">
+        <v>45593.109136053245</v>
+      </c>
+      <c r="B349" s="9" t="s">
+        <v>835</v>
+      </c>
+      <c r="C349" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="D349" s="9">
+        <v>20242363</v>
+      </c>
+      <c r="E349" s="9" t="s">
+        <v>836</v>
+      </c>
+      <c r="F349" s="10">
+        <v>0.10416666666424135</v>
+      </c>
+      <c r="G349" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H349" s="9">
+        <v>2</v>
+      </c>
+      <c r="I349" s="9">
+        <v>5</v>
+      </c>
+      <c r="J349" s="9">
+        <v>5</v>
+      </c>
+      <c r="K349" s="9">
+        <v>5</v>
+      </c>
+      <c r="L349" s="9">
+        <v>2</v>
+      </c>
+      <c r="M349" s="9">
+        <v>5</v>
+      </c>
+      <c r="N349" s="9">
+        <v>2</v>
+      </c>
+      <c r="O349" s="9">
+        <v>4</v>
+      </c>
+      <c r="P349" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q349" s="9">
+        <v>3</v>
+      </c>
+      <c r="R349" s="9">
+        <v>5</v>
+      </c>
+      <c r="S349" s="9">
+        <v>5</v>
+      </c>
+      <c r="T349" s="9">
+        <v>2</v>
+      </c>
+      <c r="U349" s="9">
+        <v>5</v>
+      </c>
+      <c r="V349" s="9">
+        <v>5</v>
+      </c>
+      <c r="W349" s="9">
+        <v>6</v>
+      </c>
+      <c r="X349" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y349" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z349" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA349" s="9">
+        <v>2</v>
+      </c>
+      <c r="AB349" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC349" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD349" s="9">
+        <v>6</v>
+      </c>
+      <c r="AE349" s="9">
+        <v>2</v>
+      </c>
+      <c r="AF349" s="9">
+        <v>6</v>
+      </c>
+      <c r="AG349" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH349" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI349" s="9">
+        <v>4</v>
+      </c>
+      <c r="AJ349" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="350" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A350" s="4">
+        <v>45593.117175706022</v>
+      </c>
+      <c r="B350" s="5" t="s">
+        <v>837</v>
+      </c>
+      <c r="C350" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="D350" s="5">
+        <v>20243967</v>
+      </c>
+      <c r="E350" s="5" t="s">
+        <v>838</v>
+      </c>
+      <c r="F350" s="6">
+        <v>0.11666666666860692</v>
+      </c>
+      <c r="G350" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H350" s="5">
+        <v>3</v>
+      </c>
+      <c r="I350" s="5">
+        <v>3</v>
+      </c>
+      <c r="J350" s="5">
+        <v>3</v>
+      </c>
+      <c r="K350" s="5">
+        <v>3</v>
+      </c>
+      <c r="L350" s="5">
+        <v>3</v>
+      </c>
+      <c r="M350" s="5">
+        <v>3</v>
+      </c>
+      <c r="N350" s="5">
+        <v>3</v>
+      </c>
+      <c r="O350" s="5">
+        <v>3</v>
+      </c>
+      <c r="P350" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q350" s="5">
+        <v>3</v>
+      </c>
+      <c r="R350" s="5">
+        <v>3</v>
+      </c>
+      <c r="S350" s="5">
+        <v>3</v>
+      </c>
+      <c r="T350" s="5">
+        <v>3</v>
+      </c>
+      <c r="U350" s="5">
+        <v>2</v>
+      </c>
+      <c r="V350" s="5">
+        <v>3</v>
+      </c>
+      <c r="W350" s="5">
+        <v>3</v>
+      </c>
+      <c r="X350" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y350" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z350" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA350" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB350" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC350" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD350" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE350" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF350" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG350" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH350" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI350" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ350" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A351" s="8">
+        <v>45593.147527488429</v>
+      </c>
+      <c r="B351" s="9" t="s">
+        <v>839</v>
+      </c>
+      <c r="C351" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D351" s="9">
+        <v>20244152</v>
+      </c>
+      <c r="E351" s="9" t="s">
+        <v>840</v>
+      </c>
+      <c r="F351" s="10">
+        <v>0.14583333333575865</v>
+      </c>
+      <c r="G351" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H351" s="9">
+        <v>1</v>
+      </c>
+      <c r="I351" s="9">
+        <v>5</v>
+      </c>
+      <c r="J351" s="9">
+        <v>6</v>
+      </c>
+      <c r="K351" s="9">
+        <v>6</v>
+      </c>
+      <c r="L351" s="9">
+        <v>2</v>
+      </c>
+      <c r="M351" s="9">
+        <v>3</v>
+      </c>
+      <c r="N351" s="9">
+        <v>6</v>
+      </c>
+      <c r="O351" s="9">
+        <v>6</v>
+      </c>
+      <c r="P351" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q351" s="9">
+        <v>1</v>
+      </c>
+      <c r="R351" s="9">
+        <v>6</v>
+      </c>
+      <c r="S351" s="9">
+        <v>6</v>
+      </c>
+      <c r="T351" s="9">
+        <v>1</v>
+      </c>
+      <c r="U351" s="9">
+        <v>1</v>
+      </c>
+      <c r="V351" s="9">
+        <v>6</v>
+      </c>
+      <c r="W351" s="9">
+        <v>6</v>
+      </c>
+      <c r="X351" s="9">
+        <v>6</v>
+      </c>
+      <c r="Y351" s="9">
+        <v>6</v>
+      </c>
+      <c r="Z351" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA351" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB351" s="9">
+        <v>6</v>
+      </c>
+      <c r="AC351" s="9">
+        <v>6</v>
+      </c>
+      <c r="AD351" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE351" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF351" s="9">
+        <v>6</v>
+      </c>
+      <c r="AG351" s="9">
+        <v>6</v>
+      </c>
+      <c r="AH351" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI351" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ351" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A352" s="4">
+        <v>45593.230722222223</v>
+      </c>
+      <c r="B352" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="C352" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D352" s="5">
+        <v>20246222</v>
+      </c>
+      <c r="E352" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="F352" s="6">
+        <v>0.22916666666424135</v>
+      </c>
+      <c r="G352" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK352" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL352" s="5">
+        <v>2</v>
+      </c>
+      <c r="AM352" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN352" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO352" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP352" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ352" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR352" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS352" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT352" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU352" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV352" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW352" s="5">
+        <v>2</v>
+      </c>
+      <c r="AX352" s="5">
+        <v>1</v>
+      </c>
+      <c r="AY352" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ352" s="5">
+        <v>6</v>
+      </c>
+      <c r="BA352" s="5">
+        <v>6</v>
+      </c>
+      <c r="BB352" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC352" s="5">
+        <v>1</v>
+      </c>
+      <c r="BD352" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE352" s="5">
+        <v>1</v>
+      </c>
+      <c r="BF352" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG352" s="5">
+        <v>2</v>
+      </c>
+      <c r="BH352" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI352" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ352" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK352" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL352" s="5">
+        <v>2</v>
+      </c>
+      <c r="BM352" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="353" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A353" s="18">
+        <v>45593.321597060189</v>
+      </c>
+      <c r="B353" s="19" t="s">
+        <v>843</v>
+      </c>
+      <c r="C353" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D353" s="19">
+        <v>20244110</v>
+      </c>
+      <c r="E353" s="19" t="s">
+        <v>844</v>
+      </c>
+      <c r="F353" s="20">
+        <v>0.29027777777810115</v>
+      </c>
+      <c r="G353" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H353" s="19">
+        <v>4</v>
+      </c>
+      <c r="I353" s="19">
+        <v>4</v>
+      </c>
+      <c r="J353" s="19">
+        <v>4</v>
+      </c>
+      <c r="K353" s="19">
+        <v>4</v>
+      </c>
+      <c r="L353" s="19">
+        <v>4</v>
+      </c>
+      <c r="M353" s="19">
+        <v>4</v>
+      </c>
+      <c r="N353" s="19">
+        <v>4</v>
+      </c>
+      <c r="O353" s="19">
+        <v>4</v>
+      </c>
+      <c r="P353" s="19">
+        <v>4</v>
+      </c>
+      <c r="Q353" s="19">
+        <v>4</v>
+      </c>
+      <c r="R353" s="19">
+        <v>4</v>
+      </c>
+      <c r="S353" s="19">
+        <v>4</v>
+      </c>
+      <c r="T353" s="19">
+        <v>4</v>
+      </c>
+      <c r="U353" s="19">
+        <v>4</v>
+      </c>
+      <c r="V353" s="19">
+        <v>4</v>
+      </c>
+      <c r="W353" s="19">
+        <v>4</v>
+      </c>
+      <c r="X353" s="19">
+        <v>4</v>
+      </c>
+      <c r="Y353" s="19">
+        <v>4</v>
+      </c>
+      <c r="Z353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AA353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AB353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AC353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AD353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AE353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AF353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AG353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AH353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AI353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AJ353" s="19">
+        <v>4</v>
+      </c>
+      <c r="AK353" s="24"/>
+      <c r="AL353" s="24"/>
+      <c r="AM353" s="24"/>
+      <c r="AN353" s="24"/>
+      <c r="AO353" s="24"/>
+      <c r="AP353" s="24"/>
+      <c r="AQ353" s="24"/>
+      <c r="AR353" s="24"/>
+      <c r="AS353" s="24"/>
+      <c r="AT353" s="24"/>
+      <c r="AU353" s="24"/>
+      <c r="AV353" s="24"/>
+      <c r="AW353" s="24"/>
+      <c r="AX353" s="24"/>
+      <c r="AY353" s="24"/>
+      <c r="AZ353" s="24"/>
+      <c r="BA353" s="24"/>
+      <c r="BB353" s="24"/>
+      <c r="BC353" s="24"/>
+      <c r="BD353" s="24"/>
+      <c r="BE353" s="24"/>
+      <c r="BF353" s="24"/>
+      <c r="BG353" s="24"/>
+      <c r="BH353" s="24"/>
+      <c r="BI353" s="24"/>
+      <c r="BJ353" s="24"/>
+      <c r="BK353" s="24"/>
+      <c r="BL353" s="24"/>
+      <c r="BM353" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
oxford, 241021 modified 10/30 09:16
</commit_message>
<xml_diff>
--- a/R/data/oxford_241021.xlsx
+++ b/R/data/oxford_241021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BE626B-B754-D54C-A834-A7155D0863E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F379F3D-7211-D943-AEA6-7E7D95D4AD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="56280" yWindow="1360" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="931">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2696,6 +2696,126 @@
   </si>
   <si>
     <t>서준석</t>
+  </si>
+  <si>
+    <t>jiah1622@naver.com</t>
+  </si>
+  <si>
+    <t>최지아</t>
+  </si>
+  <si>
+    <t>r67890@naver.com</t>
+  </si>
+  <si>
+    <t>이규형</t>
+  </si>
+  <si>
+    <t>jym85362@naver.com</t>
+  </si>
+  <si>
+    <t>유수현</t>
+  </si>
+  <si>
+    <t>jklucky09@naver.com</t>
+  </si>
+  <si>
+    <t>최준근</t>
+  </si>
+  <si>
+    <t>junseok5310@naver.com</t>
+  </si>
+  <si>
+    <t>오준석</t>
+  </si>
+  <si>
+    <t>leyy2k@naver.com</t>
+  </si>
+  <si>
+    <t>김대현</t>
+  </si>
+  <si>
+    <t>schoe357@gmail.com</t>
+  </si>
+  <si>
+    <t>최성민</t>
+  </si>
+  <si>
+    <t>dabinchoe05@gmail.com</t>
+  </si>
+  <si>
+    <t>최다빈</t>
+  </si>
+  <si>
+    <t>imhyeongu00@gmail.com</t>
+  </si>
+  <si>
+    <t>언론방송융합미디어전공</t>
+  </si>
+  <si>
+    <t>임현구</t>
+  </si>
+  <si>
+    <t>jione0831@naver.com</t>
+  </si>
+  <si>
+    <t>윤지원</t>
+  </si>
+  <si>
+    <t>yeel6945@naver.com</t>
+  </si>
+  <si>
+    <t>이수빈</t>
+  </si>
+  <si>
+    <t>joazzzzz@naver.com</t>
+  </si>
+  <si>
+    <t>김진구</t>
+  </si>
+  <si>
+    <t>yongwoo7701@gmail.com</t>
+  </si>
+  <si>
+    <t>유용우</t>
+  </si>
+  <si>
+    <t>csm06125@naver.com</t>
+  </si>
+  <si>
+    <t>박근태</t>
+  </si>
+  <si>
+    <t>cindy_lol@naver.com</t>
+  </si>
+  <si>
+    <t>권한별</t>
+  </si>
+  <si>
+    <t>ksy91637@gmail.com</t>
+  </si>
+  <si>
+    <t>스마트IOT</t>
+  </si>
+  <si>
+    <t>김성열</t>
+  </si>
+  <si>
+    <t>ohsolbi050521@gmail.com</t>
+  </si>
+  <si>
+    <t>오솔비</t>
+  </si>
+  <si>
+    <t>lucas3767@naver.com</t>
+  </si>
+  <si>
+    <t>권민재</t>
+  </si>
+  <si>
+    <t>msy123581@naver.com</t>
+  </si>
+  <si>
+    <t>문신영</t>
   </si>
 </sst>
 </file>
@@ -3121,7 +3241,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM374">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM393">
   <tableColumns count="65">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -3394,11 +3514,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM374"/>
+  <dimension ref="A1:BM393"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A380" sqref="A380"/>
+      <pane ySplit="1" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C399" sqref="C399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -45529,35 +45649,2125 @@
       <c r="AJ374" s="16">
         <v>1</v>
       </c>
-      <c r="AK374" s="25"/>
-      <c r="AL374" s="25"/>
-      <c r="AM374" s="25"/>
-      <c r="AN374" s="25"/>
-      <c r="AO374" s="25"/>
-      <c r="AP374" s="25"/>
-      <c r="AQ374" s="25"/>
-      <c r="AR374" s="25"/>
-      <c r="AS374" s="25"/>
-      <c r="AT374" s="25"/>
-      <c r="AU374" s="25"/>
-      <c r="AV374" s="25"/>
-      <c r="AW374" s="25"/>
-      <c r="AX374" s="25"/>
-      <c r="AY374" s="25"/>
-      <c r="AZ374" s="25"/>
-      <c r="BA374" s="25"/>
-      <c r="BB374" s="25"/>
-      <c r="BC374" s="25"/>
-      <c r="BD374" s="25"/>
-      <c r="BE374" s="25"/>
-      <c r="BF374" s="25"/>
-      <c r="BG374" s="25"/>
-      <c r="BH374" s="25"/>
-      <c r="BI374" s="25"/>
-      <c r="BJ374" s="25"/>
-      <c r="BK374" s="25"/>
-      <c r="BL374" s="25"/>
-      <c r="BM374" s="25"/>
+    </row>
+    <row r="375" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A375" s="8">
+        <v>45594.451676770834</v>
+      </c>
+      <c r="B375" s="9" t="s">
+        <v>891</v>
+      </c>
+      <c r="C375" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D375" s="9">
+        <v>20245271</v>
+      </c>
+      <c r="E375" s="9" t="s">
+        <v>892</v>
+      </c>
+      <c r="F375" s="10">
+        <v>0.44652777777810115</v>
+      </c>
+      <c r="G375" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK375" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL375" s="9">
+        <v>4</v>
+      </c>
+      <c r="AM375" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN375" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO375" s="9">
+        <v>2</v>
+      </c>
+      <c r="AP375" s="9">
+        <v>2</v>
+      </c>
+      <c r="AQ375" s="9">
+        <v>4</v>
+      </c>
+      <c r="AR375" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS375" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT375" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU375" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV375" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW375" s="9">
+        <v>1</v>
+      </c>
+      <c r="AX375" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY375" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ375" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA375" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB375" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC375" s="9">
+        <v>1</v>
+      </c>
+      <c r="BD375" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE375" s="9">
+        <v>1</v>
+      </c>
+      <c r="BF375" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG375" s="9">
+        <v>1</v>
+      </c>
+      <c r="BH375" s="9">
+        <v>1</v>
+      </c>
+      <c r="BI375" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ375" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK375" s="9">
+        <v>1</v>
+      </c>
+      <c r="BL375" s="9">
+        <v>1</v>
+      </c>
+      <c r="BM375" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A376" s="4">
+        <v>45594.474792858797</v>
+      </c>
+      <c r="B376" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="C376" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="D376" s="5">
+        <v>20205217</v>
+      </c>
+      <c r="E376" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="F376" s="6">
+        <v>0.47291666666569654</v>
+      </c>
+      <c r="G376" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H376" s="5">
+        <v>1</v>
+      </c>
+      <c r="I376" s="5">
+        <v>5</v>
+      </c>
+      <c r="J376" s="5">
+        <v>5</v>
+      </c>
+      <c r="K376" s="5">
+        <v>4</v>
+      </c>
+      <c r="L376" s="5">
+        <v>1</v>
+      </c>
+      <c r="M376" s="5">
+        <v>2</v>
+      </c>
+      <c r="N376" s="5">
+        <v>5</v>
+      </c>
+      <c r="O376" s="5">
+        <v>3</v>
+      </c>
+      <c r="P376" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q376" s="5">
+        <v>3</v>
+      </c>
+      <c r="R376" s="5">
+        <v>5</v>
+      </c>
+      <c r="S376" s="5">
+        <v>5</v>
+      </c>
+      <c r="T376" s="5">
+        <v>2</v>
+      </c>
+      <c r="U376" s="5">
+        <v>3</v>
+      </c>
+      <c r="V376" s="5">
+        <v>5</v>
+      </c>
+      <c r="W376" s="5">
+        <v>4</v>
+      </c>
+      <c r="X376" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y376" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z376" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA376" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB376" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC376" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD376" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE376" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF376" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG376" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH376" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI376" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ376" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A377" s="8">
+        <v>45594.511361342593</v>
+      </c>
+      <c r="B377" s="9" t="s">
+        <v>895</v>
+      </c>
+      <c r="C377" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="D377" s="9">
+        <v>20243234</v>
+      </c>
+      <c r="E377" s="9" t="s">
+        <v>896</v>
+      </c>
+      <c r="F377" s="10">
+        <v>1.0416666664241347E-2</v>
+      </c>
+      <c r="G377" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H377" s="9">
+        <v>1</v>
+      </c>
+      <c r="I377" s="9">
+        <v>3</v>
+      </c>
+      <c r="J377" s="9">
+        <v>3</v>
+      </c>
+      <c r="K377" s="9">
+        <v>3</v>
+      </c>
+      <c r="L377" s="9">
+        <v>3</v>
+      </c>
+      <c r="M377" s="9">
+        <v>3</v>
+      </c>
+      <c r="N377" s="9">
+        <v>3</v>
+      </c>
+      <c r="O377" s="9">
+        <v>3</v>
+      </c>
+      <c r="P377" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q377" s="9">
+        <v>3</v>
+      </c>
+      <c r="R377" s="9">
+        <v>3</v>
+      </c>
+      <c r="S377" s="9">
+        <v>3</v>
+      </c>
+      <c r="T377" s="9">
+        <v>3</v>
+      </c>
+      <c r="U377" s="9">
+        <v>3</v>
+      </c>
+      <c r="V377" s="9">
+        <v>3</v>
+      </c>
+      <c r="W377" s="9">
+        <v>3</v>
+      </c>
+      <c r="X377" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y377" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI377" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ377" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="378" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A378" s="4">
+        <v>45594.554153611112</v>
+      </c>
+      <c r="B378" s="5" t="s">
+        <v>897</v>
+      </c>
+      <c r="C378" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D378" s="5">
+        <v>20171101</v>
+      </c>
+      <c r="E378" s="5" t="s">
+        <v>898</v>
+      </c>
+      <c r="F378" s="6">
+        <v>0.5506944444423425</v>
+      </c>
+      <c r="G378" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H378" s="5">
+        <v>4</v>
+      </c>
+      <c r="I378" s="5">
+        <v>4</v>
+      </c>
+      <c r="J378" s="5">
+        <v>2</v>
+      </c>
+      <c r="K378" s="5">
+        <v>2</v>
+      </c>
+      <c r="L378" s="5">
+        <v>4</v>
+      </c>
+      <c r="M378" s="5">
+        <v>4</v>
+      </c>
+      <c r="N378" s="5">
+        <v>3</v>
+      </c>
+      <c r="O378" s="5">
+        <v>2</v>
+      </c>
+      <c r="P378" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q378" s="5">
+        <v>5</v>
+      </c>
+      <c r="R378" s="5">
+        <v>4</v>
+      </c>
+      <c r="S378" s="5">
+        <v>4</v>
+      </c>
+      <c r="T378" s="5">
+        <v>2</v>
+      </c>
+      <c r="U378" s="5">
+        <v>3</v>
+      </c>
+      <c r="V378" s="5">
+        <v>3</v>
+      </c>
+      <c r="W378" s="5">
+        <v>3</v>
+      </c>
+      <c r="X378" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y378" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z378" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA378" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB378" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC378" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD378" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE378" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF378" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG378" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH378" s="5">
+        <v>4</v>
+      </c>
+      <c r="AI378" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ378" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="379" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A379" s="8">
+        <v>45594.569208483794</v>
+      </c>
+      <c r="B379" s="9" t="s">
+        <v>899</v>
+      </c>
+      <c r="C379" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D379" s="9">
+        <v>20193626</v>
+      </c>
+      <c r="E379" s="9" t="s">
+        <v>900</v>
+      </c>
+      <c r="F379" s="10">
+        <v>0.56805555555911269</v>
+      </c>
+      <c r="G379" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK379" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL379" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM379" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN379" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO379" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP379" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ379" s="9">
+        <v>5</v>
+      </c>
+      <c r="AR379" s="9">
+        <v>5</v>
+      </c>
+      <c r="AS379" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT379" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU379" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV379" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW379" s="9">
+        <v>4</v>
+      </c>
+      <c r="AX379" s="9">
+        <v>4</v>
+      </c>
+      <c r="AY379" s="9">
+        <v>5</v>
+      </c>
+      <c r="AZ379" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA379" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB379" s="9">
+        <v>5</v>
+      </c>
+      <c r="BC379" s="9">
+        <v>5</v>
+      </c>
+      <c r="BD379" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE379" s="9">
+        <v>5</v>
+      </c>
+      <c r="BF379" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG379" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH379" s="9">
+        <v>5</v>
+      </c>
+      <c r="BI379" s="9">
+        <v>5</v>
+      </c>
+      <c r="BJ379" s="9">
+        <v>5</v>
+      </c>
+      <c r="BK379" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL379" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM379" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="380" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A380" s="4">
+        <v>45594.584256377319</v>
+      </c>
+      <c r="B380" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="C380" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D380" s="5">
+        <v>20215115</v>
+      </c>
+      <c r="E380" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="F380" s="6">
+        <v>0.58333333333575865</v>
+      </c>
+      <c r="G380" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H380" s="5">
+        <v>4</v>
+      </c>
+      <c r="I380" s="5">
+        <v>5</v>
+      </c>
+      <c r="J380" s="5">
+        <v>4</v>
+      </c>
+      <c r="K380" s="5">
+        <v>4</v>
+      </c>
+      <c r="L380" s="5">
+        <v>5</v>
+      </c>
+      <c r="M380" s="5">
+        <v>3</v>
+      </c>
+      <c r="N380" s="5">
+        <v>4</v>
+      </c>
+      <c r="O380" s="5">
+        <v>5</v>
+      </c>
+      <c r="P380" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q380" s="5">
+        <v>2</v>
+      </c>
+      <c r="R380" s="5">
+        <v>4</v>
+      </c>
+      <c r="S380" s="5">
+        <v>3</v>
+      </c>
+      <c r="T380" s="5">
+        <v>3</v>
+      </c>
+      <c r="U380" s="5">
+        <v>5</v>
+      </c>
+      <c r="V380" s="5">
+        <v>4</v>
+      </c>
+      <c r="W380" s="5">
+        <v>4</v>
+      </c>
+      <c r="X380" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y380" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z380" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA380" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB380" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC380" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD380" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE380" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF380" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG380" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH380" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI380" s="5">
+        <v>4</v>
+      </c>
+      <c r="AJ380" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="381" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A381" s="8">
+        <v>45594.711408240742</v>
+      </c>
+      <c r="B381" s="9" t="s">
+        <v>903</v>
+      </c>
+      <c r="C381" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D381" s="9">
+        <v>20246782</v>
+      </c>
+      <c r="E381" s="9" t="s">
+        <v>904</v>
+      </c>
+      <c r="F381" s="10">
+        <v>0.70833333333575865</v>
+      </c>
+      <c r="G381" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H381" s="9">
+        <v>3</v>
+      </c>
+      <c r="I381" s="9">
+        <v>2</v>
+      </c>
+      <c r="J381" s="9">
+        <v>4</v>
+      </c>
+      <c r="K381" s="9">
+        <v>2</v>
+      </c>
+      <c r="L381" s="9">
+        <v>5</v>
+      </c>
+      <c r="M381" s="9">
+        <v>3</v>
+      </c>
+      <c r="N381" s="9">
+        <v>5</v>
+      </c>
+      <c r="O381" s="9">
+        <v>3</v>
+      </c>
+      <c r="P381" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q381" s="9">
+        <v>4</v>
+      </c>
+      <c r="R381" s="9">
+        <v>4</v>
+      </c>
+      <c r="S381" s="9">
+        <v>2</v>
+      </c>
+      <c r="T381" s="9">
+        <v>2</v>
+      </c>
+      <c r="U381" s="9">
+        <v>4</v>
+      </c>
+      <c r="V381" s="9">
+        <v>5</v>
+      </c>
+      <c r="W381" s="9">
+        <v>4</v>
+      </c>
+      <c r="X381" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y381" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z381" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA381" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB381" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC381" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD381" s="9">
+        <v>5</v>
+      </c>
+      <c r="AE381" s="9">
+        <v>6</v>
+      </c>
+      <c r="AF381" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG381" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH381" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI381" s="9">
+        <v>4</v>
+      </c>
+      <c r="AJ381" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="382" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A382" s="4">
+        <v>45594.711838020834</v>
+      </c>
+      <c r="B382" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="C382" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D382" s="5">
+        <v>20246780</v>
+      </c>
+      <c r="E382" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="F382" s="6">
+        <v>0.70902777777519077</v>
+      </c>
+      <c r="G382" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H382" s="5">
+        <v>4</v>
+      </c>
+      <c r="I382" s="5">
+        <v>2</v>
+      </c>
+      <c r="J382" s="5">
+        <v>4</v>
+      </c>
+      <c r="K382" s="5">
+        <v>3</v>
+      </c>
+      <c r="L382" s="5">
+        <v>3</v>
+      </c>
+      <c r="M382" s="5">
+        <v>4</v>
+      </c>
+      <c r="N382" s="5">
+        <v>2</v>
+      </c>
+      <c r="O382" s="5">
+        <v>4</v>
+      </c>
+      <c r="P382" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q382" s="5">
+        <v>5</v>
+      </c>
+      <c r="R382" s="5">
+        <v>5</v>
+      </c>
+      <c r="S382" s="5">
+        <v>2</v>
+      </c>
+      <c r="T382" s="5">
+        <v>3</v>
+      </c>
+      <c r="U382" s="5">
+        <v>4</v>
+      </c>
+      <c r="V382" s="5">
+        <v>4</v>
+      </c>
+      <c r="W382" s="5">
+        <v>4</v>
+      </c>
+      <c r="X382" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y382" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z382" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA382" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB382" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC382" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD382" s="5">
+        <v>5</v>
+      </c>
+      <c r="AE382" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF382" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG382" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH382" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI382" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ382" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="383" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A383" s="8">
+        <v>45594.729087615742</v>
+      </c>
+      <c r="B383" s="9" t="s">
+        <v>907</v>
+      </c>
+      <c r="C383" s="9" t="s">
+        <v>908</v>
+      </c>
+      <c r="D383" s="9">
+        <v>20192575</v>
+      </c>
+      <c r="E383" s="9" t="s">
+        <v>909</v>
+      </c>
+      <c r="F383" s="10">
+        <v>0.72916666666424135</v>
+      </c>
+      <c r="G383" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H383" s="9">
+        <v>1</v>
+      </c>
+      <c r="I383" s="9">
+        <v>5</v>
+      </c>
+      <c r="J383" s="9">
+        <v>5</v>
+      </c>
+      <c r="K383" s="9">
+        <v>4</v>
+      </c>
+      <c r="L383" s="9">
+        <v>1</v>
+      </c>
+      <c r="M383" s="9">
+        <v>2</v>
+      </c>
+      <c r="N383" s="9">
+        <v>5</v>
+      </c>
+      <c r="O383" s="9">
+        <v>5</v>
+      </c>
+      <c r="P383" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q383" s="9">
+        <v>2</v>
+      </c>
+      <c r="R383" s="9">
+        <v>5</v>
+      </c>
+      <c r="S383" s="9">
+        <v>4</v>
+      </c>
+      <c r="T383" s="9">
+        <v>2</v>
+      </c>
+      <c r="U383" s="9">
+        <v>2</v>
+      </c>
+      <c r="V383" s="9">
+        <v>5</v>
+      </c>
+      <c r="W383" s="9">
+        <v>5</v>
+      </c>
+      <c r="X383" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y383" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z383" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA383" s="9">
+        <v>6</v>
+      </c>
+      <c r="AB383" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC383" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD383" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE383" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF383" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG383" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH383" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI383" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ383" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A384" s="4">
+        <v>45594.807016712963</v>
+      </c>
+      <c r="B384" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="C384" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D384" s="5">
+        <v>20246262</v>
+      </c>
+      <c r="E384" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="F384" s="6">
+        <v>0.80416666666860692</v>
+      </c>
+      <c r="G384" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H384" s="5">
+        <v>4</v>
+      </c>
+      <c r="I384" s="5">
+        <v>2</v>
+      </c>
+      <c r="J384" s="5">
+        <v>2</v>
+      </c>
+      <c r="K384" s="5">
+        <v>3</v>
+      </c>
+      <c r="L384" s="5">
+        <v>2</v>
+      </c>
+      <c r="M384" s="5">
+        <v>4</v>
+      </c>
+      <c r="N384" s="5">
+        <v>1</v>
+      </c>
+      <c r="O384" s="5">
+        <v>1</v>
+      </c>
+      <c r="P384" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q384" s="5">
+        <v>5</v>
+      </c>
+      <c r="R384" s="5">
+        <v>5</v>
+      </c>
+      <c r="S384" s="5">
+        <v>2</v>
+      </c>
+      <c r="T384" s="5">
+        <v>3</v>
+      </c>
+      <c r="U384" s="5">
+        <v>5</v>
+      </c>
+      <c r="V384" s="5">
+        <v>2</v>
+      </c>
+      <c r="W384" s="5">
+        <v>5</v>
+      </c>
+      <c r="X384" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y384" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z384" s="5">
+        <v>6</v>
+      </c>
+      <c r="AA384" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB384" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC384" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD384" s="5">
+        <v>5</v>
+      </c>
+      <c r="AE384" s="5">
+        <v>5</v>
+      </c>
+      <c r="AF384" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG384" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH384" s="5">
+        <v>4</v>
+      </c>
+      <c r="AI384" s="5">
+        <v>5</v>
+      </c>
+      <c r="AJ384" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="385" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A385" s="8">
+        <v>45594.871521261579</v>
+      </c>
+      <c r="B385" s="9" t="s">
+        <v>912</v>
+      </c>
+      <c r="C385" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D385" s="9">
+        <v>20203635</v>
+      </c>
+      <c r="E385" s="9" t="s">
+        <v>913</v>
+      </c>
+      <c r="F385" s="10">
+        <v>0.87083333333430346</v>
+      </c>
+      <c r="G385" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H385" s="9">
+        <v>4</v>
+      </c>
+      <c r="I385" s="9">
+        <v>4</v>
+      </c>
+      <c r="J385" s="9">
+        <v>4</v>
+      </c>
+      <c r="K385" s="9">
+        <v>4</v>
+      </c>
+      <c r="L385" s="9">
+        <v>4</v>
+      </c>
+      <c r="M385" s="9">
+        <v>4</v>
+      </c>
+      <c r="N385" s="9">
+        <v>4</v>
+      </c>
+      <c r="O385" s="9">
+        <v>4</v>
+      </c>
+      <c r="P385" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q385" s="9">
+        <v>4</v>
+      </c>
+      <c r="R385" s="9">
+        <v>4</v>
+      </c>
+      <c r="S385" s="9">
+        <v>4</v>
+      </c>
+      <c r="T385" s="9">
+        <v>4</v>
+      </c>
+      <c r="U385" s="9">
+        <v>4</v>
+      </c>
+      <c r="V385" s="9">
+        <v>4</v>
+      </c>
+      <c r="W385" s="9">
+        <v>4</v>
+      </c>
+      <c r="X385" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y385" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI385" s="9">
+        <v>4</v>
+      </c>
+      <c r="AJ385" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="386" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A386" s="4">
+        <v>45594.881590474542</v>
+      </c>
+      <c r="B386" s="5" t="s">
+        <v>914</v>
+      </c>
+      <c r="C386" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="D386" s="5">
+        <v>20203213</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="F386" s="6">
+        <v>0.86805555555474712</v>
+      </c>
+      <c r="G386" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H386" s="5">
+        <v>2</v>
+      </c>
+      <c r="I386" s="5">
+        <v>2</v>
+      </c>
+      <c r="J386" s="5">
+        <v>5</v>
+      </c>
+      <c r="K386" s="5">
+        <v>3</v>
+      </c>
+      <c r="L386" s="5">
+        <v>4</v>
+      </c>
+      <c r="M386" s="5">
+        <v>4</v>
+      </c>
+      <c r="N386" s="5">
+        <v>3</v>
+      </c>
+      <c r="O386" s="5">
+        <v>2</v>
+      </c>
+      <c r="P386" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q386" s="5">
+        <v>4</v>
+      </c>
+      <c r="R386" s="5">
+        <v>2</v>
+      </c>
+      <c r="S386" s="5">
+        <v>3</v>
+      </c>
+      <c r="T386" s="5">
+        <v>2</v>
+      </c>
+      <c r="U386" s="5">
+        <v>5</v>
+      </c>
+      <c r="V386" s="5">
+        <v>5</v>
+      </c>
+      <c r="W386" s="5">
+        <v>6</v>
+      </c>
+      <c r="X386" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y386" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z386" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA386" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB386" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC386" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD386" s="5">
+        <v>5</v>
+      </c>
+      <c r="AE386" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF386" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG386" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH386" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI386" s="5">
+        <v>5</v>
+      </c>
+      <c r="AJ386" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A387" s="8">
+        <v>45594.891421400462</v>
+      </c>
+      <c r="B387" s="9" t="s">
+        <v>916</v>
+      </c>
+      <c r="C387" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D387" s="9">
+        <v>20244130</v>
+      </c>
+      <c r="E387" s="9" t="s">
+        <v>917</v>
+      </c>
+      <c r="F387" s="10">
+        <v>0.88541666666424135</v>
+      </c>
+      <c r="G387" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H387" s="9">
+        <v>1</v>
+      </c>
+      <c r="I387" s="9">
+        <v>5</v>
+      </c>
+      <c r="J387" s="9">
+        <v>5</v>
+      </c>
+      <c r="K387" s="9">
+        <v>4</v>
+      </c>
+      <c r="L387" s="9">
+        <v>2</v>
+      </c>
+      <c r="M387" s="9">
+        <v>3</v>
+      </c>
+      <c r="N387" s="9">
+        <v>5</v>
+      </c>
+      <c r="O387" s="9">
+        <v>5</v>
+      </c>
+      <c r="P387" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q387" s="9">
+        <v>2</v>
+      </c>
+      <c r="R387" s="9">
+        <v>6</v>
+      </c>
+      <c r="S387" s="9">
+        <v>5</v>
+      </c>
+      <c r="T387" s="9">
+        <v>2</v>
+      </c>
+      <c r="U387" s="9">
+        <v>3</v>
+      </c>
+      <c r="V387" s="9">
+        <v>4</v>
+      </c>
+      <c r="W387" s="9">
+        <v>4</v>
+      </c>
+      <c r="X387" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y387" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z387" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA387" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB387" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC387" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD387" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE387" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF387" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG387" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH387" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI387" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ387" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A388" s="15">
+        <v>45594.896274340281</v>
+      </c>
+      <c r="B388" s="16" t="s">
+        <v>918</v>
+      </c>
+      <c r="C388" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="D388" s="16">
+        <v>20203321</v>
+      </c>
+      <c r="E388" s="16" t="s">
+        <v>919</v>
+      </c>
+      <c r="F388" s="17">
+        <v>0.89305555555620231</v>
+      </c>
+      <c r="G388" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK388" s="16">
+        <v>3</v>
+      </c>
+      <c r="AL388" s="16">
+        <v>4</v>
+      </c>
+      <c r="AM388" s="16">
+        <v>4</v>
+      </c>
+      <c r="AN388" s="16">
+        <v>4</v>
+      </c>
+      <c r="AO388" s="16">
+        <v>2</v>
+      </c>
+      <c r="AP388" s="16">
+        <v>3</v>
+      </c>
+      <c r="AQ388" s="16">
+        <v>4</v>
+      </c>
+      <c r="AR388" s="16">
+        <v>4</v>
+      </c>
+      <c r="AS388" s="16">
+        <v>5</v>
+      </c>
+      <c r="AT388" s="16">
+        <v>2</v>
+      </c>
+      <c r="AU388" s="16">
+        <v>4</v>
+      </c>
+      <c r="AV388" s="16">
+        <v>2</v>
+      </c>
+      <c r="AW388" s="16">
+        <v>2</v>
+      </c>
+      <c r="AX388" s="16">
+        <v>2</v>
+      </c>
+      <c r="AY388" s="16">
+        <v>3</v>
+      </c>
+      <c r="AZ388" s="16">
+        <v>4</v>
+      </c>
+      <c r="BA388" s="16">
+        <v>3</v>
+      </c>
+      <c r="BB388" s="16">
+        <v>4</v>
+      </c>
+      <c r="BC388" s="16">
+        <v>3</v>
+      </c>
+      <c r="BD388" s="16">
+        <v>3</v>
+      </c>
+      <c r="BE388" s="16">
+        <v>3</v>
+      </c>
+      <c r="BF388" s="16">
+        <v>3</v>
+      </c>
+      <c r="BG388" s="16">
+        <v>3</v>
+      </c>
+      <c r="BH388" s="16">
+        <v>3</v>
+      </c>
+      <c r="BI388" s="16">
+        <v>3</v>
+      </c>
+      <c r="BJ388" s="16">
+        <v>3</v>
+      </c>
+      <c r="BK388" s="16">
+        <v>2</v>
+      </c>
+      <c r="BL388" s="16">
+        <v>2</v>
+      </c>
+      <c r="BM388" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="389" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A389" s="8">
+        <v>45594.927362662042</v>
+      </c>
+      <c r="B389" s="9" t="s">
+        <v>920</v>
+      </c>
+      <c r="C389" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="D389" s="9">
+        <v>20201007</v>
+      </c>
+      <c r="E389" s="9" t="s">
+        <v>921</v>
+      </c>
+      <c r="F389" s="10">
+        <v>0.93680555555329192</v>
+      </c>
+      <c r="G389" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AN389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AO389" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AQ389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AR389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AS389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AT389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AV389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AW389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX389" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY389" s="9">
+        <v>1</v>
+      </c>
+      <c r="AZ389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BA389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BB389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BC389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BE389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BF389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BG389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BH389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BJ389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BK389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL389" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM389" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="390" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A390" s="4">
+        <v>45594.947337650461</v>
+      </c>
+      <c r="B390" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="C390" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="D390" s="5">
+        <v>20205139</v>
+      </c>
+      <c r="E390" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="F390" s="6">
+        <v>0.94097222221898846</v>
+      </c>
+      <c r="G390" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK390" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL390" s="5">
+        <v>2</v>
+      </c>
+      <c r="AM390" s="5">
+        <v>6</v>
+      </c>
+      <c r="AN390" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO390" s="5">
+        <v>2</v>
+      </c>
+      <c r="AP390" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ390" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR390" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS390" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT390" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU390" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV390" s="5">
+        <v>6</v>
+      </c>
+      <c r="AW390" s="5">
+        <v>2</v>
+      </c>
+      <c r="AX390" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY390" s="5">
+        <v>6</v>
+      </c>
+      <c r="AZ390" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA390" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB390" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC390" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD390" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE390" s="5">
+        <v>1</v>
+      </c>
+      <c r="BF390" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG390" s="5">
+        <v>1</v>
+      </c>
+      <c r="BH390" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI390" s="5">
+        <v>6</v>
+      </c>
+      <c r="BJ390" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK390" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL390" s="5">
+        <v>1</v>
+      </c>
+      <c r="BM390" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A391" s="8">
+        <v>45594.951640150466</v>
+      </c>
+      <c r="B391" s="9" t="s">
+        <v>925</v>
+      </c>
+      <c r="C391" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D391" s="9">
+        <v>20246631</v>
+      </c>
+      <c r="E391" s="9" t="s">
+        <v>926</v>
+      </c>
+      <c r="F391" s="10">
+        <v>0.9493055555576575</v>
+      </c>
+      <c r="G391" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK391" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO391" s="9">
+        <v>2</v>
+      </c>
+      <c r="AP391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AQ391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AR391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AS391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT391" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW391" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX391" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY391" s="9">
+        <v>5</v>
+      </c>
+      <c r="AZ391" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA391" s="9">
+        <v>5</v>
+      </c>
+      <c r="BB391" s="9">
+        <v>5</v>
+      </c>
+      <c r="BC391" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD391" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE391" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF391" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG391" s="9">
+        <v>4</v>
+      </c>
+      <c r="BH391" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI391" s="9">
+        <v>5</v>
+      </c>
+      <c r="BJ391" s="9">
+        <v>5</v>
+      </c>
+      <c r="BK391" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL391" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM391" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="392" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A392" s="4">
+        <v>45595.074038275459</v>
+      </c>
+      <c r="B392" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="C392" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D392" s="5">
+        <v>20242702</v>
+      </c>
+      <c r="E392" s="5" t="s">
+        <v>928</v>
+      </c>
+      <c r="F392" s="6">
+        <v>7.2222222224809229E-2</v>
+      </c>
+      <c r="G392" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AL392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AP392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AQ392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AU392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AV392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY392" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BA392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BC392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BE392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BG392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BH392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BI392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BJ392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BL392" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM392" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="393" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A393" s="18">
+        <v>45595.142103645834</v>
+      </c>
+      <c r="B393" s="19" t="s">
+        <v>929</v>
+      </c>
+      <c r="C393" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="D393" s="19">
+        <v>20241519</v>
+      </c>
+      <c r="E393" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="F393" s="20">
+        <v>0.14027777777664596</v>
+      </c>
+      <c r="G393" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H393" s="19">
+        <v>1</v>
+      </c>
+      <c r="I393" s="19">
+        <v>3</v>
+      </c>
+      <c r="J393" s="19">
+        <v>4</v>
+      </c>
+      <c r="K393" s="19">
+        <v>3</v>
+      </c>
+      <c r="L393" s="19">
+        <v>1</v>
+      </c>
+      <c r="M393" s="19">
+        <v>1</v>
+      </c>
+      <c r="N393" s="19">
+        <v>3</v>
+      </c>
+      <c r="O393" s="19">
+        <v>3</v>
+      </c>
+      <c r="P393" s="19">
+        <v>3</v>
+      </c>
+      <c r="Q393" s="19">
+        <v>1</v>
+      </c>
+      <c r="R393" s="19">
+        <v>3</v>
+      </c>
+      <c r="S393" s="19">
+        <v>3</v>
+      </c>
+      <c r="T393" s="19">
+        <v>1</v>
+      </c>
+      <c r="U393" s="19">
+        <v>1</v>
+      </c>
+      <c r="V393" s="19">
+        <v>4</v>
+      </c>
+      <c r="W393" s="19">
+        <v>3</v>
+      </c>
+      <c r="X393" s="19">
+        <v>3</v>
+      </c>
+      <c r="Y393" s="19">
+        <v>3</v>
+      </c>
+      <c r="Z393" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA393" s="19">
+        <v>3</v>
+      </c>
+      <c r="AB393" s="19">
+        <v>3</v>
+      </c>
+      <c r="AC393" s="19">
+        <v>3</v>
+      </c>
+      <c r="AD393" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE393" s="19">
+        <v>1</v>
+      </c>
+      <c r="AF393" s="19">
+        <v>3</v>
+      </c>
+      <c r="AG393" s="19">
+        <v>3</v>
+      </c>
+      <c r="AH393" s="19">
+        <v>1</v>
+      </c>
+      <c r="AI393" s="19">
+        <v>1</v>
+      </c>
+      <c r="AJ393" s="19">
+        <v>1</v>
+      </c>
+      <c r="AK393" s="25"/>
+      <c r="AL393" s="25"/>
+      <c r="AM393" s="25"/>
+      <c r="AN393" s="25"/>
+      <c r="AO393" s="25"/>
+      <c r="AP393" s="25"/>
+      <c r="AQ393" s="25"/>
+      <c r="AR393" s="25"/>
+      <c r="AS393" s="25"/>
+      <c r="AT393" s="25"/>
+      <c r="AU393" s="25"/>
+      <c r="AV393" s="25"/>
+      <c r="AW393" s="25"/>
+      <c r="AX393" s="25"/>
+      <c r="AY393" s="25"/>
+      <c r="AZ393" s="25"/>
+      <c r="BA393" s="25"/>
+      <c r="BB393" s="25"/>
+      <c r="BC393" s="25"/>
+      <c r="BD393" s="25"/>
+      <c r="BE393" s="25"/>
+      <c r="BF393" s="25"/>
+      <c r="BG393" s="25"/>
+      <c r="BH393" s="25"/>
+      <c r="BI393" s="25"/>
+      <c r="BJ393" s="25"/>
+      <c r="BK393" s="25"/>
+      <c r="BL393" s="25"/>
+      <c r="BM393" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
241021, oxford modified sunday 06:52
</commit_message>
<xml_diff>
--- a/R/data/oxford_241021.xlsx
+++ b/R/data/oxford_241021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Dropbox/내 Mac (Kee-Won의 MacBook Air)/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED54FB9-F5F9-324F-9BC3-EB3100ACBE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE13CE3-4635-D248-AC34-8C75DE17F879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48000" yWindow="1360" windowWidth="37080" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42920" yWindow="1360" windowWidth="37080" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설문지 응답 시트1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="1164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="1195">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -3515,6 +3515,99 @@
   </si>
   <si>
     <t>유지원</t>
+  </si>
+  <si>
+    <t>jytoto33@naver.com</t>
+  </si>
+  <si>
+    <t>김지윤</t>
+  </si>
+  <si>
+    <t>benjamin27@naver.com</t>
+  </si>
+  <si>
+    <t>최재혁</t>
+  </si>
+  <si>
+    <t>hsjenny99@gmail.com</t>
+  </si>
+  <si>
+    <t>전소현</t>
+  </si>
+  <si>
+    <t>hanseoyun392@gmail.com</t>
+  </si>
+  <si>
+    <t>한서윤</t>
+  </si>
+  <si>
+    <t>a35142191@gmail.com</t>
+  </si>
+  <si>
+    <t>이윤재</t>
+  </si>
+  <si>
+    <t>vldzmgha0609@naver.com</t>
+  </si>
+  <si>
+    <t>김지수</t>
+  </si>
+  <si>
+    <t>moon050123@naver.com</t>
+  </si>
+  <si>
+    <t>문서원</t>
+  </si>
+  <si>
+    <t>ehdus1113kim@naver.com</t>
+  </si>
+  <si>
+    <t>김도연</t>
+  </si>
+  <si>
+    <t>kya01095509223@gmail.com</t>
+  </si>
+  <si>
+    <t>간호</t>
+  </si>
+  <si>
+    <t>김윤아</t>
+  </si>
+  <si>
+    <t>hyeonyonga@naver.com</t>
+  </si>
+  <si>
+    <t>안현용</t>
+  </si>
+  <si>
+    <t>krcar1002@gmail.com</t>
+  </si>
+  <si>
+    <t>김재호</t>
+  </si>
+  <si>
+    <t>jud050207@gmail.com</t>
+  </si>
+  <si>
+    <t>정의돈</t>
+  </si>
+  <si>
+    <t>jyj111212@naver.com</t>
+  </si>
+  <si>
+    <t>장예지</t>
+  </si>
+  <si>
+    <t>dmsdn6462@naver.com</t>
+  </si>
+  <si>
+    <t>김은우</t>
+  </si>
+  <si>
+    <t>gee30901@naver.com</t>
+  </si>
+  <si>
+    <t>박예원</t>
   </si>
 </sst>
 </file>
@@ -3561,7 +3654,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -3812,6 +3905,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3890,7 +3998,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -3940,7 +4050,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM508">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM523">
   <tableColumns count="65">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -4213,11 +4323,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM508"/>
+  <dimension ref="A1:BM523"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A470" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E518" sqref="E518"/>
+      <pane ySplit="1" topLeftCell="A497" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C528" sqref="C528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -61088,35 +61198,1656 @@
       <c r="AJ508" s="16">
         <v>2</v>
       </c>
-      <c r="AK508" s="25"/>
-      <c r="AL508" s="25"/>
-      <c r="AM508" s="25"/>
-      <c r="AN508" s="25"/>
-      <c r="AO508" s="25"/>
-      <c r="AP508" s="25"/>
-      <c r="AQ508" s="25"/>
-      <c r="AR508" s="25"/>
-      <c r="AS508" s="25"/>
-      <c r="AT508" s="25"/>
-      <c r="AU508" s="25"/>
-      <c r="AV508" s="25"/>
-      <c r="AW508" s="25"/>
-      <c r="AX508" s="25"/>
-      <c r="AY508" s="25"/>
-      <c r="AZ508" s="25"/>
-      <c r="BA508" s="25"/>
-      <c r="BB508" s="25"/>
-      <c r="BC508" s="25"/>
-      <c r="BD508" s="25"/>
-      <c r="BE508" s="25"/>
-      <c r="BF508" s="25"/>
-      <c r="BG508" s="25"/>
-      <c r="BH508" s="25"/>
-      <c r="BI508" s="25"/>
-      <c r="BJ508" s="25"/>
-      <c r="BK508" s="25"/>
-      <c r="BL508" s="25"/>
-      <c r="BM508" s="25"/>
+    </row>
+    <row r="509" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A509" s="8">
+        <v>45599.018801435188</v>
+      </c>
+      <c r="B509" s="9" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C509" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D509" s="9">
+        <v>20246238</v>
+      </c>
+      <c r="E509" s="9" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F509" s="10">
+        <v>1.5277777776645962E-2</v>
+      </c>
+      <c r="G509" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK509" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL509" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM509" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN509" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO509" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP509" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ509" s="9">
+        <v>4</v>
+      </c>
+      <c r="AR509" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS509" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT509" s="9">
+        <v>5</v>
+      </c>
+      <c r="AU509" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV509" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW509" s="9">
+        <v>1</v>
+      </c>
+      <c r="AX509" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY509" s="9">
+        <v>5</v>
+      </c>
+      <c r="AZ509" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA509" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB509" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC509" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD509" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE509" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF509" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG509" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH509" s="9">
+        <v>5</v>
+      </c>
+      <c r="BI509" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ509" s="9">
+        <v>5</v>
+      </c>
+      <c r="BK509" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL509" s="9">
+        <v>4</v>
+      </c>
+      <c r="BM509" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="510" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A510" s="4">
+        <v>45599.029538298608</v>
+      </c>
+      <c r="B510" s="5" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C510" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D510" s="5">
+        <v>20243912</v>
+      </c>
+      <c r="E510" s="5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="F510" s="6">
+        <v>2.5000000001455192E-2</v>
+      </c>
+      <c r="G510" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H510" s="5">
+        <v>5</v>
+      </c>
+      <c r="I510" s="5">
+        <v>3</v>
+      </c>
+      <c r="J510" s="5">
+        <v>2</v>
+      </c>
+      <c r="K510" s="5">
+        <v>3</v>
+      </c>
+      <c r="L510" s="5">
+        <v>4</v>
+      </c>
+      <c r="M510" s="5">
+        <v>5</v>
+      </c>
+      <c r="N510" s="5">
+        <v>4</v>
+      </c>
+      <c r="O510" s="5">
+        <v>2</v>
+      </c>
+      <c r="P510" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q510" s="5">
+        <v>5</v>
+      </c>
+      <c r="R510" s="5">
+        <v>3</v>
+      </c>
+      <c r="S510" s="5">
+        <v>2</v>
+      </c>
+      <c r="T510" s="5">
+        <v>2</v>
+      </c>
+      <c r="U510" s="5">
+        <v>6</v>
+      </c>
+      <c r="V510" s="5">
+        <v>3</v>
+      </c>
+      <c r="W510" s="5">
+        <v>5</v>
+      </c>
+      <c r="X510" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y510" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z510" s="5">
+        <v>6</v>
+      </c>
+      <c r="AA510" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB510" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC510" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD510" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE510" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF510" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG510" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH510" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI510" s="5">
+        <v>5</v>
+      </c>
+      <c r="AJ510" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="511" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A511" s="8">
+        <v>45599.044823217591</v>
+      </c>
+      <c r="B511" s="9" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C511" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D511" s="9">
+        <v>20212583</v>
+      </c>
+      <c r="E511" s="9" t="s">
+        <v>1167</v>
+      </c>
+      <c r="F511" s="10">
+        <v>4.0277777778101154E-2</v>
+      </c>
+      <c r="G511" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H511" s="9">
+        <v>3</v>
+      </c>
+      <c r="I511" s="9">
+        <v>2</v>
+      </c>
+      <c r="J511" s="9">
+        <v>2</v>
+      </c>
+      <c r="K511" s="9">
+        <v>2</v>
+      </c>
+      <c r="L511" s="9">
+        <v>4</v>
+      </c>
+      <c r="M511" s="9">
+        <v>5</v>
+      </c>
+      <c r="N511" s="9">
+        <v>4</v>
+      </c>
+      <c r="O511" s="9">
+        <v>3</v>
+      </c>
+      <c r="P511" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q511" s="9">
+        <v>5</v>
+      </c>
+      <c r="R511" s="9">
+        <v>5</v>
+      </c>
+      <c r="S511" s="9">
+        <v>4</v>
+      </c>
+      <c r="T511" s="9">
+        <v>3</v>
+      </c>
+      <c r="U511" s="9">
+        <v>4</v>
+      </c>
+      <c r="V511" s="9">
+        <v>3</v>
+      </c>
+      <c r="W511" s="9">
+        <v>6</v>
+      </c>
+      <c r="X511" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y511" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z511" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA511" s="9">
+        <v>2</v>
+      </c>
+      <c r="AB511" s="9">
+        <v>2</v>
+      </c>
+      <c r="AC511" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD511" s="9">
+        <v>6</v>
+      </c>
+      <c r="AE511" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF511" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG511" s="9">
+        <v>2</v>
+      </c>
+      <c r="AH511" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI511" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ511" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="512" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A512" s="4">
+        <v>45599.048208171298</v>
+      </c>
+      <c r="B512" s="5" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C512" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D512" s="5">
+        <v>20245246</v>
+      </c>
+      <c r="E512" s="5" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F512" s="6">
+        <v>4.4444444443797693E-2</v>
+      </c>
+      <c r="G512" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H512" s="5">
+        <v>2</v>
+      </c>
+      <c r="I512" s="5">
+        <v>5</v>
+      </c>
+      <c r="J512" s="5">
+        <v>5</v>
+      </c>
+      <c r="K512" s="5">
+        <v>5</v>
+      </c>
+      <c r="L512" s="5">
+        <v>2</v>
+      </c>
+      <c r="M512" s="5">
+        <v>5</v>
+      </c>
+      <c r="N512" s="5">
+        <v>5</v>
+      </c>
+      <c r="O512" s="5">
+        <v>5</v>
+      </c>
+      <c r="P512" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q512" s="5">
+        <v>1</v>
+      </c>
+      <c r="R512" s="5">
+        <v>6</v>
+      </c>
+      <c r="S512" s="5">
+        <v>5</v>
+      </c>
+      <c r="T512" s="5">
+        <v>2</v>
+      </c>
+      <c r="U512" s="5">
+        <v>4</v>
+      </c>
+      <c r="V512" s="5">
+        <v>6</v>
+      </c>
+      <c r="W512" s="5">
+        <v>5</v>
+      </c>
+      <c r="X512" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y512" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z512" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA512" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB512" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC512" s="5">
+        <v>6</v>
+      </c>
+      <c r="AD512" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE512" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF512" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG512" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH512" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI512" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ512" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A513" s="8">
+        <v>45599.056800231483</v>
+      </c>
+      <c r="B513" s="9" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C513" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D513" s="9">
+        <v>20243964</v>
+      </c>
+      <c r="E513" s="9" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F513" s="10">
+        <v>5.2777777775190771E-2</v>
+      </c>
+      <c r="G513" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL513" s="9">
+        <v>4</v>
+      </c>
+      <c r="AM513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO513" s="9">
+        <v>1</v>
+      </c>
+      <c r="AP513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU513" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW513" s="9">
+        <v>4</v>
+      </c>
+      <c r="AX513" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY513" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ513" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA513" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB513" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC513" s="9">
+        <v>4</v>
+      </c>
+      <c r="BD513" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE513" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF513" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG513" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH513" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI513" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ513" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK513" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL513" s="9">
+        <v>5</v>
+      </c>
+      <c r="BM513" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="514" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A514" s="4">
+        <v>45599.070521342597</v>
+      </c>
+      <c r="B514" s="5" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C514" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D514" s="5">
+        <v>20243241</v>
+      </c>
+      <c r="E514" s="5" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F514" s="6">
+        <v>7.0138888884685002E-2</v>
+      </c>
+      <c r="G514" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK514" s="5">
+        <v>5</v>
+      </c>
+      <c r="AL514" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM514" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN514" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO514" s="5">
+        <v>1</v>
+      </c>
+      <c r="AP514" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ514" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR514" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS514" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT514" s="5">
+        <v>3</v>
+      </c>
+      <c r="AU514" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV514" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW514" s="5">
+        <v>4</v>
+      </c>
+      <c r="AX514" s="5">
+        <v>1</v>
+      </c>
+      <c r="AY514" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ514" s="5">
+        <v>2</v>
+      </c>
+      <c r="BA514" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB514" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC514" s="5">
+        <v>5</v>
+      </c>
+      <c r="BD514" s="5">
+        <v>2</v>
+      </c>
+      <c r="BE514" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF514" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG514" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH514" s="5">
+        <v>3</v>
+      </c>
+      <c r="BI514" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ514" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK514" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL514" s="5">
+        <v>1</v>
+      </c>
+      <c r="BM514" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A515" s="8">
+        <v>45599.089457685186</v>
+      </c>
+      <c r="B515" s="9" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C515" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D515" s="9">
+        <v>20227039</v>
+      </c>
+      <c r="E515" s="9" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F515" s="10">
+        <v>8.6111111115314998E-2</v>
+      </c>
+      <c r="G515" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK515" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL515" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM515" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN515" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO515" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP515" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ515" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR515" s="9">
+        <v>5</v>
+      </c>
+      <c r="AS515" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT515" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU515" s="9">
+        <v>2</v>
+      </c>
+      <c r="AV515" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW515" s="9">
+        <v>4</v>
+      </c>
+      <c r="AX515" s="9">
+        <v>5</v>
+      </c>
+      <c r="AY515" s="9">
+        <v>2</v>
+      </c>
+      <c r="AZ515" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA515" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB515" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC515" s="9">
+        <v>5</v>
+      </c>
+      <c r="BD515" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE515" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF515" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG515" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH515" s="9">
+        <v>5</v>
+      </c>
+      <c r="BI515" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ515" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK515" s="9">
+        <v>4</v>
+      </c>
+      <c r="BL515" s="9">
+        <v>5</v>
+      </c>
+      <c r="BM515" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="516" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A516" s="4">
+        <v>45599.089483645832</v>
+      </c>
+      <c r="B516" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C516" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D516" s="5">
+        <v>20241518</v>
+      </c>
+      <c r="E516" s="5" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F516" s="6">
+        <v>8.819444444088731E-2</v>
+      </c>
+      <c r="G516" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H516" s="5">
+        <v>3</v>
+      </c>
+      <c r="I516" s="5">
+        <v>2</v>
+      </c>
+      <c r="J516" s="5">
+        <v>2</v>
+      </c>
+      <c r="K516" s="5">
+        <v>2</v>
+      </c>
+      <c r="L516" s="5">
+        <v>3</v>
+      </c>
+      <c r="M516" s="5">
+        <v>3</v>
+      </c>
+      <c r="N516" s="5">
+        <v>2</v>
+      </c>
+      <c r="O516" s="5">
+        <v>2</v>
+      </c>
+      <c r="P516" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q516" s="5">
+        <v>3</v>
+      </c>
+      <c r="R516" s="5">
+        <v>2</v>
+      </c>
+      <c r="S516" s="5">
+        <v>2</v>
+      </c>
+      <c r="T516" s="5">
+        <v>2</v>
+      </c>
+      <c r="U516" s="5">
+        <v>3</v>
+      </c>
+      <c r="V516" s="5">
+        <v>2</v>
+      </c>
+      <c r="W516" s="5">
+        <v>3</v>
+      </c>
+      <c r="X516" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y516" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z516" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA516" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB516" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC516" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD516" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE516" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF516" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG516" s="5">
+        <v>2</v>
+      </c>
+      <c r="AH516" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI516" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ516" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="517" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A517" s="8">
+        <v>45599.093982326391</v>
+      </c>
+      <c r="B517" s="9" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C517" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D517" s="9">
+        <v>20232705</v>
+      </c>
+      <c r="E517" s="9" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F517" s="10">
+        <v>9.1666666667151731E-2</v>
+      </c>
+      <c r="G517" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H517" s="9">
+        <v>3</v>
+      </c>
+      <c r="I517" s="9">
+        <v>3</v>
+      </c>
+      <c r="J517" s="9">
+        <v>2</v>
+      </c>
+      <c r="K517" s="9">
+        <v>5</v>
+      </c>
+      <c r="L517" s="9">
+        <v>2</v>
+      </c>
+      <c r="M517" s="9">
+        <v>5</v>
+      </c>
+      <c r="N517" s="9">
+        <v>2</v>
+      </c>
+      <c r="O517" s="9">
+        <v>2</v>
+      </c>
+      <c r="P517" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q517" s="9">
+        <v>4</v>
+      </c>
+      <c r="R517" s="9">
+        <v>2</v>
+      </c>
+      <c r="S517" s="9">
+        <v>4</v>
+      </c>
+      <c r="T517" s="9">
+        <v>4</v>
+      </c>
+      <c r="U517" s="9">
+        <v>4</v>
+      </c>
+      <c r="V517" s="9">
+        <v>3</v>
+      </c>
+      <c r="W517" s="9">
+        <v>3</v>
+      </c>
+      <c r="X517" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y517" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z517" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA517" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB517" s="9">
+        <v>2</v>
+      </c>
+      <c r="AC517" s="9">
+        <v>2</v>
+      </c>
+      <c r="AD517" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE517" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF517" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG517" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH517" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI517" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ517" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="518" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A518" s="4">
+        <v>45599.144704606486</v>
+      </c>
+      <c r="B518" s="5" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C518" s="5" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D518" s="5">
+        <v>20246224</v>
+      </c>
+      <c r="E518" s="5" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F518" s="6">
+        <v>0.13749999999708962</v>
+      </c>
+      <c r="G518" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK518" s="5">
+        <v>3</v>
+      </c>
+      <c r="AL518" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM518" s="5">
+        <v>2</v>
+      </c>
+      <c r="AN518" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO518" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP518" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ518" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR518" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS518" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT518" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU518" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV518" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW518" s="5">
+        <v>2</v>
+      </c>
+      <c r="AX518" s="5">
+        <v>5</v>
+      </c>
+      <c r="AY518" s="5">
+        <v>4</v>
+      </c>
+      <c r="AZ518" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA518" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB518" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC518" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD518" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE518" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF518" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG518" s="5">
+        <v>3</v>
+      </c>
+      <c r="BH518" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI518" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ518" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK518" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL518" s="5">
+        <v>4</v>
+      </c>
+      <c r="BM518" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="519" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A519" s="8">
+        <v>45599.145419907407</v>
+      </c>
+      <c r="B519" s="9" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C519" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D519" s="9">
+        <v>20243415</v>
+      </c>
+      <c r="E519" s="9" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F519" s="10">
+        <v>0.14097222222335404</v>
+      </c>
+      <c r="G519" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H519" s="9">
+        <v>2</v>
+      </c>
+      <c r="I519" s="9">
+        <v>5</v>
+      </c>
+      <c r="J519" s="9">
+        <v>4</v>
+      </c>
+      <c r="K519" s="9">
+        <v>4</v>
+      </c>
+      <c r="L519" s="9">
+        <v>5</v>
+      </c>
+      <c r="M519" s="9">
+        <v>5</v>
+      </c>
+      <c r="N519" s="9">
+        <v>3</v>
+      </c>
+      <c r="O519" s="9">
+        <v>5</v>
+      </c>
+      <c r="P519" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q519" s="9">
+        <v>2</v>
+      </c>
+      <c r="R519" s="9">
+        <v>3</v>
+      </c>
+      <c r="S519" s="9">
+        <v>4</v>
+      </c>
+      <c r="T519" s="9">
+        <v>4</v>
+      </c>
+      <c r="U519" s="9">
+        <v>3</v>
+      </c>
+      <c r="V519" s="9">
+        <v>4</v>
+      </c>
+      <c r="W519" s="9">
+        <v>2</v>
+      </c>
+      <c r="X519" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y519" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z519" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA519" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB519" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC519" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD519" s="9">
+        <v>5</v>
+      </c>
+      <c r="AE519" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF519" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG519" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH519" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI519" s="9">
+        <v>4</v>
+      </c>
+      <c r="AJ519" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="520" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A520" s="4">
+        <v>45599.172017465273</v>
+      </c>
+      <c r="B520" s="5" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C520" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D520" s="5">
+        <v>20242109</v>
+      </c>
+      <c r="E520" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F520" s="6">
+        <v>0.13541666666424135</v>
+      </c>
+      <c r="G520" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK520" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL520" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM520" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN520" s="5">
+        <v>2</v>
+      </c>
+      <c r="AO520" s="5">
+        <v>3</v>
+      </c>
+      <c r="AP520" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ520" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR520" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS520" s="5">
+        <v>4</v>
+      </c>
+      <c r="AT520" s="5">
+        <v>3</v>
+      </c>
+      <c r="AU520" s="5">
+        <v>4</v>
+      </c>
+      <c r="AV520" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW520" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX520" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY520" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ520" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA520" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB520" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC520" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD520" s="5">
+        <v>2</v>
+      </c>
+      <c r="BE520" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF520" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG520" s="5">
+        <v>6</v>
+      </c>
+      <c r="BH520" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI520" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ520" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK520" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL520" s="5">
+        <v>2</v>
+      </c>
+      <c r="BM520" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="521" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A521" s="8">
+        <v>45599.218465578699</v>
+      </c>
+      <c r="B521" s="9" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C521" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D521" s="9">
+        <v>20245252</v>
+      </c>
+      <c r="E521" s="9" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F521" s="10">
+        <v>0.21458333333430346</v>
+      </c>
+      <c r="G521" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H521" s="9">
+        <v>1</v>
+      </c>
+      <c r="I521" s="9">
+        <v>4</v>
+      </c>
+      <c r="J521" s="9">
+        <v>5</v>
+      </c>
+      <c r="K521" s="9">
+        <v>4</v>
+      </c>
+      <c r="L521" s="9">
+        <v>2</v>
+      </c>
+      <c r="M521" s="9">
+        <v>2</v>
+      </c>
+      <c r="N521" s="9">
+        <v>4</v>
+      </c>
+      <c r="O521" s="9">
+        <v>5</v>
+      </c>
+      <c r="P521" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q521" s="9">
+        <v>3</v>
+      </c>
+      <c r="R521" s="9">
+        <v>4</v>
+      </c>
+      <c r="S521" s="9">
+        <v>4</v>
+      </c>
+      <c r="T521" s="9">
+        <v>2</v>
+      </c>
+      <c r="U521" s="9">
+        <v>2</v>
+      </c>
+      <c r="V521" s="9">
+        <v>5</v>
+      </c>
+      <c r="W521" s="9">
+        <v>2</v>
+      </c>
+      <c r="X521" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y521" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z521" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA521" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB521" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC521" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD521" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE521" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF521" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG521" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH521" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI521" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ521" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="522" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A522" s="4">
+        <v>45599.226147372683</v>
+      </c>
+      <c r="B522" s="5" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C522" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D522" s="5">
+        <v>20241083</v>
+      </c>
+      <c r="E522" s="5" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F522" s="6">
+        <v>0.22499999999854481</v>
+      </c>
+      <c r="G522" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK522" s="5">
+        <v>5</v>
+      </c>
+      <c r="AL522" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM522" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN522" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO522" s="5">
+        <v>6</v>
+      </c>
+      <c r="AP522" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ522" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR522" s="5">
+        <v>6</v>
+      </c>
+      <c r="AS522" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT522" s="5">
+        <v>5</v>
+      </c>
+      <c r="AU522" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV522" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW522" s="5">
+        <v>6</v>
+      </c>
+      <c r="AX522" s="5">
+        <v>6</v>
+      </c>
+      <c r="AY522" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ522" s="5">
+        <v>6</v>
+      </c>
+      <c r="BA522" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB522" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC522" s="5">
+        <v>5</v>
+      </c>
+      <c r="BD522" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE522" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF522" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG522" s="5">
+        <v>3</v>
+      </c>
+      <c r="BH522" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI522" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ522" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK522" s="5">
+        <v>6</v>
+      </c>
+      <c r="BL522" s="5">
+        <v>5</v>
+      </c>
+      <c r="BM522" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="523" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A523" s="12">
+        <v>45599.236574050927</v>
+      </c>
+      <c r="B523" s="13" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C523" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D523" s="13">
+        <v>20202106</v>
+      </c>
+      <c r="E523" s="13" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F523" s="14">
+        <v>0.23541666666278616</v>
+      </c>
+      <c r="G523" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AL523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AM523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AN523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AO523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AP523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AQ523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AR523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AS523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AT523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AU523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AV523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AW523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AX523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AY523" s="13">
+        <v>5</v>
+      </c>
+      <c r="AZ523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BA523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BB523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BC523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BD523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BE523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BF523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BG523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BH523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BI523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BJ523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BK523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BL523" s="13">
+        <v>5</v>
+      </c>
+      <c r="BM523" s="25">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
241021, oxford modified sunday 10:52
</commit_message>
<xml_diff>
--- a/R/data/oxford_241021.xlsx
+++ b/R/data/oxford_241021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Dropbox/내 Mac (Kee-Won의 MacBook Air)/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE13CE3-4635-D248-AC34-8C75DE17F879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F8AFE5-C063-9640-84C0-29094A8AAE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42920" yWindow="1360" windowWidth="37080" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42920" yWindow="1420" windowWidth="37080" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설문지 응답 시트1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="1195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="1233">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -3608,6 +3608,120 @@
   </si>
   <si>
     <t>박예원</t>
+  </si>
+  <si>
+    <t>hlu20242513@gmail.com</t>
+  </si>
+  <si>
+    <t>김예준</t>
+  </si>
+  <si>
+    <t>yeon4262@naver.com</t>
+  </si>
+  <si>
+    <t>신수연</t>
+  </si>
+  <si>
+    <t>cbh3trust4@naver.com</t>
+  </si>
+  <si>
+    <t>조정현</t>
+  </si>
+  <si>
+    <t>hyerujys2005@naver.com</t>
+  </si>
+  <si>
+    <t>정윤수</t>
+  </si>
+  <si>
+    <t>sdw20050421@gmail.com</t>
+  </si>
+  <si>
+    <t>송도원</t>
+  </si>
+  <si>
+    <t>sjhaa303028@naver.com</t>
+  </si>
+  <si>
+    <t>신중현</t>
+  </si>
+  <si>
+    <t>ian5791@naver.com</t>
+  </si>
+  <si>
+    <t>박수현</t>
+  </si>
+  <si>
+    <t>ac3512@naver.com</t>
+  </si>
+  <si>
+    <t>융합신소재공학</t>
+  </si>
+  <si>
+    <t>김태근</t>
+  </si>
+  <si>
+    <t>dldpwls5245@naver.com</t>
+  </si>
+  <si>
+    <t>이예진</t>
+  </si>
+  <si>
+    <t>rhkddyd234@naver.com</t>
+  </si>
+  <si>
+    <t>이광용</t>
+  </si>
+  <si>
+    <t>rudongdong0302@naver.com</t>
+  </si>
+  <si>
+    <t>이정효</t>
+  </si>
+  <si>
+    <t>jeongminyoung@naver.com</t>
+  </si>
+  <si>
+    <t>정민영</t>
+  </si>
+  <si>
+    <t>jhkm7400@gmail.com</t>
+  </si>
+  <si>
+    <t>김유건</t>
+  </si>
+  <si>
+    <t>a22234781@gmail.com</t>
+  </si>
+  <si>
+    <t>hg2635394@gmail.com</t>
+  </si>
+  <si>
+    <t>철학과</t>
+  </si>
+  <si>
+    <t>김현준</t>
+  </si>
+  <si>
+    <t>sihyune1104@gmail.com</t>
+  </si>
+  <si>
+    <t>안시현</t>
+  </si>
+  <si>
+    <t>jyoon2233@naver.com</t>
+  </si>
+  <si>
+    <t>신정윤</t>
+  </si>
+  <si>
+    <t>choyunjae2153@gmail.com</t>
+  </si>
+  <si>
+    <t>AI의료융합학과</t>
+  </si>
+  <si>
+    <t>조윤재</t>
   </si>
 </sst>
 </file>
@@ -3924,7 +4038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4001,6 +4115,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -4050,7 +4165,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM523">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM541">
   <tableColumns count="65">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -4323,11 +4438,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM523"/>
+  <dimension ref="A1:BM541"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A497" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C528" sqref="C528"/>
+      <selection pane="bottomLeft" activeCell="D544" sqref="D544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -62849,6 +62964,2015 @@
         <v>5</v>
       </c>
     </row>
+    <row r="524" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A524" s="4">
+        <v>45599.281842916665</v>
+      </c>
+      <c r="B524" s="5" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C524" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D524" s="5">
+        <v>20242513</v>
+      </c>
+      <c r="E524" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F524" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="G524" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H524" s="5">
+        <v>4</v>
+      </c>
+      <c r="I524" s="5">
+        <v>5</v>
+      </c>
+      <c r="J524" s="5">
+        <v>5</v>
+      </c>
+      <c r="K524" s="5">
+        <v>4</v>
+      </c>
+      <c r="L524" s="5">
+        <v>4</v>
+      </c>
+      <c r="M524" s="5">
+        <v>3</v>
+      </c>
+      <c r="N524" s="5">
+        <v>3</v>
+      </c>
+      <c r="O524" s="5">
+        <v>4</v>
+      </c>
+      <c r="P524" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q524" s="5">
+        <v>3</v>
+      </c>
+      <c r="R524" s="5">
+        <v>4</v>
+      </c>
+      <c r="S524" s="5">
+        <v>3</v>
+      </c>
+      <c r="T524" s="5">
+        <v>4</v>
+      </c>
+      <c r="U524" s="5">
+        <v>5</v>
+      </c>
+      <c r="V524" s="5">
+        <v>3</v>
+      </c>
+      <c r="W524" s="5">
+        <v>4</v>
+      </c>
+      <c r="X524" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y524" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z524" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA524" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB524" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC524" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD524" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE524" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF524" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG524" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH524" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI524" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ524" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="525" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A525" s="8">
+        <v>45599.283132812503</v>
+      </c>
+      <c r="B525" s="9" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C525" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D525" s="9">
+        <v>20223325</v>
+      </c>
+      <c r="E525" s="9" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F525" s="10">
+        <v>0.27291666666860692</v>
+      </c>
+      <c r="G525" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK525" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL525" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM525" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN525" s="9">
+        <v>2</v>
+      </c>
+      <c r="AO525" s="9">
+        <v>1</v>
+      </c>
+      <c r="AP525" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ525" s="9">
+        <v>2</v>
+      </c>
+      <c r="AR525" s="9">
+        <v>2</v>
+      </c>
+      <c r="AS525" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT525" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU525" s="9">
+        <v>6</v>
+      </c>
+      <c r="AV525" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW525" s="9">
+        <v>1</v>
+      </c>
+      <c r="AX525" s="9">
+        <v>4</v>
+      </c>
+      <c r="AY525" s="9">
+        <v>5</v>
+      </c>
+      <c r="AZ525" s="9">
+        <v>6</v>
+      </c>
+      <c r="BA525" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB525" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC525" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD525" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE525" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF525" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG525" s="9">
+        <v>4</v>
+      </c>
+      <c r="BH525" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI525" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ525" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK525" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL525" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM525" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="526" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A526" s="4">
+        <v>45599.288081805556</v>
+      </c>
+      <c r="B526" s="5" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C526" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D526" s="5">
+        <v>20242749</v>
+      </c>
+      <c r="E526" s="5" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F526" s="6">
+        <v>0.28402777777955635</v>
+      </c>
+      <c r="G526" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK526" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL526" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM526" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN526" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO526" s="5">
+        <v>6</v>
+      </c>
+      <c r="AP526" s="5">
+        <v>3</v>
+      </c>
+      <c r="AQ526" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR526" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS526" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT526" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU526" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV526" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW526" s="5">
+        <v>2</v>
+      </c>
+      <c r="AX526" s="5">
+        <v>5</v>
+      </c>
+      <c r="AY526" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ526" s="5">
+        <v>3</v>
+      </c>
+      <c r="BA526" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB526" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC526" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD526" s="5">
+        <v>2</v>
+      </c>
+      <c r="BE526" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF526" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG526" s="5">
+        <v>5</v>
+      </c>
+      <c r="BH526" s="5">
+        <v>3</v>
+      </c>
+      <c r="BI526" s="5">
+        <v>2</v>
+      </c>
+      <c r="BJ526" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK526" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL526" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM526" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="527" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A527" s="8">
+        <v>45599.29531710648</v>
+      </c>
+      <c r="B527" s="9" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C527" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D527" s="9">
+        <v>20242575</v>
+      </c>
+      <c r="E527" s="9" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F527" s="10">
+        <v>0.29166666666424135</v>
+      </c>
+      <c r="G527" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H527" s="9">
+        <v>2</v>
+      </c>
+      <c r="I527" s="9">
+        <v>5</v>
+      </c>
+      <c r="J527" s="9">
+        <v>5</v>
+      </c>
+      <c r="K527" s="9">
+        <v>4</v>
+      </c>
+      <c r="L527" s="9">
+        <v>2</v>
+      </c>
+      <c r="M527" s="9">
+        <v>3</v>
+      </c>
+      <c r="N527" s="9">
+        <v>4</v>
+      </c>
+      <c r="O527" s="9">
+        <v>4</v>
+      </c>
+      <c r="P527" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q527" s="9">
+        <v>1</v>
+      </c>
+      <c r="R527" s="9">
+        <v>5</v>
+      </c>
+      <c r="S527" s="9">
+        <v>5</v>
+      </c>
+      <c r="T527" s="9">
+        <v>1</v>
+      </c>
+      <c r="U527" s="9">
+        <v>2</v>
+      </c>
+      <c r="V527" s="9">
+        <v>6</v>
+      </c>
+      <c r="W527" s="9">
+        <v>6</v>
+      </c>
+      <c r="X527" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y527" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z527" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA527" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB527" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC527" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD527" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE527" s="9">
+        <v>2</v>
+      </c>
+      <c r="AF527" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG527" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH527" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI527" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ527" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A528" s="4">
+        <v>45599.296636678242</v>
+      </c>
+      <c r="B528" s="5" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C528" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D528" s="5">
+        <v>20242418</v>
+      </c>
+      <c r="E528" s="5" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F528" s="6">
+        <v>0.29444444444379769</v>
+      </c>
+      <c r="G528" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H528" s="5">
+        <v>3</v>
+      </c>
+      <c r="I528" s="5">
+        <v>3</v>
+      </c>
+      <c r="J528" s="5">
+        <v>2</v>
+      </c>
+      <c r="K528" s="5">
+        <v>2</v>
+      </c>
+      <c r="L528" s="5">
+        <v>6</v>
+      </c>
+      <c r="M528" s="5">
+        <v>3</v>
+      </c>
+      <c r="N528" s="5">
+        <v>3</v>
+      </c>
+      <c r="O528" s="5">
+        <v>2</v>
+      </c>
+      <c r="P528" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q528" s="5">
+        <v>3</v>
+      </c>
+      <c r="R528" s="5">
+        <v>2</v>
+      </c>
+      <c r="S528" s="5">
+        <v>2</v>
+      </c>
+      <c r="T528" s="5">
+        <v>3</v>
+      </c>
+      <c r="U528" s="5">
+        <v>3</v>
+      </c>
+      <c r="V528" s="5">
+        <v>2</v>
+      </c>
+      <c r="W528" s="5">
+        <v>2</v>
+      </c>
+      <c r="X528" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y528" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z528" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA528" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB528" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC528" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD528" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE528" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF528" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG528" s="5">
+        <v>2</v>
+      </c>
+      <c r="AH528" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI528" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ528" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="529" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A529" s="8">
+        <v>45599.331503865746</v>
+      </c>
+      <c r="B529" s="9" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C529" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D529" s="9">
+        <v>20246741</v>
+      </c>
+      <c r="E529" s="9" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F529" s="10">
+        <v>0.33055555555620231</v>
+      </c>
+      <c r="G529" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY529" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL529" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM529" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="530" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A530" s="4">
+        <v>45599.336968125004</v>
+      </c>
+      <c r="B530" s="5" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C530" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D530" s="5">
+        <v>20241520</v>
+      </c>
+      <c r="E530" s="5" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F530" s="6">
+        <v>0.33472222222189885</v>
+      </c>
+      <c r="G530" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK530" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL530" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM530" s="5">
+        <v>6</v>
+      </c>
+      <c r="AN530" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO530" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP530" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ530" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR530" s="5">
+        <v>5</v>
+      </c>
+      <c r="AS530" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT530" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU530" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV530" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW530" s="5">
+        <v>5</v>
+      </c>
+      <c r="AX530" s="5">
+        <v>5</v>
+      </c>
+      <c r="AY530" s="5">
+        <v>6</v>
+      </c>
+      <c r="AZ530" s="5">
+        <v>5</v>
+      </c>
+      <c r="BA530" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB530" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC530" s="5">
+        <v>4</v>
+      </c>
+      <c r="BD530" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE530" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF530" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG530" s="5">
+        <v>3</v>
+      </c>
+      <c r="BH530" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI530" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ530" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK530" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL530" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM530" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="531" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A531" s="8">
+        <v>45599.355627395838</v>
+      </c>
+      <c r="B531" s="9" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C531" s="9" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D531" s="9">
+        <v>20216609</v>
+      </c>
+      <c r="E531" s="9" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F531" s="10">
+        <v>0.35486111111094942</v>
+      </c>
+      <c r="G531" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP531" s="9">
+        <v>2</v>
+      </c>
+      <c r="AQ531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR531" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS531" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU531" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX531" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY531" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BD531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BH531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BI531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BL531" s="9">
+        <v>4</v>
+      </c>
+      <c r="BM531" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="532" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A532" s="4">
+        <v>45599.356554618054</v>
+      </c>
+      <c r="B532" s="5" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C532" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D532" s="5">
+        <v>20182747</v>
+      </c>
+      <c r="E532" s="5" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F532" s="6">
+        <v>0.35416666666424135</v>
+      </c>
+      <c r="G532" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H532" s="5">
+        <v>3</v>
+      </c>
+      <c r="I532" s="5">
+        <v>3</v>
+      </c>
+      <c r="J532" s="5">
+        <v>4</v>
+      </c>
+      <c r="K532" s="5">
+        <v>2</v>
+      </c>
+      <c r="L532" s="5">
+        <v>2</v>
+      </c>
+      <c r="M532" s="5">
+        <v>3</v>
+      </c>
+      <c r="N532" s="5">
+        <v>3</v>
+      </c>
+      <c r="O532" s="5">
+        <v>3</v>
+      </c>
+      <c r="P532" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q532" s="5">
+        <v>2</v>
+      </c>
+      <c r="R532" s="5">
+        <v>5</v>
+      </c>
+      <c r="S532" s="5">
+        <v>3</v>
+      </c>
+      <c r="T532" s="5">
+        <v>3</v>
+      </c>
+      <c r="U532" s="5">
+        <v>3</v>
+      </c>
+      <c r="V532" s="5">
+        <v>4</v>
+      </c>
+      <c r="W532" s="5">
+        <v>6</v>
+      </c>
+      <c r="X532" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y532" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z532" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA532" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB532" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC532" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD532" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE532" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF532" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG532" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH532" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI532" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ532" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="533" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A533" s="8">
+        <v>45599.390445462966</v>
+      </c>
+      <c r="B533" s="9" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C533" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D533" s="9">
+        <v>20193420</v>
+      </c>
+      <c r="E533" s="9" t="s">
+        <v>1215</v>
+      </c>
+      <c r="F533" s="10">
+        <v>0.38611111111094942</v>
+      </c>
+      <c r="G533" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK533" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL533" s="9">
+        <v>4</v>
+      </c>
+      <c r="AM533" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN533" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO533" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP533" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ533" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR533" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS533" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT533" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU533" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV533" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW533" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX533" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY533" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ533" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA533" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB533" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC533" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD533" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE533" s="9">
+        <v>1</v>
+      </c>
+      <c r="BF533" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG533" s="9">
+        <v>4</v>
+      </c>
+      <c r="BH533" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI533" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ533" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK533" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL533" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM533" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="534" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A534" s="4">
+        <v>45599.393145624999</v>
+      </c>
+      <c r="B534" s="5" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C534" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D534" s="5">
+        <v>20232430</v>
+      </c>
+      <c r="E534" s="5" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F534" s="6">
+        <v>0.38958333333721384</v>
+      </c>
+      <c r="G534" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK534" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL534" s="5">
+        <v>2</v>
+      </c>
+      <c r="AM534" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN534" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO534" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP534" s="5">
+        <v>1</v>
+      </c>
+      <c r="AQ534" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR534" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS534" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT534" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU534" s="5">
+        <v>3</v>
+      </c>
+      <c r="AV534" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW534" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX534" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY534" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ534" s="5">
+        <v>2</v>
+      </c>
+      <c r="BA534" s="5">
+        <v>2</v>
+      </c>
+      <c r="BB534" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC534" s="5">
+        <v>1</v>
+      </c>
+      <c r="BD534" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE534" s="5">
+        <v>1</v>
+      </c>
+      <c r="BF534" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG534" s="5">
+        <v>5</v>
+      </c>
+      <c r="BH534" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI534" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ534" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK534" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL534" s="5">
+        <v>4</v>
+      </c>
+      <c r="BM534" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="535" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A535" s="8">
+        <v>45599.404944097223</v>
+      </c>
+      <c r="B535" s="9" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C535" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D535" s="9">
+        <v>20246281</v>
+      </c>
+      <c r="E535" s="9" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F535" s="10">
+        <v>0.40069444444088731</v>
+      </c>
+      <c r="G535" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H535" s="9">
+        <v>4</v>
+      </c>
+      <c r="I535" s="9">
+        <v>4</v>
+      </c>
+      <c r="J535" s="9">
+        <v>4</v>
+      </c>
+      <c r="K535" s="9">
+        <v>4</v>
+      </c>
+      <c r="L535" s="9">
+        <v>5</v>
+      </c>
+      <c r="M535" s="9">
+        <v>4</v>
+      </c>
+      <c r="N535" s="9">
+        <v>5</v>
+      </c>
+      <c r="O535" s="9">
+        <v>4</v>
+      </c>
+      <c r="P535" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q535" s="9">
+        <v>3</v>
+      </c>
+      <c r="R535" s="9">
+        <v>5</v>
+      </c>
+      <c r="S535" s="9">
+        <v>4</v>
+      </c>
+      <c r="T535" s="9">
+        <v>4</v>
+      </c>
+      <c r="U535" s="9">
+        <v>4</v>
+      </c>
+      <c r="V535" s="9">
+        <v>5</v>
+      </c>
+      <c r="W535" s="9">
+        <v>4</v>
+      </c>
+      <c r="X535" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y535" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z535" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA535" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB535" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC535" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD535" s="9">
+        <v>5</v>
+      </c>
+      <c r="AE535" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF535" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG535" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH535" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI535" s="9">
+        <v>5</v>
+      </c>
+      <c r="AJ535" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="536" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A536" s="4">
+        <v>45599.420231689815</v>
+      </c>
+      <c r="B536" s="5" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C536" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D536" s="5">
+        <v>20242932</v>
+      </c>
+      <c r="E536" s="5" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F536" s="6">
+        <v>0.4180555555576575</v>
+      </c>
+      <c r="G536" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H536" s="5">
+        <v>1</v>
+      </c>
+      <c r="I536" s="5">
+        <v>6</v>
+      </c>
+      <c r="J536" s="5">
+        <v>6</v>
+      </c>
+      <c r="K536" s="5">
+        <v>5</v>
+      </c>
+      <c r="L536" s="5">
+        <v>2</v>
+      </c>
+      <c r="M536" s="5">
+        <v>1</v>
+      </c>
+      <c r="N536" s="5">
+        <v>6</v>
+      </c>
+      <c r="O536" s="5">
+        <v>5</v>
+      </c>
+      <c r="P536" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q536" s="5">
+        <v>1</v>
+      </c>
+      <c r="R536" s="5">
+        <v>6</v>
+      </c>
+      <c r="S536" s="5">
+        <v>6</v>
+      </c>
+      <c r="T536" s="5">
+        <v>1</v>
+      </c>
+      <c r="U536" s="5">
+        <v>2</v>
+      </c>
+      <c r="V536" s="5">
+        <v>6</v>
+      </c>
+      <c r="W536" s="5">
+        <v>5</v>
+      </c>
+      <c r="X536" s="5">
+        <v>6</v>
+      </c>
+      <c r="Y536" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z536" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA536" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB536" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC536" s="5">
+        <v>6</v>
+      </c>
+      <c r="AD536" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE536" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF536" s="5">
+        <v>6</v>
+      </c>
+      <c r="AG536" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH536" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI536" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ536" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="537" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A537" s="8">
+        <v>45599.425269270832</v>
+      </c>
+      <c r="B537" s="9" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C537" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D537" s="9">
+        <v>20201076</v>
+      </c>
+      <c r="E537" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="F537" s="10">
+        <v>0.41666666666424135</v>
+      </c>
+      <c r="G537" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AL537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AM537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AN537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AO537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AP537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AQ537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AR537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AS537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AT537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AU537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AV537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AW537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AX537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AY537" s="9">
+        <v>6</v>
+      </c>
+      <c r="AZ537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BA537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BB537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BC537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BD537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BE537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BF537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BG537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BH537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BI537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BJ537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BK537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BL537" s="9">
+        <v>6</v>
+      </c>
+      <c r="BM537" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="538" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A538" s="4">
+        <v>45599.430936643519</v>
+      </c>
+      <c r="B538" s="5" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C538" s="5" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D538" s="5">
+        <v>20231033</v>
+      </c>
+      <c r="E538" s="5" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F538" s="6">
+        <v>0.429861111115315</v>
+      </c>
+      <c r="G538" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H538" s="5">
+        <v>1</v>
+      </c>
+      <c r="I538" s="5">
+        <v>4</v>
+      </c>
+      <c r="J538" s="5">
+        <v>4</v>
+      </c>
+      <c r="K538" s="5">
+        <v>4</v>
+      </c>
+      <c r="L538" s="5">
+        <v>2</v>
+      </c>
+      <c r="M538" s="5">
+        <v>2</v>
+      </c>
+      <c r="N538" s="5">
+        <v>3</v>
+      </c>
+      <c r="O538" s="5">
+        <v>3</v>
+      </c>
+      <c r="P538" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q538" s="5">
+        <v>4</v>
+      </c>
+      <c r="R538" s="5">
+        <v>5</v>
+      </c>
+      <c r="S538" s="5">
+        <v>4</v>
+      </c>
+      <c r="T538" s="5">
+        <v>3</v>
+      </c>
+      <c r="U538" s="5">
+        <v>3</v>
+      </c>
+      <c r="V538" s="5">
+        <v>4</v>
+      </c>
+      <c r="W538" s="5">
+        <v>4</v>
+      </c>
+      <c r="X538" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y538" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z538" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA538" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB538" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC538" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD538" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE538" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF538" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG538" s="5">
+        <v>2</v>
+      </c>
+      <c r="AH538" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI538" s="5">
+        <v>4</v>
+      </c>
+      <c r="AJ538" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="539" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A539" s="8">
+        <v>45599.436496967595</v>
+      </c>
+      <c r="B539" s="9" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C539" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D539" s="9">
+        <v>20232726</v>
+      </c>
+      <c r="E539" s="9" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F539" s="10">
+        <v>0.43333333333430346</v>
+      </c>
+      <c r="G539" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H539" s="9">
+        <v>5</v>
+      </c>
+      <c r="I539" s="9">
+        <v>5</v>
+      </c>
+      <c r="J539" s="9">
+        <v>4</v>
+      </c>
+      <c r="K539" s="9">
+        <v>4</v>
+      </c>
+      <c r="L539" s="9">
+        <v>3</v>
+      </c>
+      <c r="M539" s="9">
+        <v>5</v>
+      </c>
+      <c r="N539" s="9">
+        <v>5</v>
+      </c>
+      <c r="O539" s="9">
+        <v>5</v>
+      </c>
+      <c r="P539" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q539" s="9">
+        <v>5</v>
+      </c>
+      <c r="R539" s="9">
+        <v>4</v>
+      </c>
+      <c r="S539" s="9">
+        <v>4</v>
+      </c>
+      <c r="T539" s="9">
+        <v>4</v>
+      </c>
+      <c r="U539" s="9">
+        <v>2</v>
+      </c>
+      <c r="V539" s="9">
+        <v>5</v>
+      </c>
+      <c r="W539" s="9">
+        <v>5</v>
+      </c>
+      <c r="X539" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y539" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z539" s="9">
+        <v>5</v>
+      </c>
+      <c r="AA539" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB539" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC539" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD539" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE539" s="9">
+        <v>5</v>
+      </c>
+      <c r="AF539" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG539" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH539" s="9">
+        <v>5</v>
+      </c>
+      <c r="AI539" s="9">
+        <v>5</v>
+      </c>
+      <c r="AJ539" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="540" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A540" s="4">
+        <v>45599.439030879628</v>
+      </c>
+      <c r="B540" s="5" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C540" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D540" s="5">
+        <v>20245190</v>
+      </c>
+      <c r="E540" s="5" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F540" s="6">
+        <v>0.43819444444670808</v>
+      </c>
+      <c r="G540" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H540" s="5">
+        <v>4</v>
+      </c>
+      <c r="I540" s="5">
+        <v>4</v>
+      </c>
+      <c r="J540" s="5">
+        <v>4</v>
+      </c>
+      <c r="K540" s="5">
+        <v>4</v>
+      </c>
+      <c r="L540" s="5">
+        <v>1</v>
+      </c>
+      <c r="M540" s="5">
+        <v>1</v>
+      </c>
+      <c r="N540" s="5">
+        <v>4</v>
+      </c>
+      <c r="O540" s="5">
+        <v>4</v>
+      </c>
+      <c r="P540" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q540" s="5">
+        <v>1</v>
+      </c>
+      <c r="R540" s="5">
+        <v>4</v>
+      </c>
+      <c r="S540" s="5">
+        <v>4</v>
+      </c>
+      <c r="T540" s="5">
+        <v>1</v>
+      </c>
+      <c r="U540" s="5">
+        <v>1</v>
+      </c>
+      <c r="V540" s="5">
+        <v>4</v>
+      </c>
+      <c r="W540" s="5">
+        <v>4</v>
+      </c>
+      <c r="X540" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y540" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z540" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA540" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB540" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC540" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD540" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE540" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF540" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG540" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH540" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI540" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ540" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A541" s="18">
+        <v>45599.442593784726</v>
+      </c>
+      <c r="B541" s="19" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C541" s="19" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D541" s="19">
+        <v>20227162</v>
+      </c>
+      <c r="E541" s="19" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F541" s="20">
+        <v>0.43958333333284827</v>
+      </c>
+      <c r="G541" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H541" s="26"/>
+      <c r="I541" s="26"/>
+      <c r="J541" s="26"/>
+      <c r="K541" s="26"/>
+      <c r="L541" s="26"/>
+      <c r="M541" s="26"/>
+      <c r="N541" s="26"/>
+      <c r="O541" s="26"/>
+      <c r="P541" s="26"/>
+      <c r="Q541" s="26"/>
+      <c r="R541" s="26"/>
+      <c r="S541" s="26"/>
+      <c r="T541" s="26"/>
+      <c r="U541" s="26"/>
+      <c r="V541" s="26"/>
+      <c r="W541" s="26"/>
+      <c r="X541" s="26"/>
+      <c r="Y541" s="26"/>
+      <c r="Z541" s="26"/>
+      <c r="AA541" s="26"/>
+      <c r="AB541" s="26"/>
+      <c r="AC541" s="26"/>
+      <c r="AD541" s="26"/>
+      <c r="AE541" s="26"/>
+      <c r="AF541" s="26"/>
+      <c r="AG541" s="26"/>
+      <c r="AH541" s="26"/>
+      <c r="AI541" s="26"/>
+      <c r="AJ541" s="26"/>
+      <c r="AK541" s="19">
+        <v>2</v>
+      </c>
+      <c r="AL541" s="19">
+        <v>4</v>
+      </c>
+      <c r="AM541" s="19">
+        <v>4</v>
+      </c>
+      <c r="AN541" s="19">
+        <v>4</v>
+      </c>
+      <c r="AO541" s="19">
+        <v>2</v>
+      </c>
+      <c r="AP541" s="19">
+        <v>3</v>
+      </c>
+      <c r="AQ541" s="19">
+        <v>4</v>
+      </c>
+      <c r="AR541" s="19">
+        <v>4</v>
+      </c>
+      <c r="AS541" s="19">
+        <v>4</v>
+      </c>
+      <c r="AT541" s="19">
+        <v>2</v>
+      </c>
+      <c r="AU541" s="19">
+        <v>4</v>
+      </c>
+      <c r="AV541" s="19">
+        <v>4</v>
+      </c>
+      <c r="AW541" s="19">
+        <v>3</v>
+      </c>
+      <c r="AX541" s="19">
+        <v>3</v>
+      </c>
+      <c r="AY541" s="19">
+        <v>4</v>
+      </c>
+      <c r="AZ541" s="19">
+        <v>4</v>
+      </c>
+      <c r="BA541" s="19">
+        <v>4</v>
+      </c>
+      <c r="BB541" s="19">
+        <v>4</v>
+      </c>
+      <c r="BC541" s="19">
+        <v>4</v>
+      </c>
+      <c r="BD541" s="19">
+        <v>4</v>
+      </c>
+      <c r="BE541" s="19">
+        <v>3</v>
+      </c>
+      <c r="BF541" s="19">
+        <v>4</v>
+      </c>
+      <c r="BG541" s="19">
+        <v>3</v>
+      </c>
+      <c r="BH541" s="19">
+        <v>3</v>
+      </c>
+      <c r="BI541" s="19">
+        <v>3</v>
+      </c>
+      <c r="BJ541" s="19">
+        <v>4</v>
+      </c>
+      <c r="BK541" s="19">
+        <v>3</v>
+      </c>
+      <c r="BL541" s="19">
+        <v>2</v>
+      </c>
+      <c r="BM541" s="22">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
241021, oxford modified sunday 14:00
</commit_message>
<xml_diff>
--- a/R/data/oxford_241021.xlsx
+++ b/R/data/oxford_241021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Dropbox/내 Mac (Kee-Won의 MacBook Air)/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F8AFE5-C063-9640-84C0-29094A8AAE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F419D978-C7D9-FD47-9950-9677129BFC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42920" yWindow="1420" windowWidth="37080" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="1233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2359" uniqueCount="1307">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -3722,6 +3722,228 @@
   </si>
   <si>
     <t>조윤재</t>
+  </si>
+  <si>
+    <t>chanwoo0807@gmail.com</t>
+  </si>
+  <si>
+    <t>반도체 디스플레이</t>
+  </si>
+  <si>
+    <t>김찬우</t>
+  </si>
+  <si>
+    <t>ghskfen1215@naver.com</t>
+  </si>
+  <si>
+    <t>기정윤</t>
+  </si>
+  <si>
+    <t>soyeon2025@naver.com</t>
+  </si>
+  <si>
+    <t>soonbeom1130@naver.com</t>
+  </si>
+  <si>
+    <t>권순범</t>
+  </si>
+  <si>
+    <t>qudcksl1216@gmail.com</t>
+  </si>
+  <si>
+    <t>윤병찬</t>
+  </si>
+  <si>
+    <t>dudwndi09@naver.com</t>
+  </si>
+  <si>
+    <t>광고홍보</t>
+  </si>
+  <si>
+    <t>권영주</t>
+  </si>
+  <si>
+    <t>5tmddk@naver.com</t>
+  </si>
+  <si>
+    <t>최승아</t>
+  </si>
+  <si>
+    <t>mingtto0920@gmail.com</t>
+  </si>
+  <si>
+    <t>유민서</t>
+  </si>
+  <si>
+    <t>sueuisa04@gmail.com</t>
+  </si>
+  <si>
+    <t>인공지능융학부</t>
+  </si>
+  <si>
+    <t>신동윤</t>
+  </si>
+  <si>
+    <t>bmj4033@gmail.com</t>
+  </si>
+  <si>
+    <t>백민제</t>
+  </si>
+  <si>
+    <t>kt433@naver.com</t>
+  </si>
+  <si>
+    <t>주혜린</t>
+  </si>
+  <si>
+    <t>aks186@naver.com</t>
+  </si>
+  <si>
+    <t>안준선</t>
+  </si>
+  <si>
+    <t>csqwe2@naver.com</t>
+  </si>
+  <si>
+    <t>장재호</t>
+  </si>
+  <si>
+    <t>kty030122@gmail.com</t>
+  </si>
+  <si>
+    <t>김태연</t>
+  </si>
+  <si>
+    <t>kgh1321@gmail.com</t>
+  </si>
+  <si>
+    <t>김가희</t>
+  </si>
+  <si>
+    <t>wlgus4770752@naver.com</t>
+  </si>
+  <si>
+    <t>의예과</t>
+  </si>
+  <si>
+    <t>김지현</t>
+  </si>
+  <si>
+    <t>bhyejin420@gmail.com</t>
+  </si>
+  <si>
+    <t>박혜진</t>
+  </si>
+  <si>
+    <t>byl0730@naver.com</t>
+  </si>
+  <si>
+    <t>변예림</t>
+  </si>
+  <si>
+    <t>psh020509@naver.com</t>
+  </si>
+  <si>
+    <t>박시환</t>
+  </si>
+  <si>
+    <t>kje9714@gmail.com</t>
+  </si>
+  <si>
+    <t>김재은</t>
+  </si>
+  <si>
+    <t>to_csm@naver.com</t>
+  </si>
+  <si>
+    <t>천상미</t>
+  </si>
+  <si>
+    <t>dong45657@gmail.com</t>
+  </si>
+  <si>
+    <t>채동엽</t>
+  </si>
+  <si>
+    <t>koreavjr@naver.com</t>
+  </si>
+  <si>
+    <t>박지성</t>
+  </si>
+  <si>
+    <t>a01075976680@gmail.com</t>
+  </si>
+  <si>
+    <t>김우진</t>
+  </si>
+  <si>
+    <t>whrhdwn2003@gmail.com</t>
+  </si>
+  <si>
+    <t>조은서</t>
+  </si>
+  <si>
+    <t>abc6518@gmail.com</t>
+  </si>
+  <si>
+    <t>반도체</t>
+  </si>
+  <si>
+    <t>박상준</t>
+  </si>
+  <si>
+    <t>wndus6604@naver.com</t>
+  </si>
+  <si>
+    <t>남주연</t>
+  </si>
+  <si>
+    <t>chaseoyeon0103@naver.com</t>
+  </si>
+  <si>
+    <t>차서연</t>
+  </si>
+  <si>
+    <t>seoeunwkd@gmail.com</t>
+  </si>
+  <si>
+    <t>정서은</t>
+  </si>
+  <si>
+    <t>junwoni20@gmail.com</t>
+  </si>
+  <si>
+    <t>이준원</t>
+  </si>
+  <si>
+    <t>geonu4496@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">디지털미디어콘텐츠 </t>
+  </si>
+  <si>
+    <t>이건우</t>
+  </si>
+  <si>
+    <t>h20191240@glab.hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>홍이래</t>
+  </si>
+  <si>
+    <t>ereere05@naver.com</t>
+  </si>
+  <si>
+    <t>황은상</t>
+  </si>
+  <si>
+    <t>kdk3265@naver.com</t>
+  </si>
+  <si>
+    <t>언론방송융합미디어</t>
+  </si>
+  <si>
+    <t>강은비</t>
   </si>
 </sst>
 </file>
@@ -4165,7 +4387,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM541">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM575">
   <tableColumns count="65">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -4438,11 +4660,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM541"/>
+  <dimension ref="A1:BM575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A497" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D544" sqref="D544"/>
+      <pane ySplit="1" topLeftCell="A538" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C580" sqref="C580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -64856,35 +65078,6 @@
       <c r="G541" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H541" s="26"/>
-      <c r="I541" s="26"/>
-      <c r="J541" s="26"/>
-      <c r="K541" s="26"/>
-      <c r="L541" s="26"/>
-      <c r="M541" s="26"/>
-      <c r="N541" s="26"/>
-      <c r="O541" s="26"/>
-      <c r="P541" s="26"/>
-      <c r="Q541" s="26"/>
-      <c r="R541" s="26"/>
-      <c r="S541" s="26"/>
-      <c r="T541" s="26"/>
-      <c r="U541" s="26"/>
-      <c r="V541" s="26"/>
-      <c r="W541" s="26"/>
-      <c r="X541" s="26"/>
-      <c r="Y541" s="26"/>
-      <c r="Z541" s="26"/>
-      <c r="AA541" s="26"/>
-      <c r="AB541" s="26"/>
-      <c r="AC541" s="26"/>
-      <c r="AD541" s="26"/>
-      <c r="AE541" s="26"/>
-      <c r="AF541" s="26"/>
-      <c r="AG541" s="26"/>
-      <c r="AH541" s="26"/>
-      <c r="AI541" s="26"/>
-      <c r="AJ541" s="26"/>
       <c r="AK541" s="19">
         <v>2</v>
       </c>
@@ -64972,6 +65165,3775 @@
       <c r="BM541" s="22">
         <v>2</v>
       </c>
+    </row>
+    <row r="542" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A542" s="4">
+        <v>45599.452051828703</v>
+      </c>
+      <c r="B542" s="5" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C542" s="5" t="s">
+        <v>1234</v>
+      </c>
+      <c r="D542" s="5">
+        <v>20223316</v>
+      </c>
+      <c r="E542" s="5" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F542" s="6">
+        <v>0.44861111111094942</v>
+      </c>
+      <c r="G542" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H542" s="5">
+        <v>2</v>
+      </c>
+      <c r="I542" s="5">
+        <v>4</v>
+      </c>
+      <c r="J542" s="5">
+        <v>4</v>
+      </c>
+      <c r="K542" s="5">
+        <v>3</v>
+      </c>
+      <c r="L542" s="5">
+        <v>2</v>
+      </c>
+      <c r="M542" s="5">
+        <v>2</v>
+      </c>
+      <c r="N542" s="5">
+        <v>4</v>
+      </c>
+      <c r="O542" s="5">
+        <v>4</v>
+      </c>
+      <c r="P542" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q542" s="5">
+        <v>2</v>
+      </c>
+      <c r="R542" s="5">
+        <v>4</v>
+      </c>
+      <c r="S542" s="5">
+        <v>4</v>
+      </c>
+      <c r="T542" s="5">
+        <v>2</v>
+      </c>
+      <c r="U542" s="5">
+        <v>2</v>
+      </c>
+      <c r="V542" s="5">
+        <v>4</v>
+      </c>
+      <c r="W542" s="5">
+        <v>5</v>
+      </c>
+      <c r="X542" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y542" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z542" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA542" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB542" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC542" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD542" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE542" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF542" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG542" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH542" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI542" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ542" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="543" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A543" s="8">
+        <v>45599.461358506946</v>
+      </c>
+      <c r="B543" s="9" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C543" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D543" s="9">
+        <v>20236705</v>
+      </c>
+      <c r="E543" s="9" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F543" s="10">
+        <v>0.45902777777519077</v>
+      </c>
+      <c r="G543" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK543" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL543" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM543" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN543" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO543" s="9">
+        <v>2</v>
+      </c>
+      <c r="AP543" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ543" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR543" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS543" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT543" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU543" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV543" s="9">
+        <v>2</v>
+      </c>
+      <c r="AW543" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX543" s="9">
+        <v>4</v>
+      </c>
+      <c r="AY543" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ543" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA543" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB543" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC543" s="9">
+        <v>5</v>
+      </c>
+      <c r="BD543" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE543" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF543" s="9">
+        <v>2</v>
+      </c>
+      <c r="BG543" s="9">
+        <v>2</v>
+      </c>
+      <c r="BH543" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI543" s="9">
+        <v>1</v>
+      </c>
+      <c r="BJ543" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK543" s="9">
+        <v>4</v>
+      </c>
+      <c r="BL543" s="9">
+        <v>4</v>
+      </c>
+      <c r="BM543" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="544" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A544" s="4">
+        <v>45599.465858321761</v>
+      </c>
+      <c r="B544" s="5" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C544" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D544" s="5">
+        <v>20246221</v>
+      </c>
+      <c r="E544" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="F544" s="6">
+        <v>0.46319444444088731</v>
+      </c>
+      <c r="G544" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK544" s="5">
+        <v>3</v>
+      </c>
+      <c r="AL544" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM544" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN544" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO544" s="5">
+        <v>3</v>
+      </c>
+      <c r="AP544" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ544" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR544" s="5">
+        <v>5</v>
+      </c>
+      <c r="AS544" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT544" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU544" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV544" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW544" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX544" s="5">
+        <v>5</v>
+      </c>
+      <c r="AY544" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ544" s="5">
+        <v>6</v>
+      </c>
+      <c r="BA544" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB544" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC544" s="5">
+        <v>5</v>
+      </c>
+      <c r="BD544" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE544" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF544" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG544" s="5">
+        <v>3</v>
+      </c>
+      <c r="BH544" s="5">
+        <v>5</v>
+      </c>
+      <c r="BI544" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ544" s="5">
+        <v>6</v>
+      </c>
+      <c r="BK544" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL544" s="5">
+        <v>5</v>
+      </c>
+      <c r="BM544" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="545" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A545" s="8">
+        <v>45599.466416759256</v>
+      </c>
+      <c r="B545" s="9" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C545" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="D545" s="9">
+        <v>20235112</v>
+      </c>
+      <c r="E545" s="9" t="s">
+        <v>1240</v>
+      </c>
+      <c r="F545" s="10">
+        <v>0.46527777778101154</v>
+      </c>
+      <c r="G545" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK545" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL545" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM545" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN545" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO545" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP545" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ545" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR545" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS545" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT545" s="9">
+        <v>4</v>
+      </c>
+      <c r="AU545" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV545" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW545" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX545" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY545" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ545" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA545" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB545" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC545" s="9">
+        <v>4</v>
+      </c>
+      <c r="BD545" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE545" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF545" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG545" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH545" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI545" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ545" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK545" s="9">
+        <v>4</v>
+      </c>
+      <c r="BL545" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM545" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="546" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A546" s="4">
+        <v>45599.468864351853</v>
+      </c>
+      <c r="B546" s="5" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C546" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="D546" s="5">
+        <v>20192926</v>
+      </c>
+      <c r="E546" s="5" t="s">
+        <v>1242</v>
+      </c>
+      <c r="F546" s="6">
+        <v>0.46736111110658385</v>
+      </c>
+      <c r="G546" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H546" s="5">
+        <v>4</v>
+      </c>
+      <c r="I546" s="5">
+        <v>3</v>
+      </c>
+      <c r="J546" s="5">
+        <v>3</v>
+      </c>
+      <c r="K546" s="5">
+        <v>4</v>
+      </c>
+      <c r="L546" s="5">
+        <v>4</v>
+      </c>
+      <c r="M546" s="5">
+        <v>4</v>
+      </c>
+      <c r="N546" s="5">
+        <v>3</v>
+      </c>
+      <c r="O546" s="5">
+        <v>4</v>
+      </c>
+      <c r="P546" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q546" s="5">
+        <v>4</v>
+      </c>
+      <c r="R546" s="5">
+        <v>5</v>
+      </c>
+      <c r="S546" s="5">
+        <v>4</v>
+      </c>
+      <c r="T546" s="5">
+        <v>4</v>
+      </c>
+      <c r="U546" s="5">
+        <v>4</v>
+      </c>
+      <c r="V546" s="5">
+        <v>4</v>
+      </c>
+      <c r="W546" s="5">
+        <v>4</v>
+      </c>
+      <c r="X546" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y546" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z546" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA546" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB546" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC546" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD546" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE546" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF546" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG546" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH546" s="5">
+        <v>4</v>
+      </c>
+      <c r="AI546" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ546" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="547" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A547" s="8">
+        <v>45599.491471967594</v>
+      </c>
+      <c r="B547" s="9" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C547" s="9" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D547" s="9">
+        <v>20212603</v>
+      </c>
+      <c r="E547" s="9" t="s">
+        <v>1245</v>
+      </c>
+      <c r="F547" s="10">
+        <v>0.49097222222189885</v>
+      </c>
+      <c r="G547" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H547" s="9">
+        <v>3</v>
+      </c>
+      <c r="I547" s="9">
+        <v>4</v>
+      </c>
+      <c r="J547" s="9">
+        <v>3</v>
+      </c>
+      <c r="K547" s="9">
+        <v>4</v>
+      </c>
+      <c r="L547" s="9">
+        <v>3</v>
+      </c>
+      <c r="M547" s="9">
+        <v>3</v>
+      </c>
+      <c r="N547" s="9">
+        <v>4</v>
+      </c>
+      <c r="O547" s="9">
+        <v>4</v>
+      </c>
+      <c r="P547" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q547" s="9">
+        <v>3</v>
+      </c>
+      <c r="R547" s="9">
+        <v>3</v>
+      </c>
+      <c r="S547" s="9">
+        <v>3</v>
+      </c>
+      <c r="T547" s="9">
+        <v>4</v>
+      </c>
+      <c r="U547" s="9">
+        <v>3</v>
+      </c>
+      <c r="V547" s="9">
+        <v>4</v>
+      </c>
+      <c r="W547" s="9">
+        <v>4</v>
+      </c>
+      <c r="X547" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y547" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z547" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA547" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB547" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC547" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD547" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE547" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF547" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG547" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH547" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI547" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ547" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="548" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A548" s="4">
+        <v>45599.496055983793</v>
+      </c>
+      <c r="B548" s="5" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C548" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D548" s="5">
+        <v>20192634</v>
+      </c>
+      <c r="E548" s="5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F548" s="6">
+        <v>0.49375000000145519</v>
+      </c>
+      <c r="G548" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H548" s="5">
+        <v>1</v>
+      </c>
+      <c r="I548" s="5">
+        <v>4</v>
+      </c>
+      <c r="J548" s="5">
+        <v>5</v>
+      </c>
+      <c r="K548" s="5">
+        <v>5</v>
+      </c>
+      <c r="L548" s="5">
+        <v>2</v>
+      </c>
+      <c r="M548" s="5">
+        <v>1</v>
+      </c>
+      <c r="N548" s="5">
+        <v>5</v>
+      </c>
+      <c r="O548" s="5">
+        <v>4</v>
+      </c>
+      <c r="P548" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q548" s="5">
+        <v>1</v>
+      </c>
+      <c r="R548" s="5">
+        <v>6</v>
+      </c>
+      <c r="S548" s="5">
+        <v>5</v>
+      </c>
+      <c r="T548" s="5">
+        <v>1</v>
+      </c>
+      <c r="U548" s="5">
+        <v>2</v>
+      </c>
+      <c r="V548" s="5">
+        <v>5</v>
+      </c>
+      <c r="W548" s="5">
+        <v>6</v>
+      </c>
+      <c r="X548" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y548" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z548" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA548" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB548" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC548" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD548" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE548" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF548" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG548" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH548" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI548" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ548" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="549" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A549" s="8">
+        <v>45599.505431423611</v>
+      </c>
+      <c r="B549" s="9" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C549" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D549" s="9">
+        <v>20242540</v>
+      </c>
+      <c r="E549" s="9" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F549" s="10">
+        <v>0.50208333333284827</v>
+      </c>
+      <c r="G549" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK549" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL549" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM549" s="9">
+        <v>2</v>
+      </c>
+      <c r="AN549" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO549" s="9">
+        <v>2</v>
+      </c>
+      <c r="AP549" s="9">
+        <v>5</v>
+      </c>
+      <c r="AQ549" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR549" s="9">
+        <v>5</v>
+      </c>
+      <c r="AS549" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT549" s="9">
+        <v>6</v>
+      </c>
+      <c r="AU549" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV549" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW549" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX549" s="9">
+        <v>5</v>
+      </c>
+      <c r="AY549" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ549" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA549" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB549" s="9">
+        <v>5</v>
+      </c>
+      <c r="BC549" s="9">
+        <v>5</v>
+      </c>
+      <c r="BD549" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE549" s="9">
+        <v>2</v>
+      </c>
+      <c r="BF549" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG549" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH549" s="9">
+        <v>5</v>
+      </c>
+      <c r="BI549" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ549" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK549" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL549" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM549" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="550" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A550" s="4">
+        <v>45599.513808113421</v>
+      </c>
+      <c r="B550" s="5" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C550" s="5" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D550" s="5">
+        <v>20236739</v>
+      </c>
+      <c r="E550" s="5" t="s">
+        <v>1252</v>
+      </c>
+      <c r="F550" s="6">
+        <v>0.51041666666424135</v>
+      </c>
+      <c r="G550" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK550" s="5">
+        <v>3</v>
+      </c>
+      <c r="AL550" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM550" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN550" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO550" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP550" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ550" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR550" s="5">
+        <v>5</v>
+      </c>
+      <c r="AS550" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT550" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU550" s="5">
+        <v>4</v>
+      </c>
+      <c r="AV550" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW550" s="5">
+        <v>5</v>
+      </c>
+      <c r="AX550" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY550" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ550" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA550" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB550" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC550" s="5">
+        <v>4</v>
+      </c>
+      <c r="BD550" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE550" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF550" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG550" s="5">
+        <v>5</v>
+      </c>
+      <c r="BH550" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI550" s="5">
+        <v>3</v>
+      </c>
+      <c r="BJ550" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK550" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL550" s="5">
+        <v>2</v>
+      </c>
+      <c r="BM550" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="551" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A551" s="8">
+        <v>45599.533016030095</v>
+      </c>
+      <c r="B551" s="9" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C551" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="D551" s="9">
+        <v>20231712</v>
+      </c>
+      <c r="E551" s="9" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F551" s="10">
+        <v>0.52986111110658385</v>
+      </c>
+      <c r="G551" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H551" s="9">
+        <v>2</v>
+      </c>
+      <c r="I551" s="9">
+        <v>5</v>
+      </c>
+      <c r="J551" s="9">
+        <v>6</v>
+      </c>
+      <c r="K551" s="9">
+        <v>5</v>
+      </c>
+      <c r="L551" s="9">
+        <v>4</v>
+      </c>
+      <c r="M551" s="9">
+        <v>3</v>
+      </c>
+      <c r="N551" s="9">
+        <v>5</v>
+      </c>
+      <c r="O551" s="9">
+        <v>4</v>
+      </c>
+      <c r="P551" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q551" s="9">
+        <v>3</v>
+      </c>
+      <c r="R551" s="9">
+        <v>6</v>
+      </c>
+      <c r="S551" s="9">
+        <v>5</v>
+      </c>
+      <c r="T551" s="9">
+        <v>3</v>
+      </c>
+      <c r="U551" s="9">
+        <v>4</v>
+      </c>
+      <c r="V551" s="9">
+        <v>5</v>
+      </c>
+      <c r="W551" s="9">
+        <v>5</v>
+      </c>
+      <c r="X551" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y551" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z551" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA551" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB551" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC551" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD551" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE551" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF551" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG551" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH551" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI551" s="9">
+        <v>5</v>
+      </c>
+      <c r="AJ551" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="552" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A552" s="4">
+        <v>45599.533469756949</v>
+      </c>
+      <c r="B552" s="5" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C552" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D552" s="5">
+        <v>20222361</v>
+      </c>
+      <c r="E552" s="5" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F552" s="6">
+        <v>0.53055555555329192</v>
+      </c>
+      <c r="G552" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK552" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO552" s="5">
+        <v>2</v>
+      </c>
+      <c r="AP552" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT552" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AV552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW552" s="5">
+        <v>2</v>
+      </c>
+      <c r="AX552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY552" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ552" s="5">
+        <v>3</v>
+      </c>
+      <c r="BA552" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB552" s="5">
+        <v>3</v>
+      </c>
+      <c r="BC552" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD552" s="5">
+        <v>3</v>
+      </c>
+      <c r="BE552" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF552" s="5">
+        <v>3</v>
+      </c>
+      <c r="BG552" s="5">
+        <v>2</v>
+      </c>
+      <c r="BH552" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI552" s="5">
+        <v>3</v>
+      </c>
+      <c r="BJ552" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK552" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL552" s="5">
+        <v>2</v>
+      </c>
+      <c r="BM552" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="553" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A553" s="8">
+        <v>45599.534865844907</v>
+      </c>
+      <c r="B553" s="9" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C553" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D553" s="9">
+        <v>20232728</v>
+      </c>
+      <c r="E553" s="9" t="s">
+        <v>1258</v>
+      </c>
+      <c r="F553" s="10">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G553" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK553" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL553" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM553" s="9">
+        <v>6</v>
+      </c>
+      <c r="AN553" s="9">
+        <v>6</v>
+      </c>
+      <c r="AO553" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP553" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ553" s="9">
+        <v>4</v>
+      </c>
+      <c r="AR553" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS553" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT553" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU553" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV553" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW553" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX553" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY553" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ553" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA553" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB553" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC553" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD553" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE553" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF553" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG553" s="9">
+        <v>2</v>
+      </c>
+      <c r="BH553" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI553" s="9">
+        <v>5</v>
+      </c>
+      <c r="BJ553" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK553" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL553" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM553" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="554" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A554" s="4">
+        <v>45599.536409166671</v>
+      </c>
+      <c r="B554" s="5" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C554" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D554" s="5">
+        <v>20196638</v>
+      </c>
+      <c r="E554" s="5" t="s">
+        <v>1260</v>
+      </c>
+      <c r="F554" s="6">
+        <v>0.53055555555329192</v>
+      </c>
+      <c r="G554" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK554" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL554" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM554" s="5">
+        <v>2</v>
+      </c>
+      <c r="AN554" s="5">
+        <v>1</v>
+      </c>
+      <c r="AO554" s="5">
+        <v>2</v>
+      </c>
+      <c r="AP554" s="5">
+        <v>6</v>
+      </c>
+      <c r="AQ554" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR554" s="5">
+        <v>2</v>
+      </c>
+      <c r="AS554" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT554" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU554" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV554" s="5">
+        <v>1</v>
+      </c>
+      <c r="AW554" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX554" s="5">
+        <v>1</v>
+      </c>
+      <c r="AY554" s="5">
+        <v>4</v>
+      </c>
+      <c r="AZ554" s="5">
+        <v>5</v>
+      </c>
+      <c r="BA554" s="5">
+        <v>1</v>
+      </c>
+      <c r="BB554" s="5">
+        <v>2</v>
+      </c>
+      <c r="BC554" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD554" s="5">
+        <v>1</v>
+      </c>
+      <c r="BE554" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF554" s="5">
+        <v>6</v>
+      </c>
+      <c r="BG554" s="5">
+        <v>1</v>
+      </c>
+      <c r="BH554" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI554" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ554" s="5">
+        <v>2</v>
+      </c>
+      <c r="BK554" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL554" s="5">
+        <v>6</v>
+      </c>
+      <c r="BM554" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="555" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A555" s="8">
+        <v>45599.537873796296</v>
+      </c>
+      <c r="B555" s="9" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C555" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D555" s="9">
+        <v>20214113</v>
+      </c>
+      <c r="E555" s="9" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F555" s="10">
+        <v>0.53611111111240461</v>
+      </c>
+      <c r="G555" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H555" s="9">
+        <v>1</v>
+      </c>
+      <c r="I555" s="9">
+        <v>4</v>
+      </c>
+      <c r="J555" s="9">
+        <v>5</v>
+      </c>
+      <c r="K555" s="9">
+        <v>4</v>
+      </c>
+      <c r="L555" s="9">
+        <v>2</v>
+      </c>
+      <c r="M555" s="9">
+        <v>1</v>
+      </c>
+      <c r="N555" s="9">
+        <v>4</v>
+      </c>
+      <c r="O555" s="9">
+        <v>4</v>
+      </c>
+      <c r="P555" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q555" s="9">
+        <v>5</v>
+      </c>
+      <c r="R555" s="9">
+        <v>5</v>
+      </c>
+      <c r="S555" s="9">
+        <v>5</v>
+      </c>
+      <c r="T555" s="9">
+        <v>1</v>
+      </c>
+      <c r="U555" s="9">
+        <v>3</v>
+      </c>
+      <c r="V555" s="9">
+        <v>6</v>
+      </c>
+      <c r="W555" s="9">
+        <v>6</v>
+      </c>
+      <c r="X555" s="9">
+        <v>6</v>
+      </c>
+      <c r="Y555" s="9">
+        <v>6</v>
+      </c>
+      <c r="Z555" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA555" s="9">
+        <v>6</v>
+      </c>
+      <c r="AB555" s="9">
+        <v>6</v>
+      </c>
+      <c r="AC555" s="9">
+        <v>6</v>
+      </c>
+      <c r="AD555" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE555" s="9">
+        <v>2</v>
+      </c>
+      <c r="AF555" s="9">
+        <v>6</v>
+      </c>
+      <c r="AG555" s="9">
+        <v>6</v>
+      </c>
+      <c r="AH555" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI555" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ555" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="556" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A556" s="4">
+        <v>45599.541646724538</v>
+      </c>
+      <c r="B556" s="5" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C556" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D556" s="5">
+        <v>20242914</v>
+      </c>
+      <c r="E556" s="5" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F556" s="6">
+        <v>0.54027777777810115</v>
+      </c>
+      <c r="G556" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H556" s="5">
+        <v>2</v>
+      </c>
+      <c r="I556" s="5">
+        <v>2</v>
+      </c>
+      <c r="J556" s="5">
+        <v>3</v>
+      </c>
+      <c r="K556" s="5">
+        <v>3</v>
+      </c>
+      <c r="L556" s="5">
+        <v>2</v>
+      </c>
+      <c r="M556" s="5">
+        <v>2</v>
+      </c>
+      <c r="N556" s="5">
+        <v>3</v>
+      </c>
+      <c r="O556" s="5">
+        <v>3</v>
+      </c>
+      <c r="P556" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q556" s="5">
+        <v>2</v>
+      </c>
+      <c r="R556" s="5">
+        <v>3</v>
+      </c>
+      <c r="S556" s="5">
+        <v>3</v>
+      </c>
+      <c r="T556" s="5">
+        <v>2</v>
+      </c>
+      <c r="U556" s="5">
+        <v>2</v>
+      </c>
+      <c r="V556" s="5">
+        <v>3</v>
+      </c>
+      <c r="W556" s="5">
+        <v>3</v>
+      </c>
+      <c r="X556" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y556" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z556" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA556" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB556" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC556" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD556" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE556" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF556" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG556" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH556" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI556" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ556" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="557" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A557" s="8">
+        <v>45599.542223900462</v>
+      </c>
+      <c r="B557" s="9" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C557" s="9" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D557" s="9">
+        <v>20236121</v>
+      </c>
+      <c r="E557" s="9" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F557" s="10">
+        <v>0.54166666666424135</v>
+      </c>
+      <c r="G557" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H557" s="9">
+        <v>6</v>
+      </c>
+      <c r="I557" s="9">
+        <v>4</v>
+      </c>
+      <c r="J557" s="9">
+        <v>1</v>
+      </c>
+      <c r="K557" s="9">
+        <v>1</v>
+      </c>
+      <c r="L557" s="9">
+        <v>5</v>
+      </c>
+      <c r="M557" s="9">
+        <v>5</v>
+      </c>
+      <c r="N557" s="9">
+        <v>1</v>
+      </c>
+      <c r="O557" s="9">
+        <v>2</v>
+      </c>
+      <c r="P557" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q557" s="9">
+        <v>5</v>
+      </c>
+      <c r="R557" s="9">
+        <v>2</v>
+      </c>
+      <c r="S557" s="9">
+        <v>1</v>
+      </c>
+      <c r="T557" s="9">
+        <v>5</v>
+      </c>
+      <c r="U557" s="9">
+        <v>3</v>
+      </c>
+      <c r="V557" s="9">
+        <v>2</v>
+      </c>
+      <c r="W557" s="9">
+        <v>2</v>
+      </c>
+      <c r="X557" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y557" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z557" s="9">
+        <v>5</v>
+      </c>
+      <c r="AA557" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB557" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC557" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD557" s="9">
+        <v>5</v>
+      </c>
+      <c r="AE557" s="9">
+        <v>5</v>
+      </c>
+      <c r="AF557" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG557" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH557" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI557" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ557" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="558" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A558" s="4">
+        <v>45599.542298819448</v>
+      </c>
+      <c r="B558" s="5" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C558" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D558" s="5">
+        <v>20245176</v>
+      </c>
+      <c r="E558" s="5" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F558" s="6">
+        <v>0.53819444444525288</v>
+      </c>
+      <c r="G558" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H558" s="5">
+        <v>3</v>
+      </c>
+      <c r="I558" s="5">
+        <v>3</v>
+      </c>
+      <c r="J558" s="5">
+        <v>3</v>
+      </c>
+      <c r="K558" s="5">
+        <v>2</v>
+      </c>
+      <c r="L558" s="5">
+        <v>3</v>
+      </c>
+      <c r="M558" s="5">
+        <v>4</v>
+      </c>
+      <c r="N558" s="5">
+        <v>2</v>
+      </c>
+      <c r="O558" s="5">
+        <v>1</v>
+      </c>
+      <c r="P558" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q558" s="5">
+        <v>4</v>
+      </c>
+      <c r="R558" s="5">
+        <v>4</v>
+      </c>
+      <c r="S558" s="5">
+        <v>3</v>
+      </c>
+      <c r="T558" s="5">
+        <v>3</v>
+      </c>
+      <c r="U558" s="5">
+        <v>3</v>
+      </c>
+      <c r="V558" s="5">
+        <v>3</v>
+      </c>
+      <c r="W558" s="5">
+        <v>4</v>
+      </c>
+      <c r="X558" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y558" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z558" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA558" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB558" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC558" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD558" s="5">
+        <v>5</v>
+      </c>
+      <c r="AE558" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF558" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG558" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH558" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI558" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ558" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="559" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A559" s="8">
+        <v>45599.544533460648</v>
+      </c>
+      <c r="B559" s="9" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C559" s="9">
+        <v>20243715</v>
+      </c>
+      <c r="D559" s="9">
+        <v>20243715</v>
+      </c>
+      <c r="E559" s="9" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F559" s="10">
+        <v>0.46041666666860692</v>
+      </c>
+      <c r="G559" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H559" s="9">
+        <v>4</v>
+      </c>
+      <c r="I559" s="9">
+        <v>4</v>
+      </c>
+      <c r="J559" s="9">
+        <v>4</v>
+      </c>
+      <c r="K559" s="9">
+        <v>4</v>
+      </c>
+      <c r="L559" s="9">
+        <v>2</v>
+      </c>
+      <c r="M559" s="9">
+        <v>2</v>
+      </c>
+      <c r="N559" s="9">
+        <v>4</v>
+      </c>
+      <c r="O559" s="9">
+        <v>4</v>
+      </c>
+      <c r="P559" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q559" s="9">
+        <v>2</v>
+      </c>
+      <c r="R559" s="9">
+        <v>4</v>
+      </c>
+      <c r="S559" s="9">
+        <v>4</v>
+      </c>
+      <c r="T559" s="9">
+        <v>4</v>
+      </c>
+      <c r="U559" s="9">
+        <v>4</v>
+      </c>
+      <c r="V559" s="9">
+        <v>5</v>
+      </c>
+      <c r="W559" s="9">
+        <v>4</v>
+      </c>
+      <c r="X559" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y559" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z559" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA559" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB559" s="9">
+        <v>2</v>
+      </c>
+      <c r="AC559" s="9">
+        <v>2</v>
+      </c>
+      <c r="AD559" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE559" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF559" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG559" s="9">
+        <v>2</v>
+      </c>
+      <c r="AH559" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI559" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ559" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="560" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A560" s="4">
+        <v>45599.544612372687</v>
+      </c>
+      <c r="B560" s="5" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C560" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D560" s="5">
+        <v>20212820</v>
+      </c>
+      <c r="E560" s="5" t="s">
+        <v>1273</v>
+      </c>
+      <c r="F560" s="6">
+        <v>0.54374999999708962</v>
+      </c>
+      <c r="G560" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK560" s="5">
+        <v>3</v>
+      </c>
+      <c r="AL560" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM560" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN560" s="5">
+        <v>2</v>
+      </c>
+      <c r="AO560" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP560" s="5">
+        <v>3</v>
+      </c>
+      <c r="AQ560" s="5">
+        <v>2</v>
+      </c>
+      <c r="AR560" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS560" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT560" s="5">
+        <v>3</v>
+      </c>
+      <c r="AU560" s="5">
+        <v>3</v>
+      </c>
+      <c r="AV560" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW560" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX560" s="5">
+        <v>2</v>
+      </c>
+      <c r="AY560" s="5">
+        <v>2</v>
+      </c>
+      <c r="AZ560" s="5">
+        <v>2</v>
+      </c>
+      <c r="BA560" s="5">
+        <v>2</v>
+      </c>
+      <c r="BB560" s="5">
+        <v>2</v>
+      </c>
+      <c r="BC560" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD560" s="5">
+        <v>2</v>
+      </c>
+      <c r="BE560" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF560" s="5">
+        <v>3</v>
+      </c>
+      <c r="BG560" s="5">
+        <v>2</v>
+      </c>
+      <c r="BH560" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI560" s="5">
+        <v>3</v>
+      </c>
+      <c r="BJ560" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK560" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL560" s="5">
+        <v>5</v>
+      </c>
+      <c r="BM560" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="561" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A561" s="8">
+        <v>45599.545339930555</v>
+      </c>
+      <c r="B561" s="9" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C561" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="D561" s="9">
+        <v>20233509</v>
+      </c>
+      <c r="E561" s="9" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F561" s="10">
+        <v>0.54444444444379769</v>
+      </c>
+      <c r="G561" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK561" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL561" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM561" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN561" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO561" s="9">
+        <v>2</v>
+      </c>
+      <c r="AP561" s="9">
+        <v>2</v>
+      </c>
+      <c r="AQ561" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR561" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS561" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT561" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU561" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV561" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW561" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX561" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY561" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ561" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA561" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB561" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC561" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD561" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE561" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF561" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG561" s="9">
+        <v>1</v>
+      </c>
+      <c r="BH561" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI561" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ561" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK561" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL561" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM561" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="562" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A562" s="4">
+        <v>45599.546892395832</v>
+      </c>
+      <c r="B562" s="5" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C562" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D562" s="5">
+        <v>20242844</v>
+      </c>
+      <c r="E562" s="5" t="s">
+        <v>1277</v>
+      </c>
+      <c r="F562" s="6">
+        <v>0.54513888889050577</v>
+      </c>
+      <c r="G562" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK562" s="5">
+        <v>5</v>
+      </c>
+      <c r="AL562" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM562" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN562" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO562" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP562" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ562" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR562" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS562" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT562" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU562" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV562" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW562" s="5">
+        <v>5</v>
+      </c>
+      <c r="AX562" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY562" s="5">
+        <v>4</v>
+      </c>
+      <c r="AZ562" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA562" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB562" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC562" s="5">
+        <v>5</v>
+      </c>
+      <c r="BD562" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE562" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF562" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG562" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH562" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI562" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ562" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK562" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL562" s="5">
+        <v>4</v>
+      </c>
+      <c r="BM562" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="563" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A563" s="8">
+        <v>45599.550257222218</v>
+      </c>
+      <c r="B563" s="9" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C563" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="D563" s="9">
+        <v>20193429</v>
+      </c>
+      <c r="E563" s="9" t="s">
+        <v>1279</v>
+      </c>
+      <c r="F563" s="10">
+        <v>0.54513888889050577</v>
+      </c>
+      <c r="G563" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK563" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL563" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM563" s="9">
+        <v>2</v>
+      </c>
+      <c r="AN563" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO563" s="9">
+        <v>5</v>
+      </c>
+      <c r="AP563" s="9">
+        <v>2</v>
+      </c>
+      <c r="AQ563" s="9">
+        <v>2</v>
+      </c>
+      <c r="AR563" s="9">
+        <v>2</v>
+      </c>
+      <c r="AS563" s="9">
+        <v>2</v>
+      </c>
+      <c r="AT563" s="9">
+        <v>4</v>
+      </c>
+      <c r="AU563" s="9">
+        <v>2</v>
+      </c>
+      <c r="AV563" s="9">
+        <v>2</v>
+      </c>
+      <c r="AW563" s="9">
+        <v>4</v>
+      </c>
+      <c r="AX563" s="9">
+        <v>5</v>
+      </c>
+      <c r="AY563" s="9">
+        <v>2</v>
+      </c>
+      <c r="AZ563" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA563" s="9">
+        <v>2</v>
+      </c>
+      <c r="BB563" s="9">
+        <v>2</v>
+      </c>
+      <c r="BC563" s="9">
+        <v>4</v>
+      </c>
+      <c r="BD563" s="9">
+        <v>2</v>
+      </c>
+      <c r="BE563" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF563" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG563" s="9">
+        <v>4</v>
+      </c>
+      <c r="BH563" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI563" s="9">
+        <v>2</v>
+      </c>
+      <c r="BJ563" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK563" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL563" s="9">
+        <v>4</v>
+      </c>
+      <c r="BM563" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="564" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A564" s="4">
+        <v>45599.551279039355</v>
+      </c>
+      <c r="B564" s="5" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C564" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D564" s="5">
+        <v>20212827</v>
+      </c>
+      <c r="E564" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F564" s="6">
+        <v>0.52986111110658385</v>
+      </c>
+      <c r="G564" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H564" s="5">
+        <v>6</v>
+      </c>
+      <c r="I564" s="5">
+        <v>3</v>
+      </c>
+      <c r="J564" s="5">
+        <v>6</v>
+      </c>
+      <c r="K564" s="5">
+        <v>4</v>
+      </c>
+      <c r="L564" s="5">
+        <v>1</v>
+      </c>
+      <c r="M564" s="5">
+        <v>1</v>
+      </c>
+      <c r="N564" s="5">
+        <v>6</v>
+      </c>
+      <c r="O564" s="5">
+        <v>5</v>
+      </c>
+      <c r="P564" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q564" s="5">
+        <v>1</v>
+      </c>
+      <c r="R564" s="5">
+        <v>5</v>
+      </c>
+      <c r="S564" s="5">
+        <v>5</v>
+      </c>
+      <c r="T564" s="5">
+        <v>1</v>
+      </c>
+      <c r="U564" s="5">
+        <v>3</v>
+      </c>
+      <c r="V564" s="5">
+        <v>5</v>
+      </c>
+      <c r="W564" s="5">
+        <v>5</v>
+      </c>
+      <c r="X564" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y564" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z564" s="5">
+        <v>6</v>
+      </c>
+      <c r="AA564" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB564" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC564" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD564" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE564" s="5">
+        <v>6</v>
+      </c>
+      <c r="AF564" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG564" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH564" s="5">
+        <v>5</v>
+      </c>
+      <c r="AI564" s="5">
+        <v>5</v>
+      </c>
+      <c r="AJ564" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="565" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A565" s="8">
+        <v>45599.557771782405</v>
+      </c>
+      <c r="B565" s="9" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C565" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D565" s="9">
+        <v>20243309</v>
+      </c>
+      <c r="E565" s="9" t="s">
+        <v>1283</v>
+      </c>
+      <c r="F565" s="10">
+        <v>0.55625000000145519</v>
+      </c>
+      <c r="G565" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H565" s="9">
+        <v>1</v>
+      </c>
+      <c r="I565" s="9">
+        <v>4</v>
+      </c>
+      <c r="J565" s="9">
+        <v>5</v>
+      </c>
+      <c r="K565" s="9">
+        <v>4</v>
+      </c>
+      <c r="L565" s="9">
+        <v>1</v>
+      </c>
+      <c r="M565" s="9">
+        <v>3</v>
+      </c>
+      <c r="N565" s="9">
+        <v>5</v>
+      </c>
+      <c r="O565" s="9">
+        <v>3</v>
+      </c>
+      <c r="P565" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q565" s="9">
+        <v>3</v>
+      </c>
+      <c r="R565" s="9">
+        <v>6</v>
+      </c>
+      <c r="S565" s="9">
+        <v>4</v>
+      </c>
+      <c r="T565" s="9">
+        <v>2</v>
+      </c>
+      <c r="U565" s="9">
+        <v>4</v>
+      </c>
+      <c r="V565" s="9">
+        <v>6</v>
+      </c>
+      <c r="W565" s="9">
+        <v>4</v>
+      </c>
+      <c r="X565" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y565" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z565" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA565" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB565" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC565" s="9">
+        <v>6</v>
+      </c>
+      <c r="AD565" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE565" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF565" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG565" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH565" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI565" s="9">
+        <v>4</v>
+      </c>
+      <c r="AJ565" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="566" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A566" s="4">
+        <v>45599.557835312502</v>
+      </c>
+      <c r="B566" s="5" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C566" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D566" s="5">
+        <v>20232750</v>
+      </c>
+      <c r="E566" s="5" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F566" s="6">
+        <v>0.54583333333721384</v>
+      </c>
+      <c r="G566" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK566" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL566" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM566" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN566" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO566" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP566" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ566" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR566" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS566" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT566" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU566" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV566" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW566" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX566" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY566" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ566" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA566" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB566" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC566" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD566" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE566" s="5">
+        <v>2</v>
+      </c>
+      <c r="BF566" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG566" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH566" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI566" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ566" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK566" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL566" s="5">
+        <v>2</v>
+      </c>
+      <c r="BM566" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="567" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A567" s="8">
+        <v>45599.559689895832</v>
+      </c>
+      <c r="B567" s="9" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C567" s="9" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D567" s="9">
+        <v>20203322</v>
+      </c>
+      <c r="E567" s="9" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F567" s="10">
+        <v>0.55763888888759539</v>
+      </c>
+      <c r="G567" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H567" s="9">
+        <v>3</v>
+      </c>
+      <c r="I567" s="9">
+        <v>3</v>
+      </c>
+      <c r="J567" s="9">
+        <v>2</v>
+      </c>
+      <c r="K567" s="9">
+        <v>2</v>
+      </c>
+      <c r="L567" s="9">
+        <v>2</v>
+      </c>
+      <c r="M567" s="9">
+        <v>4</v>
+      </c>
+      <c r="N567" s="9">
+        <v>4</v>
+      </c>
+      <c r="O567" s="9">
+        <v>2</v>
+      </c>
+      <c r="P567" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q567" s="9">
+        <v>2</v>
+      </c>
+      <c r="R567" s="9">
+        <v>4</v>
+      </c>
+      <c r="S567" s="9">
+        <v>3</v>
+      </c>
+      <c r="T567" s="9">
+        <v>4</v>
+      </c>
+      <c r="U567" s="9">
+        <v>4</v>
+      </c>
+      <c r="V567" s="9">
+        <v>3</v>
+      </c>
+      <c r="W567" s="9">
+        <v>3</v>
+      </c>
+      <c r="X567" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y567" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z567" s="9">
+        <v>5</v>
+      </c>
+      <c r="AA567" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB567" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC567" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD567" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE567" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF567" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG567" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH567" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI567" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ567" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="568" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A568" s="4">
+        <v>45599.562911423607</v>
+      </c>
+      <c r="B568" s="5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C568" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D568" s="5">
+        <v>20223611</v>
+      </c>
+      <c r="E568" s="5" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F568" s="6">
+        <v>0.56041666666715173</v>
+      </c>
+      <c r="G568" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H568" s="5">
+        <v>2</v>
+      </c>
+      <c r="I568" s="5">
+        <v>5</v>
+      </c>
+      <c r="J568" s="5">
+        <v>4</v>
+      </c>
+      <c r="K568" s="5">
+        <v>3</v>
+      </c>
+      <c r="L568" s="5">
+        <v>2</v>
+      </c>
+      <c r="M568" s="5">
+        <v>2</v>
+      </c>
+      <c r="N568" s="5">
+        <v>3</v>
+      </c>
+      <c r="O568" s="5">
+        <v>4</v>
+      </c>
+      <c r="P568" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q568" s="5">
+        <v>3</v>
+      </c>
+      <c r="R568" s="5">
+        <v>5</v>
+      </c>
+      <c r="S568" s="5">
+        <v>4</v>
+      </c>
+      <c r="T568" s="5">
+        <v>3</v>
+      </c>
+      <c r="U568" s="5">
+        <v>3</v>
+      </c>
+      <c r="V568" s="5">
+        <v>4</v>
+      </c>
+      <c r="W568" s="5">
+        <v>6</v>
+      </c>
+      <c r="X568" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y568" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z568" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA568" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB568" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC568" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD568" s="5">
+        <v>5</v>
+      </c>
+      <c r="AE568" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF568" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG568" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH568" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI568" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ568" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="569" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A569" s="8">
+        <v>45599.571777256948</v>
+      </c>
+      <c r="B569" s="9" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C569" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="D569" s="9">
+        <v>20241537</v>
+      </c>
+      <c r="E569" s="9" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F569" s="10">
+        <v>0.57083333333139308</v>
+      </c>
+      <c r="G569" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H569" s="9">
+        <v>2</v>
+      </c>
+      <c r="I569" s="9">
+        <v>4</v>
+      </c>
+      <c r="J569" s="9">
+        <v>5</v>
+      </c>
+      <c r="K569" s="9">
+        <v>5</v>
+      </c>
+      <c r="L569" s="9">
+        <v>5</v>
+      </c>
+      <c r="M569" s="9">
+        <v>3</v>
+      </c>
+      <c r="N569" s="9">
+        <v>5</v>
+      </c>
+      <c r="O569" s="9">
+        <v>5</v>
+      </c>
+      <c r="P569" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q569" s="9">
+        <v>3</v>
+      </c>
+      <c r="R569" s="9">
+        <v>5</v>
+      </c>
+      <c r="S569" s="9">
+        <v>5</v>
+      </c>
+      <c r="T569" s="9">
+        <v>3</v>
+      </c>
+      <c r="U569" s="9">
+        <v>5</v>
+      </c>
+      <c r="V569" s="9">
+        <v>5</v>
+      </c>
+      <c r="W569" s="9">
+        <v>6</v>
+      </c>
+      <c r="X569" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y569" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z569" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA569" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB569" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC569" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD569" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE569" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF569" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG569" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH569" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI569" s="9">
+        <v>5</v>
+      </c>
+      <c r="AJ569" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="570" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A570" s="4">
+        <v>45599.572726909726</v>
+      </c>
+      <c r="B570" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C570" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D570" s="5">
+        <v>20243426</v>
+      </c>
+      <c r="E570" s="5" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F570" s="6">
+        <v>0.57152777777810115</v>
+      </c>
+      <c r="G570" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H570" s="5">
+        <v>3</v>
+      </c>
+      <c r="I570" s="5">
+        <v>3</v>
+      </c>
+      <c r="J570" s="5">
+        <v>3</v>
+      </c>
+      <c r="K570" s="5">
+        <v>3</v>
+      </c>
+      <c r="L570" s="5">
+        <v>3</v>
+      </c>
+      <c r="M570" s="5">
+        <v>3</v>
+      </c>
+      <c r="N570" s="5">
+        <v>3</v>
+      </c>
+      <c r="O570" s="5">
+        <v>3</v>
+      </c>
+      <c r="P570" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q570" s="5">
+        <v>3</v>
+      </c>
+      <c r="R570" s="5">
+        <v>3</v>
+      </c>
+      <c r="S570" s="5">
+        <v>3</v>
+      </c>
+      <c r="T570" s="5">
+        <v>3</v>
+      </c>
+      <c r="U570" s="5">
+        <v>3</v>
+      </c>
+      <c r="V570" s="5">
+        <v>3</v>
+      </c>
+      <c r="W570" s="5">
+        <v>3</v>
+      </c>
+      <c r="X570" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y570" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI570" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ570" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="571" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A571" s="8">
+        <v>45599.578043263886</v>
+      </c>
+      <c r="B571" s="9" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C571" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D571" s="9">
+        <v>20211630</v>
+      </c>
+      <c r="E571" s="9" t="s">
+        <v>1296</v>
+      </c>
+      <c r="F571" s="10">
+        <v>0.57638888889050577</v>
+      </c>
+      <c r="G571" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H571" s="9">
+        <v>3</v>
+      </c>
+      <c r="I571" s="9">
+        <v>4</v>
+      </c>
+      <c r="J571" s="9">
+        <v>4</v>
+      </c>
+      <c r="K571" s="9">
+        <v>2</v>
+      </c>
+      <c r="L571" s="9">
+        <v>2</v>
+      </c>
+      <c r="M571" s="9">
+        <v>2</v>
+      </c>
+      <c r="N571" s="9">
+        <v>4</v>
+      </c>
+      <c r="O571" s="9">
+        <v>4</v>
+      </c>
+      <c r="P571" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q571" s="9">
+        <v>2</v>
+      </c>
+      <c r="R571" s="9">
+        <v>6</v>
+      </c>
+      <c r="S571" s="9">
+        <v>4</v>
+      </c>
+      <c r="T571" s="9">
+        <v>3</v>
+      </c>
+      <c r="U571" s="9">
+        <v>5</v>
+      </c>
+      <c r="V571" s="9">
+        <v>4</v>
+      </c>
+      <c r="W571" s="9">
+        <v>6</v>
+      </c>
+      <c r="X571" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y571" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z571" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA571" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB571" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC571" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD571" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE571" s="9">
+        <v>2</v>
+      </c>
+      <c r="AF571" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG571" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH571" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI571" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ571" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="572" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A572" s="4">
+        <v>45599.578563067131</v>
+      </c>
+      <c r="B572" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C572" s="5" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D572" s="5">
+        <v>20212549</v>
+      </c>
+      <c r="E572" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="F572" s="6">
+        <v>0.57777777777664596</v>
+      </c>
+      <c r="G572" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H572" s="5">
+        <v>4</v>
+      </c>
+      <c r="I572" s="5">
+        <v>4</v>
+      </c>
+      <c r="J572" s="5">
+        <v>4</v>
+      </c>
+      <c r="K572" s="5">
+        <v>4</v>
+      </c>
+      <c r="L572" s="5">
+        <v>4</v>
+      </c>
+      <c r="M572" s="5">
+        <v>4</v>
+      </c>
+      <c r="N572" s="5">
+        <v>4</v>
+      </c>
+      <c r="O572" s="5">
+        <v>4</v>
+      </c>
+      <c r="P572" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q572" s="5">
+        <v>1</v>
+      </c>
+      <c r="R572" s="5">
+        <v>4</v>
+      </c>
+      <c r="S572" s="5">
+        <v>4</v>
+      </c>
+      <c r="T572" s="5">
+        <v>1</v>
+      </c>
+      <c r="U572" s="5">
+        <v>1</v>
+      </c>
+      <c r="V572" s="5">
+        <v>4</v>
+      </c>
+      <c r="W572" s="5">
+        <v>4</v>
+      </c>
+      <c r="X572" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y572" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z572" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA572" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB572" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC572" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD572" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE572" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF572" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG572" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH572" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI572" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ572" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="573" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A573" s="8">
+        <v>45599.579088784725</v>
+      </c>
+      <c r="B573" s="9" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C573" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D573" s="9">
+        <v>20191240</v>
+      </c>
+      <c r="E573" s="9" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F573" s="10">
+        <v>0.57708333333721384</v>
+      </c>
+      <c r="G573" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK573" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL573" s="9">
+        <v>4</v>
+      </c>
+      <c r="AM573" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN573" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO573" s="9">
+        <v>1</v>
+      </c>
+      <c r="AP573" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ573" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR573" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS573" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT573" s="9">
+        <v>4</v>
+      </c>
+      <c r="AU573" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV573" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW573" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX573" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY573" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ573" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA573" s="9">
+        <v>5</v>
+      </c>
+      <c r="BB573" s="9">
+        <v>5</v>
+      </c>
+      <c r="BC573" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD573" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE573" s="9">
+        <v>6</v>
+      </c>
+      <c r="BF573" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG573" s="9">
+        <v>2</v>
+      </c>
+      <c r="BH573" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI573" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ573" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK573" s="9">
+        <v>1</v>
+      </c>
+      <c r="BL573" s="9">
+        <v>1</v>
+      </c>
+      <c r="BM573" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="574" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A574" s="4">
+        <v>45599.583014884258</v>
+      </c>
+      <c r="B574" s="5" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C574" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D574" s="5">
+        <v>20243064</v>
+      </c>
+      <c r="E574" s="5" t="s">
+        <v>1303</v>
+      </c>
+      <c r="F574" s="6">
+        <v>0.58263888888905058</v>
+      </c>
+      <c r="G574" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AT574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AV574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AX574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY574" s="5">
+        <v>4</v>
+      </c>
+      <c r="AZ574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BD574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL574" s="5">
+        <v>4</v>
+      </c>
+      <c r="BM574" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="575" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A575" s="18">
+        <v>45599.585069224537</v>
+      </c>
+      <c r="B575" s="19" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C575" s="19" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D575" s="19">
+        <v>20201002</v>
+      </c>
+      <c r="E575" s="19" t="s">
+        <v>1306</v>
+      </c>
+      <c r="F575" s="20">
+        <v>0.58055555555620231</v>
+      </c>
+      <c r="G575" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H575" s="19">
+        <v>3</v>
+      </c>
+      <c r="I575" s="19">
+        <v>3</v>
+      </c>
+      <c r="J575" s="19">
+        <v>4</v>
+      </c>
+      <c r="K575" s="19">
+        <v>3</v>
+      </c>
+      <c r="L575" s="19">
+        <v>2</v>
+      </c>
+      <c r="M575" s="19">
+        <v>3</v>
+      </c>
+      <c r="N575" s="19">
+        <v>4</v>
+      </c>
+      <c r="O575" s="19">
+        <v>4</v>
+      </c>
+      <c r="P575" s="19">
+        <v>5</v>
+      </c>
+      <c r="Q575" s="19">
+        <v>3</v>
+      </c>
+      <c r="R575" s="19">
+        <v>4</v>
+      </c>
+      <c r="S575" s="19">
+        <v>4</v>
+      </c>
+      <c r="T575" s="19">
+        <v>2</v>
+      </c>
+      <c r="U575" s="19">
+        <v>3</v>
+      </c>
+      <c r="V575" s="19">
+        <v>4</v>
+      </c>
+      <c r="W575" s="19">
+        <v>4</v>
+      </c>
+      <c r="X575" s="19">
+        <v>4</v>
+      </c>
+      <c r="Y575" s="19">
+        <v>4</v>
+      </c>
+      <c r="Z575" s="19">
+        <v>3</v>
+      </c>
+      <c r="AA575" s="19">
+        <v>3</v>
+      </c>
+      <c r="AB575" s="19">
+        <v>4</v>
+      </c>
+      <c r="AC575" s="19">
+        <v>4</v>
+      </c>
+      <c r="AD575" s="19">
+        <v>4</v>
+      </c>
+      <c r="AE575" s="19">
+        <v>4</v>
+      </c>
+      <c r="AF575" s="19">
+        <v>3</v>
+      </c>
+      <c r="AG575" s="19">
+        <v>4</v>
+      </c>
+      <c r="AH575" s="19">
+        <v>2</v>
+      </c>
+      <c r="AI575" s="19">
+        <v>2</v>
+      </c>
+      <c r="AJ575" s="19">
+        <v>4</v>
+      </c>
+      <c r="AK575" s="26"/>
+      <c r="AL575" s="26"/>
+      <c r="AM575" s="26"/>
+      <c r="AN575" s="26"/>
+      <c r="AO575" s="26"/>
+      <c r="AP575" s="26"/>
+      <c r="AQ575" s="26"/>
+      <c r="AR575" s="26"/>
+      <c r="AS575" s="26"/>
+      <c r="AT575" s="26"/>
+      <c r="AU575" s="26"/>
+      <c r="AV575" s="26"/>
+      <c r="AW575" s="26"/>
+      <c r="AX575" s="26"/>
+      <c r="AY575" s="26"/>
+      <c r="AZ575" s="26"/>
+      <c r="BA575" s="26"/>
+      <c r="BB575" s="26"/>
+      <c r="BC575" s="26"/>
+      <c r="BD575" s="26"/>
+      <c r="BE575" s="26"/>
+      <c r="BF575" s="26"/>
+      <c r="BG575" s="26"/>
+      <c r="BH575" s="26"/>
+      <c r="BI575" s="26"/>
+      <c r="BJ575" s="26"/>
+      <c r="BK575" s="26"/>
+      <c r="BL575" s="26"/>
+      <c r="BM575" s="26"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
241021, oxford modified sunday 16:40
</commit_message>
<xml_diff>
--- a/R/data/oxford_241021.xlsx
+++ b/R/data/oxford_241021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Dropbox/내 Mac (Kee-Won의 MacBook Air)/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F419D978-C7D9-FD47-9950-9677129BFC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E74342-7970-A148-8BAE-9B312C77B5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42920" yWindow="1420" windowWidth="37080" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2359" uniqueCount="1307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="1372">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -3944,6 +3944,201 @@
   </si>
   <si>
     <t>강은비</t>
+  </si>
+  <si>
+    <t>pjy35870859@gmail.com</t>
+  </si>
+  <si>
+    <t>박지연</t>
+  </si>
+  <si>
+    <t>cmin0945@gmail.com</t>
+  </si>
+  <si>
+    <t>조상민</t>
+  </si>
+  <si>
+    <t>whdudgus1013@gmail.com</t>
+  </si>
+  <si>
+    <t>조영현</t>
+  </si>
+  <si>
+    <t>bluelion-gbn9981@naver.com</t>
+  </si>
+  <si>
+    <t>구보늬</t>
+  </si>
+  <si>
+    <t>wnsgud9624@naver.com</t>
+  </si>
+  <si>
+    <t>임준형</t>
+  </si>
+  <si>
+    <t>psw9879@naver.com</t>
+  </si>
+  <si>
+    <t>박상원</t>
+  </si>
+  <si>
+    <t>nyo07@naver.com</t>
+  </si>
+  <si>
+    <t>윤효라</t>
+  </si>
+  <si>
+    <t>77sunhwa@gmail.com</t>
+  </si>
+  <si>
+    <t>박선화</t>
+  </si>
+  <si>
+    <t>minchan6020@gmail.com</t>
+  </si>
+  <si>
+    <t>jin050828@gmail.com</t>
+  </si>
+  <si>
+    <t>김진영</t>
+  </si>
+  <si>
+    <t>zjxps2007@gmail.com</t>
+  </si>
+  <si>
+    <t>콘텐츠 it</t>
+  </si>
+  <si>
+    <t>조인호</t>
+  </si>
+  <si>
+    <t>solar08230@naver.com</t>
+  </si>
+  <si>
+    <t>안다빈</t>
+  </si>
+  <si>
+    <t>duke102426@gmail.com</t>
+  </si>
+  <si>
+    <t>문진혁</t>
+  </si>
+  <si>
+    <t>andy9925@naver.com</t>
+  </si>
+  <si>
+    <t>김무극</t>
+  </si>
+  <si>
+    <t>happyfish123@naver.com</t>
+  </si>
+  <si>
+    <t>dustinwon2005@gmail.com</t>
+  </si>
+  <si>
+    <t>원지현</t>
+  </si>
+  <si>
+    <t>leehanseo0521@naver.com</t>
+  </si>
+  <si>
+    <t>이한서</t>
+  </si>
+  <si>
+    <t>h20231025@glab.hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>dltmdwo0301@naver.com</t>
+  </si>
+  <si>
+    <t>이승재</t>
+  </si>
+  <si>
+    <t>choikang2010@naver.com</t>
+  </si>
+  <si>
+    <t>최연희</t>
+  </si>
+  <si>
+    <t>minsung5342@naver.com</t>
+  </si>
+  <si>
+    <t>ksj101710@naver.com</t>
+  </si>
+  <si>
+    <t>김경록</t>
+  </si>
+  <si>
+    <t>dydwndus1115@naver.com</t>
+  </si>
+  <si>
+    <t>용주연</t>
+  </si>
+  <si>
+    <t>ahs042400@naver.com</t>
+  </si>
+  <si>
+    <t>안현성</t>
+  </si>
+  <si>
+    <t>rkdwndms112@naver.com</t>
+  </si>
+  <si>
+    <t>강주은</t>
+  </si>
+  <si>
+    <t>akeb110@naver.com</t>
+  </si>
+  <si>
+    <t>김은빈</t>
+  </si>
+  <si>
+    <t>jina20050429@gmail.com</t>
+  </si>
+  <si>
+    <t>이진아</t>
+  </si>
+  <si>
+    <t>seungye04@naver.com</t>
+  </si>
+  <si>
+    <t>정승예</t>
+  </si>
+  <si>
+    <t>jb9517asd@naver.com</t>
+  </si>
+  <si>
+    <t>곽우주</t>
+  </si>
+  <si>
+    <t>vcx76613@gmail.com</t>
+  </si>
+  <si>
+    <t>황인태</t>
+  </si>
+  <si>
+    <t>ydy7495@naver.com</t>
+  </si>
+  <si>
+    <t>윤다연</t>
+  </si>
+  <si>
+    <t>joon020978@gmail.com</t>
+  </si>
+  <si>
+    <t>이준</t>
+  </si>
+  <si>
+    <t>jangsinhyeog6@gmail.cm</t>
+  </si>
+  <si>
+    <t>장신혁</t>
+  </si>
+  <si>
+    <t>oj5803@naver.com</t>
+  </si>
+  <si>
+    <t>이영주</t>
   </si>
 </sst>
 </file>
@@ -4387,7 +4582,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM575">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM609">
   <tableColumns count="65">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -4660,11 +4855,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM575"/>
+  <dimension ref="A1:BM609"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A538" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C580" sqref="C580"/>
+      <pane ySplit="1" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C614" sqref="C614"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -68905,35 +69100,3775 @@
       <c r="AJ575" s="19">
         <v>4</v>
       </c>
-      <c r="AK575" s="26"/>
-      <c r="AL575" s="26"/>
-      <c r="AM575" s="26"/>
-      <c r="AN575" s="26"/>
-      <c r="AO575" s="26"/>
-      <c r="AP575" s="26"/>
-      <c r="AQ575" s="26"/>
-      <c r="AR575" s="26"/>
-      <c r="AS575" s="26"/>
-      <c r="AT575" s="26"/>
-      <c r="AU575" s="26"/>
-      <c r="AV575" s="26"/>
-      <c r="AW575" s="26"/>
-      <c r="AX575" s="26"/>
-      <c r="AY575" s="26"/>
-      <c r="AZ575" s="26"/>
-      <c r="BA575" s="26"/>
-      <c r="BB575" s="26"/>
-      <c r="BC575" s="26"/>
-      <c r="BD575" s="26"/>
-      <c r="BE575" s="26"/>
-      <c r="BF575" s="26"/>
-      <c r="BG575" s="26"/>
-      <c r="BH575" s="26"/>
-      <c r="BI575" s="26"/>
-      <c r="BJ575" s="26"/>
-      <c r="BK575" s="26"/>
-      <c r="BL575" s="26"/>
-      <c r="BM575" s="26"/>
+    </row>
+    <row r="576" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A576" s="4">
+        <v>45599.592273599541</v>
+      </c>
+      <c r="B576" s="5" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C576" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D576" s="5">
+        <v>20242618</v>
+      </c>
+      <c r="E576" s="5" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F576" s="6">
+        <v>0.59027777778101154</v>
+      </c>
+      <c r="G576" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H576" s="5">
+        <v>2</v>
+      </c>
+      <c r="I576" s="5">
+        <v>4</v>
+      </c>
+      <c r="J576" s="5">
+        <v>4</v>
+      </c>
+      <c r="K576" s="5">
+        <v>3</v>
+      </c>
+      <c r="L576" s="5">
+        <v>2</v>
+      </c>
+      <c r="M576" s="5">
+        <v>4</v>
+      </c>
+      <c r="N576" s="5">
+        <v>3</v>
+      </c>
+      <c r="O576" s="5">
+        <v>3</v>
+      </c>
+      <c r="P576" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q576" s="5">
+        <v>2</v>
+      </c>
+      <c r="R576" s="5">
+        <v>5</v>
+      </c>
+      <c r="S576" s="5">
+        <v>4</v>
+      </c>
+      <c r="T576" s="5">
+        <v>2</v>
+      </c>
+      <c r="U576" s="5">
+        <v>3</v>
+      </c>
+      <c r="V576" s="5">
+        <v>4</v>
+      </c>
+      <c r="W576" s="5">
+        <v>2</v>
+      </c>
+      <c r="X576" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y576" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z576" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA576" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB576" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC576" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD576" s="5">
+        <v>6</v>
+      </c>
+      <c r="AE576" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF576" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG576" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH576" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI576" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ576" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="577" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A577" s="8">
+        <v>45599.597542222225</v>
+      </c>
+      <c r="B577" s="9" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C577" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D577" s="9">
+        <v>20246776</v>
+      </c>
+      <c r="E577" s="9" t="s">
+        <v>1310</v>
+      </c>
+      <c r="F577" s="10">
+        <v>9.5833333332848269E-2</v>
+      </c>
+      <c r="G577" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H577" s="9">
+        <v>3</v>
+      </c>
+      <c r="I577" s="9">
+        <v>2</v>
+      </c>
+      <c r="J577" s="9">
+        <v>2</v>
+      </c>
+      <c r="K577" s="9">
+        <v>3</v>
+      </c>
+      <c r="L577" s="9">
+        <v>4</v>
+      </c>
+      <c r="M577" s="9">
+        <v>4</v>
+      </c>
+      <c r="N577" s="9">
+        <v>3</v>
+      </c>
+      <c r="O577" s="9">
+        <v>2</v>
+      </c>
+      <c r="P577" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q577" s="9">
+        <v>3</v>
+      </c>
+      <c r="R577" s="9">
+        <v>3</v>
+      </c>
+      <c r="S577" s="9">
+        <v>2</v>
+      </c>
+      <c r="T577" s="9">
+        <v>3</v>
+      </c>
+      <c r="U577" s="9">
+        <v>4</v>
+      </c>
+      <c r="V577" s="9">
+        <v>3</v>
+      </c>
+      <c r="W577" s="9">
+        <v>1</v>
+      </c>
+      <c r="X577" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y577" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z577" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA577" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB577" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC577" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD577" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE577" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF577" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG577" s="9">
+        <v>2</v>
+      </c>
+      <c r="AH577" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI577" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ577" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="578" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A578" s="4">
+        <v>45599.599140763894</v>
+      </c>
+      <c r="B578" s="5" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C578" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D578" s="5">
+        <v>20243253</v>
+      </c>
+      <c r="E578" s="5" t="s">
+        <v>1312</v>
+      </c>
+      <c r="F578" s="6">
+        <v>0.59652777777955635</v>
+      </c>
+      <c r="G578" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H578" s="5">
+        <v>5</v>
+      </c>
+      <c r="I578" s="5">
+        <v>3</v>
+      </c>
+      <c r="J578" s="5">
+        <v>4</v>
+      </c>
+      <c r="K578" s="5">
+        <v>2</v>
+      </c>
+      <c r="L578" s="5">
+        <v>2</v>
+      </c>
+      <c r="M578" s="5">
+        <v>4</v>
+      </c>
+      <c r="N578" s="5">
+        <v>2</v>
+      </c>
+      <c r="O578" s="5">
+        <v>3</v>
+      </c>
+      <c r="P578" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q578" s="5">
+        <v>5</v>
+      </c>
+      <c r="R578" s="5">
+        <v>3</v>
+      </c>
+      <c r="S578" s="5">
+        <v>3</v>
+      </c>
+      <c r="T578" s="5">
+        <v>3</v>
+      </c>
+      <c r="U578" s="5">
+        <v>4</v>
+      </c>
+      <c r="V578" s="5">
+        <v>3</v>
+      </c>
+      <c r="W578" s="5">
+        <v>2</v>
+      </c>
+      <c r="X578" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y578" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z578" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA578" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB578" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC578" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD578" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE578" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF578" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG578" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH578" s="5">
+        <v>4</v>
+      </c>
+      <c r="AI578" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ578" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="579" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A579" s="8">
+        <v>45599.599642638888</v>
+      </c>
+      <c r="B579" s="9" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C579" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D579" s="9">
+        <v>20243403</v>
+      </c>
+      <c r="E579" s="9" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F579" s="10">
+        <v>0.46041666666860692</v>
+      </c>
+      <c r="G579" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK579" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL579" s="9">
+        <v>4</v>
+      </c>
+      <c r="AM579" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN579" s="9">
+        <v>2</v>
+      </c>
+      <c r="AO579" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP579" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ579" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR579" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS579" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT579" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU579" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV579" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW579" s="9">
+        <v>4</v>
+      </c>
+      <c r="AX579" s="9">
+        <v>5</v>
+      </c>
+      <c r="AY579" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ579" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA579" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB579" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC579" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD579" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE579" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF579" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG579" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH579" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI579" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ579" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK579" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL579" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM579" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="580" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A580" s="4">
+        <v>45599.600650740744</v>
+      </c>
+      <c r="B580" s="5" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C580" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D580" s="5">
+        <v>20181090</v>
+      </c>
+      <c r="E580" s="5" t="s">
+        <v>1316</v>
+      </c>
+      <c r="F580" s="6">
+        <v>0.59791666666569654</v>
+      </c>
+      <c r="G580" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H580" s="5">
+        <v>2</v>
+      </c>
+      <c r="I580" s="5">
+        <v>5</v>
+      </c>
+      <c r="J580" s="5">
+        <v>5</v>
+      </c>
+      <c r="K580" s="5">
+        <v>5</v>
+      </c>
+      <c r="L580" s="5">
+        <v>4</v>
+      </c>
+      <c r="M580" s="5">
+        <v>2</v>
+      </c>
+      <c r="N580" s="5">
+        <v>5</v>
+      </c>
+      <c r="O580" s="5">
+        <v>6</v>
+      </c>
+      <c r="P580" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q580" s="5">
+        <v>3</v>
+      </c>
+      <c r="R580" s="5">
+        <v>5</v>
+      </c>
+      <c r="S580" s="5">
+        <v>4</v>
+      </c>
+      <c r="T580" s="5">
+        <v>2</v>
+      </c>
+      <c r="U580" s="5">
+        <v>5</v>
+      </c>
+      <c r="V580" s="5">
+        <v>5</v>
+      </c>
+      <c r="W580" s="5">
+        <v>4</v>
+      </c>
+      <c r="X580" s="5">
+        <v>6</v>
+      </c>
+      <c r="Y580" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z580" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA580" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB580" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC580" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD580" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE580" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF580" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG580" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH580" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI580" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ580" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="581" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A581" s="8">
+        <v>45599.601514780094</v>
+      </c>
+      <c r="B581" s="9" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C581" s="9" t="s">
+        <v>692</v>
+      </c>
+      <c r="D581" s="9">
+        <v>20235164</v>
+      </c>
+      <c r="E581" s="9" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F581" s="10">
+        <v>0.58958333333430346</v>
+      </c>
+      <c r="G581" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK581" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL581" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM581" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN581" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO581" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP581" s="9">
+        <v>2</v>
+      </c>
+      <c r="AQ581" s="9">
+        <v>4</v>
+      </c>
+      <c r="AR581" s="9">
+        <v>5</v>
+      </c>
+      <c r="AS581" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT581" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU581" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV581" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW581" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX581" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY581" s="9">
+        <v>5</v>
+      </c>
+      <c r="AZ581" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA581" s="9">
+        <v>5</v>
+      </c>
+      <c r="BB581" s="9">
+        <v>5</v>
+      </c>
+      <c r="BC581" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD581" s="9">
+        <v>5</v>
+      </c>
+      <c r="BE581" s="9">
+        <v>5</v>
+      </c>
+      <c r="BF581" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG581" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH581" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI581" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ581" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK581" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL581" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM581" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="582" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A582" s="4">
+        <v>45599.602577268517</v>
+      </c>
+      <c r="B582" s="5" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C582" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D582" s="5">
+        <v>20217087</v>
+      </c>
+      <c r="E582" s="5" t="s">
+        <v>1320</v>
+      </c>
+      <c r="F582" s="6">
+        <v>0.59861111111240461</v>
+      </c>
+      <c r="G582" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H582" s="5">
+        <v>2</v>
+      </c>
+      <c r="I582" s="5">
+        <v>1</v>
+      </c>
+      <c r="J582" s="5">
+        <v>3</v>
+      </c>
+      <c r="K582" s="5">
+        <v>1</v>
+      </c>
+      <c r="L582" s="5">
+        <v>5</v>
+      </c>
+      <c r="M582" s="5">
+        <v>2</v>
+      </c>
+      <c r="N582" s="5">
+        <v>5</v>
+      </c>
+      <c r="O582" s="5">
+        <v>2</v>
+      </c>
+      <c r="P582" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q582" s="5">
+        <v>2</v>
+      </c>
+      <c r="R582" s="5">
+        <v>5</v>
+      </c>
+      <c r="S582" s="5">
+        <v>1</v>
+      </c>
+      <c r="T582" s="5">
+        <v>2</v>
+      </c>
+      <c r="U582" s="5">
+        <v>2</v>
+      </c>
+      <c r="V582" s="5">
+        <v>1</v>
+      </c>
+      <c r="W582" s="5">
+        <v>3</v>
+      </c>
+      <c r="X582" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y582" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z582" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA582" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB582" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC582" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD582" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE582" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF582" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG582" s="5">
+        <v>2</v>
+      </c>
+      <c r="AH582" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI582" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ582" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="583" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A583" s="8">
+        <v>45599.60531219907</v>
+      </c>
+      <c r="B583" s="9" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C583" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D583" s="9">
+        <v>20242956</v>
+      </c>
+      <c r="E583" s="9" t="s">
+        <v>1322</v>
+      </c>
+      <c r="F583" s="10">
+        <v>0.60347222222480923</v>
+      </c>
+      <c r="G583" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H583" s="9">
+        <v>2</v>
+      </c>
+      <c r="I583" s="9">
+        <v>4</v>
+      </c>
+      <c r="J583" s="9">
+        <v>5</v>
+      </c>
+      <c r="K583" s="9">
+        <v>4</v>
+      </c>
+      <c r="L583" s="9">
+        <v>1</v>
+      </c>
+      <c r="M583" s="9">
+        <v>2</v>
+      </c>
+      <c r="N583" s="9">
+        <v>5</v>
+      </c>
+      <c r="O583" s="9">
+        <v>3</v>
+      </c>
+      <c r="P583" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q583" s="9">
+        <v>2</v>
+      </c>
+      <c r="R583" s="9">
+        <v>5</v>
+      </c>
+      <c r="S583" s="9">
+        <v>5</v>
+      </c>
+      <c r="T583" s="9">
+        <v>2</v>
+      </c>
+      <c r="U583" s="9">
+        <v>2</v>
+      </c>
+      <c r="V583" s="9">
+        <v>5</v>
+      </c>
+      <c r="W583" s="9">
+        <v>5</v>
+      </c>
+      <c r="X583" s="9">
+        <v>6</v>
+      </c>
+      <c r="Y583" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z583" s="9">
+        <v>5</v>
+      </c>
+      <c r="AA583" s="9">
+        <v>2</v>
+      </c>
+      <c r="AB583" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC583" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD583" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE583" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF583" s="9">
+        <v>6</v>
+      </c>
+      <c r="AG583" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH583" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI583" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ583" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="584" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A584" s="4">
+        <v>45599.61166480324</v>
+      </c>
+      <c r="B584" s="5" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C584" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D584" s="5">
+        <v>20242508</v>
+      </c>
+      <c r="E584" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="F584" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="G584" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AM584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AO584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AP584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AQ584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AR584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AS584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AT584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AV584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AW584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AY584" s="5">
+        <v>1</v>
+      </c>
+      <c r="AZ584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BA584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BB584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BC584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BD584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BE584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BF584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BG584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BH584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BJ584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BK584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL584" s="5">
+        <v>1</v>
+      </c>
+      <c r="BM584" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="585" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A585" s="8">
+        <v>45599.615580416663</v>
+      </c>
+      <c r="B585" s="9" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C585" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D585" s="9">
+        <v>20246715</v>
+      </c>
+      <c r="E585" s="9" t="s">
+        <v>1325</v>
+      </c>
+      <c r="F585" s="10">
+        <v>0.63541666666424135</v>
+      </c>
+      <c r="G585" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK585" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL585" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM585" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN585" s="9">
+        <v>2</v>
+      </c>
+      <c r="AO585" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP585" s="9">
+        <v>2</v>
+      </c>
+      <c r="AQ585" s="9">
+        <v>5</v>
+      </c>
+      <c r="AR585" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS585" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT585" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU585" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV585" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW585" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX585" s="9">
+        <v>6</v>
+      </c>
+      <c r="AY585" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ585" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA585" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB585" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC585" s="9">
+        <v>5</v>
+      </c>
+      <c r="BD585" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE585" s="9">
+        <v>2</v>
+      </c>
+      <c r="BF585" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG585" s="9">
+        <v>4</v>
+      </c>
+      <c r="BH585" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI585" s="9">
+        <v>2</v>
+      </c>
+      <c r="BJ585" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK585" s="9">
+        <v>4</v>
+      </c>
+      <c r="BL585" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM585" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="586" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A586" s="4">
+        <v>45599.624398148153</v>
+      </c>
+      <c r="B586" s="5" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C586" s="5" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D586" s="5">
+        <v>20195258</v>
+      </c>
+      <c r="E586" s="5" t="s">
+        <v>1328</v>
+      </c>
+      <c r="F586" s="6">
+        <v>0.62152777778101154</v>
+      </c>
+      <c r="G586" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK586" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL586" s="5">
+        <v>1</v>
+      </c>
+      <c r="AM586" s="5">
+        <v>6</v>
+      </c>
+      <c r="AN586" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO586" s="5">
+        <v>6</v>
+      </c>
+      <c r="AP586" s="5">
+        <v>1</v>
+      </c>
+      <c r="AQ586" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR586" s="5">
+        <v>5</v>
+      </c>
+      <c r="AS586" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT586" s="5">
+        <v>6</v>
+      </c>
+      <c r="AU586" s="5">
+        <v>3</v>
+      </c>
+      <c r="AV586" s="5">
+        <v>6</v>
+      </c>
+      <c r="AW586" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX586" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY586" s="5">
+        <v>6</v>
+      </c>
+      <c r="AZ586" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA586" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB586" s="5">
+        <v>6</v>
+      </c>
+      <c r="BC586" s="5">
+        <v>1</v>
+      </c>
+      <c r="BD586" s="5">
+        <v>6</v>
+      </c>
+      <c r="BE586" s="5">
+        <v>6</v>
+      </c>
+      <c r="BF586" s="5">
+        <v>6</v>
+      </c>
+      <c r="BG586" s="5">
+        <v>6</v>
+      </c>
+      <c r="BH586" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI586" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ586" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK586" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL586" s="5">
+        <v>1</v>
+      </c>
+      <c r="BM586" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="587" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A587" s="8">
+        <v>45599.626215578704</v>
+      </c>
+      <c r="B587" s="9" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C587" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="D587" s="9">
+        <v>20221717</v>
+      </c>
+      <c r="E587" s="9" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F587" s="10">
+        <v>0.96597222222044365</v>
+      </c>
+      <c r="G587" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H587" s="9">
+        <v>2</v>
+      </c>
+      <c r="I587" s="9">
+        <v>4</v>
+      </c>
+      <c r="J587" s="9">
+        <v>4</v>
+      </c>
+      <c r="K587" s="9">
+        <v>3</v>
+      </c>
+      <c r="L587" s="9">
+        <v>3</v>
+      </c>
+      <c r="M587" s="9">
+        <v>4</v>
+      </c>
+      <c r="N587" s="9">
+        <v>5</v>
+      </c>
+      <c r="O587" s="9">
+        <v>4</v>
+      </c>
+      <c r="P587" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q587" s="9">
+        <v>4</v>
+      </c>
+      <c r="R587" s="9">
+        <v>5</v>
+      </c>
+      <c r="S587" s="9">
+        <v>5</v>
+      </c>
+      <c r="T587" s="9">
+        <v>3</v>
+      </c>
+      <c r="U587" s="9">
+        <v>2</v>
+      </c>
+      <c r="V587" s="9">
+        <v>5</v>
+      </c>
+      <c r="W587" s="9">
+        <v>4</v>
+      </c>
+      <c r="X587" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y587" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z587" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA587" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB587" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC587" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD587" s="9">
+        <v>2</v>
+      </c>
+      <c r="AE587" s="9">
+        <v>2</v>
+      </c>
+      <c r="AF587" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG587" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH587" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI587" s="9">
+        <v>4</v>
+      </c>
+      <c r="AJ587" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="588" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A588" s="4">
+        <v>45599.630768807867</v>
+      </c>
+      <c r="B588" s="5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C588" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D588" s="5">
+        <v>20182862</v>
+      </c>
+      <c r="E588" s="5" t="s">
+        <v>1332</v>
+      </c>
+      <c r="F588" s="6">
+        <v>0.62986111111240461</v>
+      </c>
+      <c r="G588" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK588" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL588" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM588" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN588" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO588" s="5">
+        <v>3</v>
+      </c>
+      <c r="AP588" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ588" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR588" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS588" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT588" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU588" s="5">
+        <v>3</v>
+      </c>
+      <c r="AV588" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW588" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX588" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY588" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ588" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA588" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB588" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC588" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD588" s="5">
+        <v>3</v>
+      </c>
+      <c r="BE588" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF588" s="5">
+        <v>2</v>
+      </c>
+      <c r="BG588" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH588" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI588" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ588" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK588" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL588" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM588" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="589" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A589" s="8">
+        <v>45599.631750555556</v>
+      </c>
+      <c r="B589" s="9" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C589" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D589" s="9">
+        <v>20234110</v>
+      </c>
+      <c r="E589" s="9" t="s">
+        <v>1334</v>
+      </c>
+      <c r="F589" s="10">
+        <v>0.62986111111240461</v>
+      </c>
+      <c r="G589" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H589" s="9">
+        <v>1</v>
+      </c>
+      <c r="I589" s="9">
+        <v>4</v>
+      </c>
+      <c r="J589" s="9">
+        <v>4</v>
+      </c>
+      <c r="K589" s="9">
+        <v>5</v>
+      </c>
+      <c r="L589" s="9">
+        <v>2</v>
+      </c>
+      <c r="M589" s="9">
+        <v>1</v>
+      </c>
+      <c r="N589" s="9">
+        <v>4</v>
+      </c>
+      <c r="O589" s="9">
+        <v>5</v>
+      </c>
+      <c r="P589" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q589" s="9">
+        <v>1</v>
+      </c>
+      <c r="R589" s="9">
+        <v>4</v>
+      </c>
+      <c r="S589" s="9">
+        <v>5</v>
+      </c>
+      <c r="T589" s="9">
+        <v>2</v>
+      </c>
+      <c r="U589" s="9">
+        <v>1</v>
+      </c>
+      <c r="V589" s="9">
+        <v>6</v>
+      </c>
+      <c r="W589" s="9">
+        <v>5</v>
+      </c>
+      <c r="X589" s="9">
+        <v>6</v>
+      </c>
+      <c r="Y589" s="9">
+        <v>6</v>
+      </c>
+      <c r="Z589" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA589" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB589" s="9">
+        <v>6</v>
+      </c>
+      <c r="AC589" s="9">
+        <v>6</v>
+      </c>
+      <c r="AD589" s="9">
+        <v>2</v>
+      </c>
+      <c r="AE589" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF589" s="9">
+        <v>6</v>
+      </c>
+      <c r="AG589" s="9">
+        <v>6</v>
+      </c>
+      <c r="AH589" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI589" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ589" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="590" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A590" s="4">
+        <v>45599.631849224534</v>
+      </c>
+      <c r="B590" s="5" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C590" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D590" s="5">
+        <v>20242919</v>
+      </c>
+      <c r="E590" s="5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F590" s="6">
+        <v>0.62986111111240461</v>
+      </c>
+      <c r="G590" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H590" s="5">
+        <v>2</v>
+      </c>
+      <c r="I590" s="5">
+        <v>3</v>
+      </c>
+      <c r="J590" s="5">
+        <v>3</v>
+      </c>
+      <c r="K590" s="5">
+        <v>3</v>
+      </c>
+      <c r="L590" s="5">
+        <v>1</v>
+      </c>
+      <c r="M590" s="5">
+        <v>2</v>
+      </c>
+      <c r="N590" s="5">
+        <v>2</v>
+      </c>
+      <c r="O590" s="5">
+        <v>3</v>
+      </c>
+      <c r="P590" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q590" s="5">
+        <v>3</v>
+      </c>
+      <c r="R590" s="5">
+        <v>3</v>
+      </c>
+      <c r="S590" s="5">
+        <v>3</v>
+      </c>
+      <c r="T590" s="5">
+        <v>3</v>
+      </c>
+      <c r="U590" s="5">
+        <v>1</v>
+      </c>
+      <c r="V590" s="5">
+        <v>3</v>
+      </c>
+      <c r="W590" s="5">
+        <v>3</v>
+      </c>
+      <c r="X590" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y590" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z590" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA590" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB590" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC590" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD590" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE590" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF590" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG590" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH590" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI590" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ590" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="591" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A591" s="8">
+        <v>45599.631905821763</v>
+      </c>
+      <c r="B591" s="9" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C591" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D591" s="9">
+        <v>20246747</v>
+      </c>
+      <c r="E591" s="9" t="s">
+        <v>1337</v>
+      </c>
+      <c r="F591" s="10">
+        <v>0.63055555555911269</v>
+      </c>
+      <c r="G591" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK591" s="9">
+        <v>5</v>
+      </c>
+      <c r="AL591" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM591" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN591" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO591" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP591" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ591" s="9">
+        <v>5</v>
+      </c>
+      <c r="AR591" s="9">
+        <v>5</v>
+      </c>
+      <c r="AS591" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT591" s="9">
+        <v>5</v>
+      </c>
+      <c r="AU591" s="9">
+        <v>6</v>
+      </c>
+      <c r="AV591" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW591" s="9">
+        <v>4</v>
+      </c>
+      <c r="AX591" s="9">
+        <v>5</v>
+      </c>
+      <c r="AY591" s="9">
+        <v>5</v>
+      </c>
+      <c r="AZ591" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA591" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB591" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC591" s="9">
+        <v>5</v>
+      </c>
+      <c r="BD591" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE591" s="9">
+        <v>5</v>
+      </c>
+      <c r="BF591" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG591" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH591" s="9">
+        <v>4</v>
+      </c>
+      <c r="BI591" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ591" s="9">
+        <v>5</v>
+      </c>
+      <c r="BK591" s="9">
+        <v>4</v>
+      </c>
+      <c r="BL591" s="9">
+        <v>5</v>
+      </c>
+      <c r="BM591" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="592" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A592" s="4">
+        <v>45599.632177210646</v>
+      </c>
+      <c r="B592" s="5" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C592" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D592" s="5">
+        <v>20236283</v>
+      </c>
+      <c r="E592" s="5" t="s">
+        <v>1339</v>
+      </c>
+      <c r="F592" s="6">
+        <v>0.62638888889341615</v>
+      </c>
+      <c r="G592" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK592" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL592" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM592" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN592" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO592" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP592" s="5">
+        <v>1</v>
+      </c>
+      <c r="AQ592" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR592" s="5">
+        <v>5</v>
+      </c>
+      <c r="AS592" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT592" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU592" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV592" s="5">
+        <v>6</v>
+      </c>
+      <c r="AW592" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX592" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY592" s="5">
+        <v>6</v>
+      </c>
+      <c r="AZ592" s="5">
+        <v>5</v>
+      </c>
+      <c r="BA592" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB592" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC592" s="5">
+        <v>1</v>
+      </c>
+      <c r="BD592" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE592" s="5">
+        <v>6</v>
+      </c>
+      <c r="BF592" s="5">
+        <v>6</v>
+      </c>
+      <c r="BG592" s="5">
+        <v>6</v>
+      </c>
+      <c r="BH592" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI592" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ592" s="5">
+        <v>6</v>
+      </c>
+      <c r="BK592" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL592" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM592" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="593" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A593" s="8">
+        <v>45599.635710532406</v>
+      </c>
+      <c r="B593" s="9" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C593" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D593" s="9">
+        <v>20231025</v>
+      </c>
+      <c r="E593" s="9" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F593" s="10">
+        <v>0.632638888884685</v>
+      </c>
+      <c r="G593" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK593" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL593" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM593" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN593" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO593" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP593" s="9">
+        <v>2</v>
+      </c>
+      <c r="AQ593" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR593" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS593" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT593" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU593" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV593" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW593" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX593" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY593" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ593" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA593" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB593" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC593" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD593" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE593" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF593" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG593" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH593" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI593" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ593" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK593" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL593" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM593" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="594" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A594" s="4">
+        <v>45599.646001851856</v>
+      </c>
+      <c r="B594" s="5" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C594" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D594" s="5">
+        <v>20222830</v>
+      </c>
+      <c r="E594" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F594" s="6">
+        <v>0.38194444444525288</v>
+      </c>
+      <c r="G594" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H594" s="5">
+        <v>2</v>
+      </c>
+      <c r="I594" s="5">
+        <v>3</v>
+      </c>
+      <c r="J594" s="5">
+        <v>2</v>
+      </c>
+      <c r="K594" s="5">
+        <v>3</v>
+      </c>
+      <c r="L594" s="5">
+        <v>2</v>
+      </c>
+      <c r="M594" s="5">
+        <v>3</v>
+      </c>
+      <c r="N594" s="5">
+        <v>2</v>
+      </c>
+      <c r="O594" s="5">
+        <v>3</v>
+      </c>
+      <c r="P594" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q594" s="5">
+        <v>3</v>
+      </c>
+      <c r="R594" s="5">
+        <v>2</v>
+      </c>
+      <c r="S594" s="5">
+        <v>3</v>
+      </c>
+      <c r="T594" s="5">
+        <v>2</v>
+      </c>
+      <c r="U594" s="5">
+        <v>3</v>
+      </c>
+      <c r="V594" s="5">
+        <v>2</v>
+      </c>
+      <c r="W594" s="5">
+        <v>3</v>
+      </c>
+      <c r="X594" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y594" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z594" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA594" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB594" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC594" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD594" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE594" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF594" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG594" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH594" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI594" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ594" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="595" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A595" s="8">
+        <v>45599.647112523147</v>
+      </c>
+      <c r="B595" s="9" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C595" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D595" s="9">
+        <v>20222238</v>
+      </c>
+      <c r="E595" s="9" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F595" s="10">
+        <v>0.64583333333575865</v>
+      </c>
+      <c r="G595" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H595" s="9">
+        <v>4</v>
+      </c>
+      <c r="I595" s="9">
+        <v>4</v>
+      </c>
+      <c r="J595" s="9">
+        <v>4</v>
+      </c>
+      <c r="K595" s="9">
+        <v>4</v>
+      </c>
+      <c r="L595" s="9">
+        <v>4</v>
+      </c>
+      <c r="M595" s="9">
+        <v>4</v>
+      </c>
+      <c r="N595" s="9">
+        <v>4</v>
+      </c>
+      <c r="O595" s="9">
+        <v>4</v>
+      </c>
+      <c r="P595" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q595" s="9">
+        <v>4</v>
+      </c>
+      <c r="R595" s="9">
+        <v>3</v>
+      </c>
+      <c r="S595" s="9">
+        <v>2</v>
+      </c>
+      <c r="T595" s="9">
+        <v>5</v>
+      </c>
+      <c r="U595" s="9">
+        <v>4</v>
+      </c>
+      <c r="V595" s="9">
+        <v>4</v>
+      </c>
+      <c r="W595" s="9">
+        <v>3</v>
+      </c>
+      <c r="X595" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y595" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z595" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA595" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB595" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC595" s="9">
+        <v>2</v>
+      </c>
+      <c r="AD595" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE595" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF595" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG595" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH595" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI595" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ595" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="596" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A596" s="4">
+        <v>45599.651298136574</v>
+      </c>
+      <c r="B596" s="5" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C596" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D596" s="5">
+        <v>20232311</v>
+      </c>
+      <c r="E596" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="F596" s="6">
+        <v>0.648611111115315</v>
+      </c>
+      <c r="G596" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H596" s="5">
+        <v>1</v>
+      </c>
+      <c r="I596" s="5">
+        <v>5</v>
+      </c>
+      <c r="J596" s="5">
+        <v>4</v>
+      </c>
+      <c r="K596" s="5">
+        <v>4</v>
+      </c>
+      <c r="L596" s="5">
+        <v>1</v>
+      </c>
+      <c r="M596" s="5">
+        <v>1</v>
+      </c>
+      <c r="N596" s="5">
+        <v>6</v>
+      </c>
+      <c r="O596" s="5">
+        <v>5</v>
+      </c>
+      <c r="P596" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q596" s="5">
+        <v>1</v>
+      </c>
+      <c r="R596" s="5">
+        <v>6</v>
+      </c>
+      <c r="S596" s="5">
+        <v>6</v>
+      </c>
+      <c r="T596" s="5">
+        <v>1</v>
+      </c>
+      <c r="U596" s="5">
+        <v>3</v>
+      </c>
+      <c r="V596" s="5">
+        <v>6</v>
+      </c>
+      <c r="W596" s="5">
+        <v>6</v>
+      </c>
+      <c r="X596" s="5">
+        <v>6</v>
+      </c>
+      <c r="Y596" s="5">
+        <v>6</v>
+      </c>
+      <c r="Z596" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA596" s="5">
+        <v>6</v>
+      </c>
+      <c r="AB596" s="5">
+        <v>6</v>
+      </c>
+      <c r="AC596" s="5">
+        <v>6</v>
+      </c>
+      <c r="AD596" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE596" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF596" s="5">
+        <v>6</v>
+      </c>
+      <c r="AG596" s="5">
+        <v>6</v>
+      </c>
+      <c r="AH596" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI596" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ596" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="597" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A597" s="8">
+        <v>45599.651325497689</v>
+      </c>
+      <c r="B597" s="9" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C597" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D597" s="9">
+        <v>20245117</v>
+      </c>
+      <c r="E597" s="9" t="s">
+        <v>1347</v>
+      </c>
+      <c r="F597" s="10">
+        <v>0.148611111115315</v>
+      </c>
+      <c r="G597" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H597" s="9">
+        <v>1</v>
+      </c>
+      <c r="I597" s="9">
+        <v>3</v>
+      </c>
+      <c r="J597" s="9">
+        <v>4</v>
+      </c>
+      <c r="K597" s="9">
+        <v>3</v>
+      </c>
+      <c r="L597" s="9">
+        <v>3</v>
+      </c>
+      <c r="M597" s="9">
+        <v>4</v>
+      </c>
+      <c r="N597" s="9">
+        <v>3</v>
+      </c>
+      <c r="O597" s="9">
+        <v>5</v>
+      </c>
+      <c r="P597" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q597" s="9">
+        <v>3</v>
+      </c>
+      <c r="R597" s="9">
+        <v>4</v>
+      </c>
+      <c r="S597" s="9">
+        <v>4</v>
+      </c>
+      <c r="T597" s="9">
+        <v>2</v>
+      </c>
+      <c r="U597" s="9">
+        <v>6</v>
+      </c>
+      <c r="V597" s="9">
+        <v>3</v>
+      </c>
+      <c r="W597" s="9">
+        <v>3</v>
+      </c>
+      <c r="X597" s="9">
+        <v>6</v>
+      </c>
+      <c r="Y597" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z597" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA597" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB597" s="9">
+        <v>6</v>
+      </c>
+      <c r="AC597" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD597" s="9">
+        <v>5</v>
+      </c>
+      <c r="AE597" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF597" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG597" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH597" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI597" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ597" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="598" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A598" s="4">
+        <v>45599.653055717594</v>
+      </c>
+      <c r="B598" s="5" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C598" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D598" s="5">
+        <v>20243723</v>
+      </c>
+      <c r="E598" s="5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="F598" s="6">
+        <v>0.65000000000145519</v>
+      </c>
+      <c r="G598" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK598" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL598" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM598" s="5">
+        <v>6</v>
+      </c>
+      <c r="AN598" s="5">
+        <v>6</v>
+      </c>
+      <c r="AO598" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP598" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ598" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR598" s="5">
+        <v>6</v>
+      </c>
+      <c r="AS598" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT598" s="5">
+        <v>3</v>
+      </c>
+      <c r="AU598" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV598" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW598" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX598" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY598" s="5">
+        <v>6</v>
+      </c>
+      <c r="AZ598" s="5">
+        <v>6</v>
+      </c>
+      <c r="BA598" s="5">
+        <v>6</v>
+      </c>
+      <c r="BB598" s="5">
+        <v>6</v>
+      </c>
+      <c r="BC598" s="5">
+        <v>4</v>
+      </c>
+      <c r="BD598" s="5">
+        <v>6</v>
+      </c>
+      <c r="BE598" s="5">
+        <v>6</v>
+      </c>
+      <c r="BF598" s="5">
+        <v>6</v>
+      </c>
+      <c r="BG598" s="5">
+        <v>5</v>
+      </c>
+      <c r="BH598" s="5">
+        <v>3</v>
+      </c>
+      <c r="BI598" s="5">
+        <v>2</v>
+      </c>
+      <c r="BJ598" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK598" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL598" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM598" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="599" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A599" s="8">
+        <v>45599.655378599535</v>
+      </c>
+      <c r="B599" s="9" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C599" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D599" s="9">
+        <v>20213719</v>
+      </c>
+      <c r="E599" s="9" t="s">
+        <v>1351</v>
+      </c>
+      <c r="F599" s="10">
+        <v>0.65486111110658385</v>
+      </c>
+      <c r="G599" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL599" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN599" s="9">
+        <v>2</v>
+      </c>
+      <c r="AO599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT599" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY599" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ599" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA599" s="9">
+        <v>2</v>
+      </c>
+      <c r="BB599" s="9">
+        <v>2</v>
+      </c>
+      <c r="BC599" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD599" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE599" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF599" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG599" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH599" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI599" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ599" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK599" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL599" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM599" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="600" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A600" s="4">
+        <v>45599.657546840273</v>
+      </c>
+      <c r="B600" s="5" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C600" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D600" s="5">
+        <v>20202501</v>
+      </c>
+      <c r="E600" s="5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="F600" s="6">
+        <v>0.65486111110658385</v>
+      </c>
+      <c r="G600" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H600" s="5">
+        <v>3</v>
+      </c>
+      <c r="I600" s="5">
+        <v>5</v>
+      </c>
+      <c r="J600" s="5">
+        <v>4</v>
+      </c>
+      <c r="K600" s="5">
+        <v>3</v>
+      </c>
+      <c r="L600" s="5">
+        <v>1</v>
+      </c>
+      <c r="M600" s="5">
+        <v>4</v>
+      </c>
+      <c r="N600" s="5">
+        <v>3</v>
+      </c>
+      <c r="O600" s="5">
+        <v>5</v>
+      </c>
+      <c r="P600" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q600" s="5">
+        <v>4</v>
+      </c>
+      <c r="R600" s="5">
+        <v>3</v>
+      </c>
+      <c r="S600" s="5">
+        <v>2</v>
+      </c>
+      <c r="T600" s="5">
+        <v>4</v>
+      </c>
+      <c r="U600" s="5">
+        <v>3</v>
+      </c>
+      <c r="V600" s="5">
+        <v>3</v>
+      </c>
+      <c r="W600" s="5">
+        <v>3</v>
+      </c>
+      <c r="X600" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y600" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z600" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA600" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB600" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC600" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD600" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE600" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF600" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG600" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH600" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI600" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ600" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="601" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A601" s="8">
+        <v>45599.663020601853</v>
+      </c>
+      <c r="B601" s="9" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C601" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="D601" s="9">
+        <v>20231708</v>
+      </c>
+      <c r="E601" s="9" t="s">
+        <v>1355</v>
+      </c>
+      <c r="F601" s="10">
+        <v>0.66111111111240461</v>
+      </c>
+      <c r="G601" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H601" s="9">
+        <v>1</v>
+      </c>
+      <c r="I601" s="9">
+        <v>4</v>
+      </c>
+      <c r="J601" s="9">
+        <v>2</v>
+      </c>
+      <c r="K601" s="9">
+        <v>3</v>
+      </c>
+      <c r="L601" s="9">
+        <v>3</v>
+      </c>
+      <c r="M601" s="9">
+        <v>3</v>
+      </c>
+      <c r="N601" s="9">
+        <v>2</v>
+      </c>
+      <c r="O601" s="9">
+        <v>3</v>
+      </c>
+      <c r="P601" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q601" s="9">
+        <v>3</v>
+      </c>
+      <c r="R601" s="9">
+        <v>3</v>
+      </c>
+      <c r="S601" s="9">
+        <v>3</v>
+      </c>
+      <c r="T601" s="9">
+        <v>3</v>
+      </c>
+      <c r="U601" s="9">
+        <v>3</v>
+      </c>
+      <c r="V601" s="9">
+        <v>3</v>
+      </c>
+      <c r="W601" s="9">
+        <v>3</v>
+      </c>
+      <c r="X601" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y601" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI601" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ601" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="602" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A602" s="4">
+        <v>45599.664273831018</v>
+      </c>
+      <c r="B602" s="5" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C602" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D602" s="5">
+        <v>20243731</v>
+      </c>
+      <c r="E602" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F602" s="6">
+        <v>0.66319444444525288</v>
+      </c>
+      <c r="G602" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H602" s="5">
+        <v>5</v>
+      </c>
+      <c r="I602" s="5">
+        <v>5</v>
+      </c>
+      <c r="J602" s="5">
+        <v>5</v>
+      </c>
+      <c r="K602" s="5">
+        <v>5</v>
+      </c>
+      <c r="L602" s="5">
+        <v>5</v>
+      </c>
+      <c r="M602" s="5">
+        <v>5</v>
+      </c>
+      <c r="N602" s="5">
+        <v>5</v>
+      </c>
+      <c r="O602" s="5">
+        <v>5</v>
+      </c>
+      <c r="P602" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q602" s="5">
+        <v>3</v>
+      </c>
+      <c r="R602" s="5">
+        <v>3</v>
+      </c>
+      <c r="S602" s="5">
+        <v>3</v>
+      </c>
+      <c r="T602" s="5">
+        <v>4</v>
+      </c>
+      <c r="U602" s="5">
+        <v>5</v>
+      </c>
+      <c r="V602" s="5">
+        <v>3</v>
+      </c>
+      <c r="W602" s="5">
+        <v>4</v>
+      </c>
+      <c r="X602" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y602" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z602" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA602" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB602" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC602" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD602" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE602" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF602" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG602" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH602" s="5">
+        <v>4</v>
+      </c>
+      <c r="AI602" s="5">
+        <v>4</v>
+      </c>
+      <c r="AJ602" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="603" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A603" s="8">
+        <v>45599.666742997681</v>
+      </c>
+      <c r="B603" s="9" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C603" s="9" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D603" s="9">
+        <v>20233846</v>
+      </c>
+      <c r="E603" s="9" t="s">
+        <v>1359</v>
+      </c>
+      <c r="F603" s="10">
+        <v>0.66527777777810115</v>
+      </c>
+      <c r="G603" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK603" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL603" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM603" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN603" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO603" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP603" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ603" s="9">
+        <v>4</v>
+      </c>
+      <c r="AR603" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS603" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT603" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU603" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV603" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW603" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX603" s="9">
+        <v>4</v>
+      </c>
+      <c r="AY603" s="9">
+        <v>5</v>
+      </c>
+      <c r="AZ603" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA603" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB603" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC603" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD603" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE603" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF603" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG603" s="9">
+        <v>4</v>
+      </c>
+      <c r="BH603" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI603" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ603" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK603" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL603" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM603" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="604" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A604" s="4">
+        <v>45599.668931539352</v>
+      </c>
+      <c r="B604" s="5" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C604" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D604" s="5">
+        <v>20245109</v>
+      </c>
+      <c r="E604" s="5" t="s">
+        <v>1361</v>
+      </c>
+      <c r="F604" s="6">
+        <v>0.16666666666424135</v>
+      </c>
+      <c r="G604" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H604" s="5">
+        <v>1</v>
+      </c>
+      <c r="I604" s="5">
+        <v>3</v>
+      </c>
+      <c r="J604" s="5">
+        <v>4</v>
+      </c>
+      <c r="K604" s="5">
+        <v>4</v>
+      </c>
+      <c r="L604" s="5">
+        <v>4</v>
+      </c>
+      <c r="M604" s="5">
+        <v>3</v>
+      </c>
+      <c r="N604" s="5">
+        <v>3</v>
+      </c>
+      <c r="O604" s="5">
+        <v>4</v>
+      </c>
+      <c r="P604" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q604" s="5">
+        <v>2</v>
+      </c>
+      <c r="R604" s="5">
+        <v>3</v>
+      </c>
+      <c r="S604" s="5">
+        <v>3</v>
+      </c>
+      <c r="T604" s="5">
+        <v>1</v>
+      </c>
+      <c r="U604" s="5">
+        <v>4</v>
+      </c>
+      <c r="V604" s="5">
+        <v>3</v>
+      </c>
+      <c r="W604" s="5">
+        <v>4</v>
+      </c>
+      <c r="X604" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y604" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z604" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA604" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB604" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC604" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD604" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE604" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF604" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG604" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH604" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI604" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ604" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="605" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A605" s="8">
+        <v>45599.669096215279</v>
+      </c>
+      <c r="B605" s="9" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C605" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D605" s="9">
+        <v>20246306</v>
+      </c>
+      <c r="E605" s="9" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F605" s="10">
+        <v>0.6680555555576575</v>
+      </c>
+      <c r="G605" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AO605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AP605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AQ605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AR605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AS605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AT605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AU605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AV605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AW605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AX605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AY605" s="9">
+        <v>1</v>
+      </c>
+      <c r="AZ605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BA605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BB605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BC605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BD605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BE605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BF605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BG605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BH605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BI605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BJ605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BK605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BL605" s="9">
+        <v>1</v>
+      </c>
+      <c r="BM605" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="606" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A606" s="4">
+        <v>45599.669593900464</v>
+      </c>
+      <c r="B606" s="5" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C606" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D606" s="5">
+        <v>20242423</v>
+      </c>
+      <c r="E606" s="5" t="s">
+        <v>1365</v>
+      </c>
+      <c r="F606" s="6">
+        <v>0.66736111111094942</v>
+      </c>
+      <c r="G606" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK606" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL606" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM606" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN606" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO606" s="5">
+        <v>2</v>
+      </c>
+      <c r="AP606" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ606" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR606" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS606" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT606" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU606" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV606" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW606" s="5">
+        <v>2</v>
+      </c>
+      <c r="AX606" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY606" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ606" s="5">
+        <v>3</v>
+      </c>
+      <c r="BA606" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB606" s="5">
+        <v>3</v>
+      </c>
+      <c r="BC606" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD606" s="5">
+        <v>3</v>
+      </c>
+      <c r="BE606" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF606" s="5">
+        <v>3</v>
+      </c>
+      <c r="BG606" s="5">
+        <v>3</v>
+      </c>
+      <c r="BH606" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI606" s="5">
+        <v>3</v>
+      </c>
+      <c r="BJ606" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK606" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL606" s="5">
+        <v>2</v>
+      </c>
+      <c r="BM606" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="607" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A607" s="8">
+        <v>45599.669851516199</v>
+      </c>
+      <c r="B607" s="9" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C607" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D607" s="9">
+        <v>20242230</v>
+      </c>
+      <c r="E607" s="9" t="s">
+        <v>1367</v>
+      </c>
+      <c r="F607" s="10">
+        <v>0.66041666666569654</v>
+      </c>
+      <c r="G607" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H607" s="9">
+        <v>1</v>
+      </c>
+      <c r="I607" s="9">
+        <v>4</v>
+      </c>
+      <c r="J607" s="9">
+        <v>5</v>
+      </c>
+      <c r="K607" s="9">
+        <v>3</v>
+      </c>
+      <c r="L607" s="9">
+        <v>1</v>
+      </c>
+      <c r="M607" s="9">
+        <v>1</v>
+      </c>
+      <c r="N607" s="9">
+        <v>4</v>
+      </c>
+      <c r="O607" s="9">
+        <v>4</v>
+      </c>
+      <c r="P607" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q607" s="9">
+        <v>2</v>
+      </c>
+      <c r="R607" s="9">
+        <v>6</v>
+      </c>
+      <c r="S607" s="9">
+        <v>4</v>
+      </c>
+      <c r="T607" s="9">
+        <v>2</v>
+      </c>
+      <c r="U607" s="9">
+        <v>1</v>
+      </c>
+      <c r="V607" s="9">
+        <v>5</v>
+      </c>
+      <c r="W607" s="9">
+        <v>5</v>
+      </c>
+      <c r="X607" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y607" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z607" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA607" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB607" s="9">
+        <v>6</v>
+      </c>
+      <c r="AC607" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD607" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE607" s="9">
+        <v>2</v>
+      </c>
+      <c r="AF607" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG607" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH607" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI607" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ607" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="608" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A608" s="4">
+        <v>45599.674149467595</v>
+      </c>
+      <c r="B608" s="5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C608" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D608" s="5">
+        <v>20246768</v>
+      </c>
+      <c r="E608" s="5" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F608" s="6">
+        <v>0.67152777777664596</v>
+      </c>
+      <c r="G608" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK608" s="5">
+        <v>5</v>
+      </c>
+      <c r="AL608" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM608" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN608" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO608" s="5">
+        <v>2</v>
+      </c>
+      <c r="AP608" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ608" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR608" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS608" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT608" s="5">
+        <v>6</v>
+      </c>
+      <c r="AU608" s="5">
+        <v>4</v>
+      </c>
+      <c r="AV608" s="5">
+        <v>6</v>
+      </c>
+      <c r="AW608" s="5">
+        <v>5</v>
+      </c>
+      <c r="AX608" s="5">
+        <v>6</v>
+      </c>
+      <c r="AY608" s="5">
+        <v>6</v>
+      </c>
+      <c r="AZ608" s="5">
+        <v>6</v>
+      </c>
+      <c r="BA608" s="5">
+        <v>6</v>
+      </c>
+      <c r="BB608" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC608" s="5">
+        <v>6</v>
+      </c>
+      <c r="BD608" s="5">
+        <v>6</v>
+      </c>
+      <c r="BE608" s="5">
+        <v>6</v>
+      </c>
+      <c r="BF608" s="5">
+        <v>6</v>
+      </c>
+      <c r="BG608" s="5">
+        <v>5</v>
+      </c>
+      <c r="BH608" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI608" s="5">
+        <v>6</v>
+      </c>
+      <c r="BJ608" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK608" s="5">
+        <v>6</v>
+      </c>
+      <c r="BL608" s="5">
+        <v>5</v>
+      </c>
+      <c r="BM608" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="609" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A609" s="18">
+        <v>45599.678108472217</v>
+      </c>
+      <c r="B609" s="19" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C609" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D609" s="19">
+        <v>20242628</v>
+      </c>
+      <c r="E609" s="19" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F609" s="20">
+        <v>0.75902777777810115</v>
+      </c>
+      <c r="G609" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H609" s="26"/>
+      <c r="I609" s="26"/>
+      <c r="J609" s="26"/>
+      <c r="K609" s="26"/>
+      <c r="L609" s="26"/>
+      <c r="M609" s="26"/>
+      <c r="N609" s="26"/>
+      <c r="O609" s="26"/>
+      <c r="P609" s="26"/>
+      <c r="Q609" s="26"/>
+      <c r="R609" s="26"/>
+      <c r="S609" s="26"/>
+      <c r="T609" s="26"/>
+      <c r="U609" s="26"/>
+      <c r="V609" s="26"/>
+      <c r="W609" s="26"/>
+      <c r="X609" s="26"/>
+      <c r="Y609" s="26"/>
+      <c r="Z609" s="26"/>
+      <c r="AA609" s="26"/>
+      <c r="AB609" s="26"/>
+      <c r="AC609" s="26"/>
+      <c r="AD609" s="26"/>
+      <c r="AE609" s="26"/>
+      <c r="AF609" s="26"/>
+      <c r="AG609" s="26"/>
+      <c r="AH609" s="26"/>
+      <c r="AI609" s="26"/>
+      <c r="AJ609" s="26"/>
+      <c r="AK609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AL609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AM609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AN609" s="19">
+        <v>4</v>
+      </c>
+      <c r="AO609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AP609" s="19">
+        <v>2</v>
+      </c>
+      <c r="AQ609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AR609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AS609" s="19">
+        <v>6</v>
+      </c>
+      <c r="AT609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AU609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AV609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AW609" s="19">
+        <v>2</v>
+      </c>
+      <c r="AX609" s="19">
+        <v>3</v>
+      </c>
+      <c r="AY609" s="19">
+        <v>6</v>
+      </c>
+      <c r="AZ609" s="19">
+        <v>6</v>
+      </c>
+      <c r="BA609" s="19">
+        <v>4</v>
+      </c>
+      <c r="BB609" s="19">
+        <v>4</v>
+      </c>
+      <c r="BC609" s="19">
+        <v>4</v>
+      </c>
+      <c r="BD609" s="19">
+        <v>4</v>
+      </c>
+      <c r="BE609" s="19">
+        <v>4</v>
+      </c>
+      <c r="BF609" s="19">
+        <v>6</v>
+      </c>
+      <c r="BG609" s="19">
+        <v>4</v>
+      </c>
+      <c r="BH609" s="19">
+        <v>3</v>
+      </c>
+      <c r="BI609" s="19">
+        <v>4</v>
+      </c>
+      <c r="BJ609" s="19">
+        <v>4</v>
+      </c>
+      <c r="BK609" s="19">
+        <v>3</v>
+      </c>
+      <c r="BL609" s="19">
+        <v>4</v>
+      </c>
+      <c r="BM609" s="22">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
241021, oxford modified sunday 18:40
</commit_message>
<xml_diff>
--- a/R/data/oxford_241021.xlsx
+++ b/R/data/oxford_241021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Dropbox/내 Mac (Kee-Won의 MacBook Air)/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E74342-7970-A148-8BAE-9B312C77B5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC0840B-FAD4-0D43-AE20-C04CE2B60FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42920" yWindow="1420" windowWidth="37080" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="1372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="1442">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -4139,6 +4139,216 @@
   </si>
   <si>
     <t>이영주</t>
+  </si>
+  <si>
+    <t>ziva0726@naver.com</t>
+  </si>
+  <si>
+    <t>김소현</t>
+  </si>
+  <si>
+    <t>kjh54088@gmail.com</t>
+  </si>
+  <si>
+    <t>김재희</t>
+  </si>
+  <si>
+    <t>dearmy0819@gmail.com</t>
+  </si>
+  <si>
+    <t>박혜원</t>
+  </si>
+  <si>
+    <t>taewon16@naver.com</t>
+  </si>
+  <si>
+    <t>류태원</t>
+  </si>
+  <si>
+    <t>joo6806898@naver.com</t>
+  </si>
+  <si>
+    <t>김승주</t>
+  </si>
+  <si>
+    <t>kusahana8047@gmail.com</t>
+  </si>
+  <si>
+    <t>유현우</t>
+  </si>
+  <si>
+    <t>goeunsue@naver.com</t>
+  </si>
+  <si>
+    <t>고은수</t>
+  </si>
+  <si>
+    <t>hyerim0v0@gmail.com</t>
+  </si>
+  <si>
+    <t>전혜림</t>
+  </si>
+  <si>
+    <t>iiiiii3314@naver.com</t>
+  </si>
+  <si>
+    <t>엄수빈</t>
+  </si>
+  <si>
+    <t>kmjung0948@gmail.com</t>
+  </si>
+  <si>
+    <t>진현수</t>
+  </si>
+  <si>
+    <t>sht05137@gmail.com</t>
+  </si>
+  <si>
+    <t>류정석</t>
+  </si>
+  <si>
+    <t>kesha11@naver.com</t>
+  </si>
+  <si>
+    <t>윤주호</t>
+  </si>
+  <si>
+    <t>crown7308@naver.com</t>
+  </si>
+  <si>
+    <t>콘텐츠it</t>
+  </si>
+  <si>
+    <t>박재환</t>
+  </si>
+  <si>
+    <t>hanyejun339@gmail.com</t>
+  </si>
+  <si>
+    <t>한예준</t>
+  </si>
+  <si>
+    <t>050624alex@gmail.com</t>
+  </si>
+  <si>
+    <t>이승현</t>
+  </si>
+  <si>
+    <t>uj5343@gmail.com</t>
+  </si>
+  <si>
+    <t>장우찬</t>
+  </si>
+  <si>
+    <t>in3019@gmail.com</t>
+  </si>
+  <si>
+    <t>이승윤</t>
+  </si>
+  <si>
+    <t>youmin43@naver.com</t>
+  </si>
+  <si>
+    <t>박유민</t>
+  </si>
+  <si>
+    <t>applehanul@naver.com</t>
+  </si>
+  <si>
+    <t>신하늘</t>
+  </si>
+  <si>
+    <t>kby5432@naver.com</t>
+  </si>
+  <si>
+    <t>윤경빈</t>
+  </si>
+  <si>
+    <t>lendjo@naver.com</t>
+  </si>
+  <si>
+    <t>오한별</t>
+  </si>
+  <si>
+    <t>cth041103@naver.com</t>
+  </si>
+  <si>
+    <t>최태희</t>
+  </si>
+  <si>
+    <t>ann12ann1209@gmail.com</t>
+  </si>
+  <si>
+    <t>김혜원</t>
+  </si>
+  <si>
+    <t>peony.chung04@gmail.com</t>
+  </si>
+  <si>
+    <t>정수영</t>
+  </si>
+  <si>
+    <t>ghksltjrl@naver.com</t>
+  </si>
+  <si>
+    <t>이용환</t>
+  </si>
+  <si>
+    <t>jign1106@naver.com</t>
+  </si>
+  <si>
+    <t>지은총</t>
+  </si>
+  <si>
+    <t>p1aymaker9926@gmail.com</t>
+  </si>
+  <si>
+    <t>김대환</t>
+  </si>
+  <si>
+    <t>ljw76825119@gmail.com</t>
+  </si>
+  <si>
+    <t>johanjoon5734@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">조한준 </t>
+  </si>
+  <si>
+    <t>hyu05145@gmail.com</t>
+  </si>
+  <si>
+    <t>정서진</t>
+  </si>
+  <si>
+    <t>mjsong4130@gmail.com</t>
+  </si>
+  <si>
+    <t>인공지능융합학부 ai로봇융합전공</t>
+  </si>
+  <si>
+    <t>송민재</t>
+  </si>
+  <si>
+    <t>slionrain0819@naver.com</t>
+  </si>
+  <si>
+    <t>정의환</t>
+  </si>
+  <si>
+    <t>sjw9802@naver.com</t>
+  </si>
+  <si>
+    <t>선지우</t>
+  </si>
+  <si>
+    <t>chaerin3940@gmail.com</t>
+  </si>
+  <si>
+    <t>김채린</t>
+  </si>
+  <si>
+    <t>20217096@hallym.ac.kr</t>
   </si>
 </sst>
 </file>
@@ -4582,7 +4792,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM609">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM644">
   <tableColumns count="65">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -4855,11 +5065,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM609"/>
+  <dimension ref="A1:BM644"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C614" sqref="C614"/>
+      <pane ySplit="1" topLeftCell="A613" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G650" sqref="G650"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -72753,35 +72963,6 @@
       <c r="G609" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H609" s="26"/>
-      <c r="I609" s="26"/>
-      <c r="J609" s="26"/>
-      <c r="K609" s="26"/>
-      <c r="L609" s="26"/>
-      <c r="M609" s="26"/>
-      <c r="N609" s="26"/>
-      <c r="O609" s="26"/>
-      <c r="P609" s="26"/>
-      <c r="Q609" s="26"/>
-      <c r="R609" s="26"/>
-      <c r="S609" s="26"/>
-      <c r="T609" s="26"/>
-      <c r="U609" s="26"/>
-      <c r="V609" s="26"/>
-      <c r="W609" s="26"/>
-      <c r="X609" s="26"/>
-      <c r="Y609" s="26"/>
-      <c r="Z609" s="26"/>
-      <c r="AA609" s="26"/>
-      <c r="AB609" s="26"/>
-      <c r="AC609" s="26"/>
-      <c r="AD609" s="26"/>
-      <c r="AE609" s="26"/>
-      <c r="AF609" s="26"/>
-      <c r="AG609" s="26"/>
-      <c r="AH609" s="26"/>
-      <c r="AI609" s="26"/>
-      <c r="AJ609" s="26"/>
       <c r="AK609" s="19">
         <v>3</v>
       </c>
@@ -72868,6 +73049,3885 @@
       </c>
       <c r="BM609" s="22">
         <v>1</v>
+      </c>
+    </row>
+    <row r="610" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A610" s="4">
+        <v>45599.68247190972</v>
+      </c>
+      <c r="B610" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C610" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D610" s="5">
+        <v>20212104</v>
+      </c>
+      <c r="E610" s="5" t="s">
+        <v>1373</v>
+      </c>
+      <c r="F610" s="6">
+        <v>0.6756944444423425</v>
+      </c>
+      <c r="G610" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK610" s="5">
+        <v>3</v>
+      </c>
+      <c r="AL610" s="5">
+        <v>2</v>
+      </c>
+      <c r="AM610" s="5">
+        <v>2</v>
+      </c>
+      <c r="AN610" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO610" s="5">
+        <v>1</v>
+      </c>
+      <c r="AP610" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ610" s="5">
+        <v>1</v>
+      </c>
+      <c r="AR610" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS610" s="5">
+        <v>1</v>
+      </c>
+      <c r="AT610" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU610" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV610" s="5">
+        <v>1</v>
+      </c>
+      <c r="AW610" s="5">
+        <v>2</v>
+      </c>
+      <c r="AX610" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY610" s="5">
+        <v>1</v>
+      </c>
+      <c r="AZ610" s="5">
+        <v>2</v>
+      </c>
+      <c r="BA610" s="5">
+        <v>1</v>
+      </c>
+      <c r="BB610" s="5">
+        <v>2</v>
+      </c>
+      <c r="BC610" s="5">
+        <v>1</v>
+      </c>
+      <c r="BD610" s="5">
+        <v>1</v>
+      </c>
+      <c r="BE610" s="5">
+        <v>2</v>
+      </c>
+      <c r="BF610" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG610" s="5">
+        <v>1</v>
+      </c>
+      <c r="BH610" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI610" s="5">
+        <v>1</v>
+      </c>
+      <c r="BJ610" s="5">
+        <v>2</v>
+      </c>
+      <c r="BK610" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL610" s="5">
+        <v>4</v>
+      </c>
+      <c r="BM610" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="611" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A611" s="8">
+        <v>45599.683703784722</v>
+      </c>
+      <c r="B611" s="9" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C611" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="D611" s="9">
+        <v>20243216</v>
+      </c>
+      <c r="E611" s="9" t="s">
+        <v>1375</v>
+      </c>
+      <c r="F611" s="10">
+        <v>0.66666666666424135</v>
+      </c>
+      <c r="G611" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK611" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL611" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM611" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN611" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO611" s="9">
+        <v>5</v>
+      </c>
+      <c r="AP611" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ611" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR611" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS611" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT611" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU611" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV611" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW611" s="9">
+        <v>4</v>
+      </c>
+      <c r="AX611" s="9">
+        <v>4</v>
+      </c>
+      <c r="AY611" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ611" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA611" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB611" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC611" s="9">
+        <v>4</v>
+      </c>
+      <c r="BD611" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE611" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF611" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG611" s="9">
+        <v>4</v>
+      </c>
+      <c r="BH611" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI611" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ611" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK611" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL611" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM611" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="612" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A612" s="4">
+        <v>45599.684193252317</v>
+      </c>
+      <c r="B612" s="5" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C612" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D612" s="5">
+        <v>20243225</v>
+      </c>
+      <c r="E612" s="5" t="s">
+        <v>1377</v>
+      </c>
+      <c r="F612" s="6">
+        <v>0.68125000000145519</v>
+      </c>
+      <c r="G612" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK612" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL612" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM612" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN612" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO612" s="5">
+        <v>6</v>
+      </c>
+      <c r="AP612" s="5">
+        <v>1</v>
+      </c>
+      <c r="AQ612" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR612" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS612" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT612" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU612" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV612" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW612" s="5">
+        <v>2</v>
+      </c>
+      <c r="AX612" s="5">
+        <v>5</v>
+      </c>
+      <c r="AY612" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ612" s="5">
+        <v>6</v>
+      </c>
+      <c r="BA612" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB612" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC612" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD612" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE612" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF612" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG612" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH612" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI612" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ612" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK612" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL612" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM612" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="613" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A613" s="8">
+        <v>45599.685538888887</v>
+      </c>
+      <c r="B613" s="9" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C613" s="9" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D613" s="9">
+        <v>20195158</v>
+      </c>
+      <c r="E613" s="9" t="s">
+        <v>1379</v>
+      </c>
+      <c r="F613" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="G613" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H613" s="9">
+        <v>4</v>
+      </c>
+      <c r="I613" s="9">
+        <v>2</v>
+      </c>
+      <c r="J613" s="9">
+        <v>2</v>
+      </c>
+      <c r="K613" s="9">
+        <v>2</v>
+      </c>
+      <c r="L613" s="9">
+        <v>4</v>
+      </c>
+      <c r="M613" s="9">
+        <v>4</v>
+      </c>
+      <c r="N613" s="9">
+        <v>2</v>
+      </c>
+      <c r="O613" s="9">
+        <v>4</v>
+      </c>
+      <c r="P613" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q613" s="9">
+        <v>4</v>
+      </c>
+      <c r="R613" s="9">
+        <v>3</v>
+      </c>
+      <c r="S613" s="9">
+        <v>3</v>
+      </c>
+      <c r="T613" s="9">
+        <v>4</v>
+      </c>
+      <c r="U613" s="9">
+        <v>4</v>
+      </c>
+      <c r="V613" s="9">
+        <v>3</v>
+      </c>
+      <c r="W613" s="9">
+        <v>2</v>
+      </c>
+      <c r="X613" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y613" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z613" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA613" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB613" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC613" s="9">
+        <v>2</v>
+      </c>
+      <c r="AD613" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE613" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF613" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG613" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH613" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI613" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ613" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="614" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A614" s="4">
+        <v>45599.687710590282</v>
+      </c>
+      <c r="B614" s="5" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C614" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D614" s="5">
+        <v>20223605</v>
+      </c>
+      <c r="E614" s="5" t="s">
+        <v>1381</v>
+      </c>
+      <c r="F614" s="6">
+        <v>0.68680555555329192</v>
+      </c>
+      <c r="G614" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AT614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AV614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AX614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY614" s="5">
+        <v>4</v>
+      </c>
+      <c r="AZ614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BD614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL614" s="5">
+        <v>4</v>
+      </c>
+      <c r="BM614" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="615" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A615" s="8">
+        <v>45599.688176712967</v>
+      </c>
+      <c r="B615" s="9" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C615" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D615" s="9">
+        <v>20192736</v>
+      </c>
+      <c r="E615" s="9" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F615" s="10">
+        <v>0.66666666666424135</v>
+      </c>
+      <c r="G615" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK615" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL615" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM615" s="9">
+        <v>2</v>
+      </c>
+      <c r="AN615" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO615" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP615" s="9">
+        <v>2</v>
+      </c>
+      <c r="AQ615" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR615" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS615" s="9">
+        <v>6</v>
+      </c>
+      <c r="AT615" s="9">
+        <v>1</v>
+      </c>
+      <c r="AU615" s="9">
+        <v>6</v>
+      </c>
+      <c r="AV615" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW615" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX615" s="9">
+        <v>4</v>
+      </c>
+      <c r="AY615" s="9">
+        <v>6</v>
+      </c>
+      <c r="AZ615" s="9">
+        <v>6</v>
+      </c>
+      <c r="BA615" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB615" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC615" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD615" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE615" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF615" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG615" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH615" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI615" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ615" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK615" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL615" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM615" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="616" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A616" s="4">
+        <v>45599.693859988431</v>
+      </c>
+      <c r="B616" s="5" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C616" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D616" s="5">
+        <v>20242907</v>
+      </c>
+      <c r="E616" s="5" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F616" s="6">
+        <v>0.69166666666569654</v>
+      </c>
+      <c r="G616" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK616" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL616" s="5">
+        <v>6</v>
+      </c>
+      <c r="AM616" s="5">
+        <v>6</v>
+      </c>
+      <c r="AN616" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO616" s="5">
+        <v>2</v>
+      </c>
+      <c r="AP616" s="5">
+        <v>1</v>
+      </c>
+      <c r="AQ616" s="5">
+        <v>6</v>
+      </c>
+      <c r="AR616" s="5">
+        <v>6</v>
+      </c>
+      <c r="AS616" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT616" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU616" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV616" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW616" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX616" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY616" s="5">
+        <v>6</v>
+      </c>
+      <c r="AZ616" s="5">
+        <v>6</v>
+      </c>
+      <c r="BA616" s="5">
+        <v>6</v>
+      </c>
+      <c r="BB616" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC616" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD616" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE616" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF616" s="5">
+        <v>6</v>
+      </c>
+      <c r="BG616" s="5">
+        <v>2</v>
+      </c>
+      <c r="BH616" s="5">
+        <v>1</v>
+      </c>
+      <c r="BI616" s="5">
+        <v>6</v>
+      </c>
+      <c r="BJ616" s="5">
+        <v>6</v>
+      </c>
+      <c r="BK616" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL616" s="5">
+        <v>1</v>
+      </c>
+      <c r="BM616" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="617" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A617" s="8">
+        <v>45599.697394710645</v>
+      </c>
+      <c r="B617" s="9" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C617" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D617" s="9">
+        <v>20231630</v>
+      </c>
+      <c r="E617" s="9" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F617" s="10">
+        <v>0.69305555555911269</v>
+      </c>
+      <c r="G617" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H617" s="9">
+        <v>3</v>
+      </c>
+      <c r="I617" s="9">
+        <v>2</v>
+      </c>
+      <c r="J617" s="9">
+        <v>4</v>
+      </c>
+      <c r="K617" s="9">
+        <v>4</v>
+      </c>
+      <c r="L617" s="9">
+        <v>4</v>
+      </c>
+      <c r="M617" s="9">
+        <v>4</v>
+      </c>
+      <c r="N617" s="9">
+        <v>3</v>
+      </c>
+      <c r="O617" s="9">
+        <v>3</v>
+      </c>
+      <c r="P617" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q617" s="9">
+        <v>4</v>
+      </c>
+      <c r="R617" s="9">
+        <v>5</v>
+      </c>
+      <c r="S617" s="9">
+        <v>4</v>
+      </c>
+      <c r="T617" s="9">
+        <v>3</v>
+      </c>
+      <c r="U617" s="9">
+        <v>4</v>
+      </c>
+      <c r="V617" s="9">
+        <v>4</v>
+      </c>
+      <c r="W617" s="9">
+        <v>4</v>
+      </c>
+      <c r="X617" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y617" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z617" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA617" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB617" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC617" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD617" s="9">
+        <v>5</v>
+      </c>
+      <c r="AE617" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF617" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG617" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH617" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI617" s="9">
+        <v>3</v>
+      </c>
+      <c r="AJ617" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="618" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A618" s="4">
+        <v>45599.699678912039</v>
+      </c>
+      <c r="B618" s="5" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C618" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D618" s="5">
+        <v>20242986</v>
+      </c>
+      <c r="E618" s="5" t="s">
+        <v>1389</v>
+      </c>
+      <c r="F618" s="6">
+        <v>0.69166666666569654</v>
+      </c>
+      <c r="G618" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK618" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL618" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM618" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN618" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO618" s="5">
+        <v>2</v>
+      </c>
+      <c r="AP618" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ618" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR618" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS618" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT618" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU618" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV618" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW618" s="5">
+        <v>4</v>
+      </c>
+      <c r="AX618" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY618" s="5">
+        <v>4</v>
+      </c>
+      <c r="AZ618" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA618" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB618" s="5">
+        <v>3</v>
+      </c>
+      <c r="BC618" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD618" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE618" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF618" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG618" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH618" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI618" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ618" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK618" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL618" s="5">
+        <v>2</v>
+      </c>
+      <c r="BM618" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="619" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A619" s="8">
+        <v>45599.699973020834</v>
+      </c>
+      <c r="B619" s="9" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C619" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="D619" s="9">
+        <v>20242352</v>
+      </c>
+      <c r="E619" s="9" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F619" s="10">
+        <v>0.19999999999708962</v>
+      </c>
+      <c r="G619" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY619" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL619" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM619" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="620" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A620" s="4">
+        <v>45599.70029418981</v>
+      </c>
+      <c r="B620" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C620" s="5" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D620" s="5">
+        <v>20195285</v>
+      </c>
+      <c r="E620" s="5" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F620" s="6">
+        <v>0.69791666666424135</v>
+      </c>
+      <c r="G620" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK620" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL620" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM620" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN620" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO620" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP620" s="5">
+        <v>3</v>
+      </c>
+      <c r="AQ620" s="5">
+        <v>4</v>
+      </c>
+      <c r="AR620" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS620" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT620" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU620" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV620" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW620" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX620" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY620" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ620" s="5">
+        <v>3</v>
+      </c>
+      <c r="BA620" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB620" s="5">
+        <v>3</v>
+      </c>
+      <c r="BC620" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD620" s="5">
+        <v>3</v>
+      </c>
+      <c r="BE620" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF620" s="5">
+        <v>3</v>
+      </c>
+      <c r="BG620" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH620" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI620" s="5">
+        <v>3</v>
+      </c>
+      <c r="BJ620" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK620" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL620" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM620" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="621" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A621" s="8">
+        <v>45599.701527488425</v>
+      </c>
+      <c r="B621" s="9" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C621" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D621" s="9">
+        <v>20211059</v>
+      </c>
+      <c r="E621" s="9" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F621" s="10">
+        <v>0.69999999999708962</v>
+      </c>
+      <c r="G621" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK621" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL621" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM621" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN621" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO621" s="9">
+        <v>2</v>
+      </c>
+      <c r="AP621" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ621" s="9">
+        <v>4</v>
+      </c>
+      <c r="AR621" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS621" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT621" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU621" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV621" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW621" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX621" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY621" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ621" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA621" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB621" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC621" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD621" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE621" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF621" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG621" s="9">
+        <v>2</v>
+      </c>
+      <c r="BH621" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI621" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ621" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK621" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL621" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM621" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="622" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A622" s="4">
+        <v>45599.701821527779</v>
+      </c>
+      <c r="B622" s="5" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C622" s="5" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D622" s="5">
+        <v>20205173</v>
+      </c>
+      <c r="E622" s="5" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F622" s="6">
+        <v>0.70069444444379769</v>
+      </c>
+      <c r="G622" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK622" s="5">
+        <v>3</v>
+      </c>
+      <c r="AL622" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM622" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN622" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO622" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP622" s="5">
+        <v>3</v>
+      </c>
+      <c r="AQ622" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR622" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS622" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT622" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU622" s="5">
+        <v>3</v>
+      </c>
+      <c r="AV622" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW622" s="5">
+        <v>4</v>
+      </c>
+      <c r="AX622" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY622" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BA622" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB622" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD622" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BG622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BH622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BI622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BJ622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BL622" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM622" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="623" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A623" s="8">
+        <v>45599.702293043985</v>
+      </c>
+      <c r="B623" s="9" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C623" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D623" s="9">
+        <v>20246649</v>
+      </c>
+      <c r="E623" s="9" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F623" s="10">
+        <v>0.70069444444379769</v>
+      </c>
+      <c r="G623" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK623" s="9">
+        <v>5</v>
+      </c>
+      <c r="AL623" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM623" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN623" s="9">
+        <v>2</v>
+      </c>
+      <c r="AO623" s="9">
+        <v>5</v>
+      </c>
+      <c r="AP623" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ623" s="9">
+        <v>2</v>
+      </c>
+      <c r="AR623" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS623" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT623" s="9">
+        <v>5</v>
+      </c>
+      <c r="AU623" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV623" s="9">
+        <v>2</v>
+      </c>
+      <c r="AW623" s="9">
+        <v>6</v>
+      </c>
+      <c r="AX623" s="9">
+        <v>5</v>
+      </c>
+      <c r="AY623" s="9">
+        <v>2</v>
+      </c>
+      <c r="AZ623" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA623" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB623" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC623" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD623" s="9">
+        <v>2</v>
+      </c>
+      <c r="BE623" s="9">
+        <v>5</v>
+      </c>
+      <c r="BF623" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG623" s="9">
+        <v>2</v>
+      </c>
+      <c r="BH623" s="9">
+        <v>5</v>
+      </c>
+      <c r="BI623" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ623" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK623" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL623" s="9">
+        <v>5</v>
+      </c>
+      <c r="BM623" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="624" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A624" s="4">
+        <v>45599.702747858799</v>
+      </c>
+      <c r="B624" s="5" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C624" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D624" s="5">
+        <v>20245224</v>
+      </c>
+      <c r="E624" s="5" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F624" s="6">
+        <v>0.69722222222480923</v>
+      </c>
+      <c r="G624" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK624" s="5">
+        <v>2</v>
+      </c>
+      <c r="AL624" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM624" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN624" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO624" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP624" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ624" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR624" s="5">
+        <v>6</v>
+      </c>
+      <c r="AS624" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT624" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU624" s="5">
+        <v>4</v>
+      </c>
+      <c r="AV624" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW624" s="5">
+        <v>5</v>
+      </c>
+      <c r="AX624" s="5">
+        <v>5</v>
+      </c>
+      <c r="AY624" s="5">
+        <v>4</v>
+      </c>
+      <c r="AZ624" s="5">
+        <v>6</v>
+      </c>
+      <c r="BA624" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB624" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC624" s="5">
+        <v>5</v>
+      </c>
+      <c r="BD624" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE624" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF624" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG624" s="5">
+        <v>6</v>
+      </c>
+      <c r="BH624" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI624" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ624" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK624" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL624" s="5">
+        <v>6</v>
+      </c>
+      <c r="BM624" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="625" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A625" s="8">
+        <v>45599.708994884262</v>
+      </c>
+      <c r="B625" s="9" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C625" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D625" s="9">
+        <v>20243973</v>
+      </c>
+      <c r="E625" s="9" t="s">
+        <v>1404</v>
+      </c>
+      <c r="F625" s="10">
+        <v>0.70763888888905058</v>
+      </c>
+      <c r="G625" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H625" s="9">
+        <v>4</v>
+      </c>
+      <c r="I625" s="9">
+        <v>5</v>
+      </c>
+      <c r="J625" s="9">
+        <v>3</v>
+      </c>
+      <c r="K625" s="9">
+        <v>4</v>
+      </c>
+      <c r="L625" s="9">
+        <v>5</v>
+      </c>
+      <c r="M625" s="9">
+        <v>5</v>
+      </c>
+      <c r="N625" s="9">
+        <v>3</v>
+      </c>
+      <c r="O625" s="9">
+        <v>5</v>
+      </c>
+      <c r="P625" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q625" s="9">
+        <v>2</v>
+      </c>
+      <c r="R625" s="9">
+        <v>5</v>
+      </c>
+      <c r="S625" s="9">
+        <v>3</v>
+      </c>
+      <c r="T625" s="9">
+        <v>3</v>
+      </c>
+      <c r="U625" s="9">
+        <v>3</v>
+      </c>
+      <c r="V625" s="9">
+        <v>3</v>
+      </c>
+      <c r="W625" s="9">
+        <v>5</v>
+      </c>
+      <c r="X625" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y625" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z625" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA625" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB625" s="9">
+        <v>2</v>
+      </c>
+      <c r="AC625" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD625" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE625" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF625" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG625" s="9">
+        <v>2</v>
+      </c>
+      <c r="AH625" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI625" s="9">
+        <v>5</v>
+      </c>
+      <c r="AJ625" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="626" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A626" s="4">
+        <v>45599.710369201392</v>
+      </c>
+      <c r="B626" s="5" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C626" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D626" s="5">
+        <v>20192229</v>
+      </c>
+      <c r="E626" s="5" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F626" s="6">
+        <v>0.70902777777519077</v>
+      </c>
+      <c r="G626" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H626" s="5">
+        <v>2</v>
+      </c>
+      <c r="I626" s="5">
+        <v>3</v>
+      </c>
+      <c r="J626" s="5">
+        <v>3</v>
+      </c>
+      <c r="K626" s="5">
+        <v>3</v>
+      </c>
+      <c r="L626" s="5">
+        <v>2</v>
+      </c>
+      <c r="M626" s="5">
+        <v>2</v>
+      </c>
+      <c r="N626" s="5">
+        <v>4</v>
+      </c>
+      <c r="O626" s="5">
+        <v>3</v>
+      </c>
+      <c r="P626" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q626" s="5">
+        <v>2</v>
+      </c>
+      <c r="R626" s="5">
+        <v>3</v>
+      </c>
+      <c r="S626" s="5">
+        <v>3</v>
+      </c>
+      <c r="T626" s="5">
+        <v>2</v>
+      </c>
+      <c r="U626" s="5">
+        <v>3</v>
+      </c>
+      <c r="V626" s="5">
+        <v>3</v>
+      </c>
+      <c r="W626" s="5">
+        <v>3</v>
+      </c>
+      <c r="X626" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y626" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z626" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA626" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB626" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC626" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD626" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE626" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF626" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG626" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH626" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI626" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ626" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="627" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A627" s="8">
+        <v>45599.713518356482</v>
+      </c>
+      <c r="B627" s="9" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C627" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D627" s="9">
+        <v>20246728</v>
+      </c>
+      <c r="E627" s="9" t="s">
+        <v>1408</v>
+      </c>
+      <c r="F627" s="10">
+        <v>0.68333333333430346</v>
+      </c>
+      <c r="G627" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H627" s="9">
+        <v>1</v>
+      </c>
+      <c r="I627" s="9">
+        <v>5</v>
+      </c>
+      <c r="J627" s="9">
+        <v>5</v>
+      </c>
+      <c r="K627" s="9">
+        <v>3</v>
+      </c>
+      <c r="L627" s="9">
+        <v>2</v>
+      </c>
+      <c r="M627" s="9">
+        <v>2</v>
+      </c>
+      <c r="N627" s="9">
+        <v>2</v>
+      </c>
+      <c r="O627" s="9">
+        <v>5</v>
+      </c>
+      <c r="P627" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q627" s="9">
+        <v>1</v>
+      </c>
+      <c r="R627" s="9">
+        <v>5</v>
+      </c>
+      <c r="S627" s="9">
+        <v>5</v>
+      </c>
+      <c r="T627" s="9">
+        <v>2</v>
+      </c>
+      <c r="U627" s="9">
+        <v>2</v>
+      </c>
+      <c r="V627" s="9">
+        <v>5</v>
+      </c>
+      <c r="W627" s="9">
+        <v>5</v>
+      </c>
+      <c r="X627" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y627" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z627" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA627" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB627" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC627" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD627" s="9">
+        <v>5</v>
+      </c>
+      <c r="AE627" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF627" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG627" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH627" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI627" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ627" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="628" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A628" s="4">
+        <v>45599.714750300926</v>
+      </c>
+      <c r="B628" s="5" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C628" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D628" s="5">
+        <v>20233412</v>
+      </c>
+      <c r="E628" s="5" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F628" s="6">
+        <v>0.71250000000145519</v>
+      </c>
+      <c r="G628" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK628" s="5">
+        <v>6</v>
+      </c>
+      <c r="AL628" s="5">
+        <v>6</v>
+      </c>
+      <c r="AM628" s="5">
+        <v>4</v>
+      </c>
+      <c r="AN628" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO628" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP628" s="5">
+        <v>6</v>
+      </c>
+      <c r="AQ628" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR628" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS628" s="5">
+        <v>2</v>
+      </c>
+      <c r="AT628" s="5">
+        <v>5</v>
+      </c>
+      <c r="AU628" s="5">
+        <v>4</v>
+      </c>
+      <c r="AV628" s="5">
+        <v>1</v>
+      </c>
+      <c r="AW628" s="5">
+        <v>6</v>
+      </c>
+      <c r="AX628" s="5">
+        <v>6</v>
+      </c>
+      <c r="AY628" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ628" s="5">
+        <v>5</v>
+      </c>
+      <c r="BA628" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB628" s="5">
+        <v>3</v>
+      </c>
+      <c r="BC628" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD628" s="5">
+        <v>2</v>
+      </c>
+      <c r="BE628" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF628" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG628" s="5">
+        <v>5</v>
+      </c>
+      <c r="BH628" s="5">
+        <v>3</v>
+      </c>
+      <c r="BI628" s="5">
+        <v>1</v>
+      </c>
+      <c r="BJ628" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK628" s="5">
+        <v>3</v>
+      </c>
+      <c r="BL628" s="5">
+        <v>5</v>
+      </c>
+      <c r="BM628" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="629" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A629" s="8">
+        <v>45599.720533437503</v>
+      </c>
+      <c r="B629" s="9" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C629" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D629" s="9">
+        <v>20192737</v>
+      </c>
+      <c r="E629" s="9" t="s">
+        <v>1412</v>
+      </c>
+      <c r="F629" s="10">
+        <v>0.71805555555329192</v>
+      </c>
+      <c r="G629" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H629" s="9">
+        <v>2</v>
+      </c>
+      <c r="I629" s="9">
+        <v>2</v>
+      </c>
+      <c r="J629" s="9">
+        <v>4</v>
+      </c>
+      <c r="K629" s="9">
+        <v>3</v>
+      </c>
+      <c r="L629" s="9">
+        <v>4</v>
+      </c>
+      <c r="M629" s="9">
+        <v>1</v>
+      </c>
+      <c r="N629" s="9">
+        <v>4</v>
+      </c>
+      <c r="O629" s="9">
+        <v>4</v>
+      </c>
+      <c r="P629" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q629" s="9">
+        <v>2</v>
+      </c>
+      <c r="R629" s="9">
+        <v>4</v>
+      </c>
+      <c r="S629" s="9">
+        <v>4</v>
+      </c>
+      <c r="T629" s="9">
+        <v>2</v>
+      </c>
+      <c r="U629" s="9">
+        <v>2</v>
+      </c>
+      <c r="V629" s="9">
+        <v>5</v>
+      </c>
+      <c r="W629" s="9">
+        <v>5</v>
+      </c>
+      <c r="X629" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y629" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z629" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA629" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB629" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC629" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD629" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE629" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF629" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG629" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH629" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI629" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ629" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="630" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A630" s="4">
+        <v>45599.721806111113</v>
+      </c>
+      <c r="B630" s="5" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C630" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D630" s="5">
+        <v>20242625</v>
+      </c>
+      <c r="E630" s="5" t="s">
+        <v>1414</v>
+      </c>
+      <c r="F630" s="6">
+        <v>0.71875</v>
+      </c>
+      <c r="G630" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H630" s="5">
+        <v>4</v>
+      </c>
+      <c r="I630" s="5">
+        <v>2</v>
+      </c>
+      <c r="J630" s="5">
+        <v>3</v>
+      </c>
+      <c r="K630" s="5">
+        <v>2</v>
+      </c>
+      <c r="L630" s="5">
+        <v>5</v>
+      </c>
+      <c r="M630" s="5">
+        <v>3</v>
+      </c>
+      <c r="N630" s="5">
+        <v>2</v>
+      </c>
+      <c r="O630" s="5">
+        <v>4</v>
+      </c>
+      <c r="P630" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q630" s="5">
+        <v>5</v>
+      </c>
+      <c r="R630" s="5">
+        <v>4</v>
+      </c>
+      <c r="S630" s="5">
+        <v>2</v>
+      </c>
+      <c r="T630" s="5">
+        <v>4</v>
+      </c>
+      <c r="U630" s="5">
+        <v>2</v>
+      </c>
+      <c r="V630" s="5">
+        <v>2</v>
+      </c>
+      <c r="W630" s="5">
+        <v>4</v>
+      </c>
+      <c r="X630" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y630" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z630" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA630" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB630" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC630" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD630" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE630" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF630" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG630" s="5">
+        <v>2</v>
+      </c>
+      <c r="AH630" s="5">
+        <v>4</v>
+      </c>
+      <c r="AI630" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ630" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="631" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A631" s="8">
+        <v>45599.735444930557</v>
+      </c>
+      <c r="B631" s="9" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C631" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="D631" s="9">
+        <v>20233544</v>
+      </c>
+      <c r="E631" s="9" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F631" s="10">
+        <v>0.72986111111094942</v>
+      </c>
+      <c r="G631" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H631" s="9">
+        <v>3</v>
+      </c>
+      <c r="I631" s="9">
+        <v>4</v>
+      </c>
+      <c r="J631" s="9">
+        <v>4</v>
+      </c>
+      <c r="K631" s="9">
+        <v>4</v>
+      </c>
+      <c r="L631" s="9">
+        <v>2</v>
+      </c>
+      <c r="M631" s="9">
+        <v>3</v>
+      </c>
+      <c r="N631" s="9">
+        <v>4</v>
+      </c>
+      <c r="O631" s="9">
+        <v>3</v>
+      </c>
+      <c r="P631" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q631" s="9">
+        <v>3</v>
+      </c>
+      <c r="R631" s="9">
+        <v>5</v>
+      </c>
+      <c r="S631" s="9">
+        <v>4</v>
+      </c>
+      <c r="T631" s="9">
+        <v>3</v>
+      </c>
+      <c r="U631" s="9">
+        <v>4</v>
+      </c>
+      <c r="V631" s="9">
+        <v>4</v>
+      </c>
+      <c r="W631" s="9">
+        <v>5</v>
+      </c>
+      <c r="X631" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y631" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z631" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA631" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB631" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC631" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD631" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE631" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF631" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG631" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH631" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI631" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ631" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="632" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A632" s="4">
+        <v>45599.740281886574</v>
+      </c>
+      <c r="B632" s="5" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C632" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="D632" s="5">
+        <v>20222933</v>
+      </c>
+      <c r="E632" s="5" t="s">
+        <v>1418</v>
+      </c>
+      <c r="F632" s="6">
+        <v>0.73958333333575865</v>
+      </c>
+      <c r="G632" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK632" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL632" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM632" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN632" s="5">
+        <v>4</v>
+      </c>
+      <c r="AO632" s="5">
+        <v>3</v>
+      </c>
+      <c r="AP632" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ632" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR632" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS632" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT632" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU632" s="5">
+        <v>3</v>
+      </c>
+      <c r="AV632" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW632" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX632" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY632" s="5">
+        <v>4</v>
+      </c>
+      <c r="AZ632" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA632" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB632" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC632" s="5">
+        <v>4</v>
+      </c>
+      <c r="BD632" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE632" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF632" s="5">
+        <v>3</v>
+      </c>
+      <c r="BG632" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH632" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI632" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ632" s="5">
+        <v>4</v>
+      </c>
+      <c r="BK632" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL632" s="5">
+        <v>4</v>
+      </c>
+      <c r="BM632" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="633" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A633" s="8">
+        <v>45599.740642256947</v>
+      </c>
+      <c r="B633" s="9" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C633" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="D633" s="9">
+        <v>20241728</v>
+      </c>
+      <c r="E633" s="9" t="s">
+        <v>1420</v>
+      </c>
+      <c r="F633" s="10">
+        <v>0.73194444444379769</v>
+      </c>
+      <c r="G633" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H633" s="9">
+        <v>1</v>
+      </c>
+      <c r="I633" s="9">
+        <v>4</v>
+      </c>
+      <c r="J633" s="9">
+        <v>4</v>
+      </c>
+      <c r="K633" s="9">
+        <v>4</v>
+      </c>
+      <c r="L633" s="9">
+        <v>4</v>
+      </c>
+      <c r="M633" s="9">
+        <v>3</v>
+      </c>
+      <c r="N633" s="9">
+        <v>3</v>
+      </c>
+      <c r="O633" s="9">
+        <v>4</v>
+      </c>
+      <c r="P633" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q633" s="9">
+        <v>3</v>
+      </c>
+      <c r="R633" s="9">
+        <v>5</v>
+      </c>
+      <c r="S633" s="9">
+        <v>5</v>
+      </c>
+      <c r="T633" s="9">
+        <v>2</v>
+      </c>
+      <c r="U633" s="9">
+        <v>2</v>
+      </c>
+      <c r="V633" s="9">
+        <v>3</v>
+      </c>
+      <c r="W633" s="9">
+        <v>6</v>
+      </c>
+      <c r="X633" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y633" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z633" s="9">
+        <v>5</v>
+      </c>
+      <c r="AA633" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB633" s="9">
+        <v>2</v>
+      </c>
+      <c r="AC633" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD633" s="9">
+        <v>5</v>
+      </c>
+      <c r="AE633" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF633" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG633" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH633" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI633" s="9">
+        <v>5</v>
+      </c>
+      <c r="AJ633" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="634" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A634" s="4">
+        <v>45599.742659039352</v>
+      </c>
+      <c r="B634" s="5" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C634" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D634" s="5">
+        <v>20215212</v>
+      </c>
+      <c r="E634" s="5" t="s">
+        <v>1422</v>
+      </c>
+      <c r="F634" s="6">
+        <v>0.74166666666860692</v>
+      </c>
+      <c r="G634" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AL634" s="5">
+        <v>4</v>
+      </c>
+      <c r="AM634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP634" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR634" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AU634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV634" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AX634" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY634" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BA634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB634" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BD634" s="5">
+        <v>4</v>
+      </c>
+      <c r="BE634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BH634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BI634" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BL634" s="5">
+        <v>5</v>
+      </c>
+      <c r="BM634" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="635" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A635" s="8">
+        <v>45599.743192256945</v>
+      </c>
+      <c r="B635" s="9" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C635" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D635" s="9">
+        <v>20246289</v>
+      </c>
+      <c r="E635" s="9" t="s">
+        <v>1424</v>
+      </c>
+      <c r="F635" s="10">
+        <v>0.7381944444423425</v>
+      </c>
+      <c r="G635" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H635" s="9">
+        <v>4</v>
+      </c>
+      <c r="I635" s="9">
+        <v>3</v>
+      </c>
+      <c r="J635" s="9">
+        <v>3</v>
+      </c>
+      <c r="K635" s="9">
+        <v>4</v>
+      </c>
+      <c r="L635" s="9">
+        <v>2</v>
+      </c>
+      <c r="M635" s="9">
+        <v>4</v>
+      </c>
+      <c r="N635" s="9">
+        <v>4</v>
+      </c>
+      <c r="O635" s="9">
+        <v>3</v>
+      </c>
+      <c r="P635" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q635" s="9">
+        <v>3</v>
+      </c>
+      <c r="R635" s="9">
+        <v>4</v>
+      </c>
+      <c r="S635" s="9">
+        <v>3</v>
+      </c>
+      <c r="T635" s="9">
+        <v>2</v>
+      </c>
+      <c r="U635" s="9">
+        <v>3</v>
+      </c>
+      <c r="V635" s="9">
+        <v>4</v>
+      </c>
+      <c r="W635" s="9">
+        <v>3</v>
+      </c>
+      <c r="X635" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y635" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z635" s="9">
+        <v>5</v>
+      </c>
+      <c r="AA635" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB635" s="9">
+        <v>5</v>
+      </c>
+      <c r="AC635" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD635" s="9">
+        <v>2</v>
+      </c>
+      <c r="AE635" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF635" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG635" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH635" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI635" s="9">
+        <v>4</v>
+      </c>
+      <c r="AJ635" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="636" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A636" s="4">
+        <v>45599.746400405093</v>
+      </c>
+      <c r="B636" s="5" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C636" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="D636" s="5">
+        <v>20246909</v>
+      </c>
+      <c r="E636" s="5" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F636" s="6">
+        <v>0.74444444444088731</v>
+      </c>
+      <c r="G636" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H636" s="5">
+        <v>2</v>
+      </c>
+      <c r="I636" s="5">
+        <v>6</v>
+      </c>
+      <c r="J636" s="5">
+        <v>2</v>
+      </c>
+      <c r="K636" s="5">
+        <v>2</v>
+      </c>
+      <c r="L636" s="5">
+        <v>1</v>
+      </c>
+      <c r="M636" s="5">
+        <v>5</v>
+      </c>
+      <c r="N636" s="5">
+        <v>3</v>
+      </c>
+      <c r="O636" s="5">
+        <v>5</v>
+      </c>
+      <c r="P636" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q636" s="5">
+        <v>2</v>
+      </c>
+      <c r="R636" s="5">
+        <v>2</v>
+      </c>
+      <c r="S636" s="5">
+        <v>2</v>
+      </c>
+      <c r="T636" s="5">
+        <v>2</v>
+      </c>
+      <c r="U636" s="5">
+        <v>2</v>
+      </c>
+      <c r="V636" s="5">
+        <v>2</v>
+      </c>
+      <c r="W636" s="5">
+        <v>2</v>
+      </c>
+      <c r="X636" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y636" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z636" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA636" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB636" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC636" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD636" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE636" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF636" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG636" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH636" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI636" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ636" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="637" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A637" s="8">
+        <v>45599.747711643518</v>
+      </c>
+      <c r="B637" s="9" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C637" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D637" s="9">
+        <v>20246640</v>
+      </c>
+      <c r="E637" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="F637" s="10">
+        <v>0.74513888888759539</v>
+      </c>
+      <c r="G637" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK637" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL637" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM637" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN637" s="9">
+        <v>2</v>
+      </c>
+      <c r="AO637" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP637" s="9">
+        <v>1</v>
+      </c>
+      <c r="AQ637" s="9">
+        <v>4</v>
+      </c>
+      <c r="AR637" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS637" s="9">
+        <v>6</v>
+      </c>
+      <c r="AT637" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU637" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV637" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW637" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX637" s="9">
+        <v>4</v>
+      </c>
+      <c r="AY637" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ637" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA637" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB637" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC637" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD637" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE637" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF637" s="9">
+        <v>5</v>
+      </c>
+      <c r="BG637" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH637" s="9">
+        <v>1</v>
+      </c>
+      <c r="BI637" s="9">
+        <v>5</v>
+      </c>
+      <c r="BJ637" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK637" s="9">
+        <v>5</v>
+      </c>
+      <c r="BL637" s="9">
+        <v>4</v>
+      </c>
+      <c r="BM637" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="638" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A638" s="4">
+        <v>45599.753833472219</v>
+      </c>
+      <c r="B638" s="5" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C638" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="D638" s="5">
+        <v>202043359</v>
+      </c>
+      <c r="E638" s="5" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F638" s="6">
+        <v>0.75277777777955635</v>
+      </c>
+      <c r="G638" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK638" s="5">
+        <v>4</v>
+      </c>
+      <c r="AL638" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM638" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN638" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO638" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP638" s="5">
+        <v>3</v>
+      </c>
+      <c r="AQ638" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR638" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS638" s="5">
+        <v>3</v>
+      </c>
+      <c r="AT638" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU638" s="5">
+        <v>4</v>
+      </c>
+      <c r="AV638" s="5">
+        <v>4</v>
+      </c>
+      <c r="AW638" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX638" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY638" s="5">
+        <v>4</v>
+      </c>
+      <c r="AZ638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BB638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BC638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BD638" s="5">
+        <v>3</v>
+      </c>
+      <c r="BE638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BF638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH638" s="5">
+        <v>3</v>
+      </c>
+      <c r="BI638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BJ638" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BL638" s="5">
+        <v>4</v>
+      </c>
+      <c r="BM638" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="639" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A639" s="8">
+        <v>45599.755587141204</v>
+      </c>
+      <c r="B639" s="9" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C639" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D639" s="9">
+        <v>20172433</v>
+      </c>
+      <c r="E639" s="9" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F639" s="10">
+        <v>0.75208333333284827</v>
+      </c>
+      <c r="G639" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY639" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL639" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM639" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="640" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A640" s="4">
+        <v>45599.757533020835</v>
+      </c>
+      <c r="B640" s="5" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C640" s="5" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D640" s="5">
+        <v>20236736</v>
+      </c>
+      <c r="E640" s="5" t="s">
+        <v>1434</v>
+      </c>
+      <c r="F640" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="G640" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK640" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL640" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM640" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN640" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO640" s="5">
+        <v>2</v>
+      </c>
+      <c r="AP640" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ640" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR640" s="5">
+        <v>4</v>
+      </c>
+      <c r="AS640" s="5">
+        <v>6</v>
+      </c>
+      <c r="AT640" s="5">
+        <v>2</v>
+      </c>
+      <c r="AU640" s="5">
+        <v>5</v>
+      </c>
+      <c r="AV640" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW640" s="5">
+        <v>2</v>
+      </c>
+      <c r="AX640" s="5">
+        <v>2</v>
+      </c>
+      <c r="AY640" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ640" s="5">
+        <v>5</v>
+      </c>
+      <c r="BA640" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB640" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC640" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD640" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE640" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF640" s="5">
+        <v>5</v>
+      </c>
+      <c r="BG640" s="5">
+        <v>2</v>
+      </c>
+      <c r="BH640" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI640" s="5">
+        <v>2</v>
+      </c>
+      <c r="BJ640" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK640" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL640" s="5">
+        <v>2</v>
+      </c>
+      <c r="BM640" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="641" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A641" s="8">
+        <v>45599.762176111108</v>
+      </c>
+      <c r="B641" s="9" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C641" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D641" s="9">
+        <v>20243951</v>
+      </c>
+      <c r="E641" s="9" t="s">
+        <v>1436</v>
+      </c>
+      <c r="F641" s="10">
+        <v>0.76041666666424135</v>
+      </c>
+      <c r="G641" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H641" s="9">
+        <v>2</v>
+      </c>
+      <c r="I641" s="9">
+        <v>4</v>
+      </c>
+      <c r="J641" s="9">
+        <v>5</v>
+      </c>
+      <c r="K641" s="9">
+        <v>5</v>
+      </c>
+      <c r="L641" s="9">
+        <v>3</v>
+      </c>
+      <c r="M641" s="9">
+        <v>2</v>
+      </c>
+      <c r="N641" s="9">
+        <v>5</v>
+      </c>
+      <c r="O641" s="9">
+        <v>3</v>
+      </c>
+      <c r="P641" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q641" s="9">
+        <v>2</v>
+      </c>
+      <c r="R641" s="9">
+        <v>5</v>
+      </c>
+      <c r="S641" s="9">
+        <v>3</v>
+      </c>
+      <c r="T641" s="9">
+        <v>5</v>
+      </c>
+      <c r="U641" s="9">
+        <v>4</v>
+      </c>
+      <c r="V641" s="9">
+        <v>5</v>
+      </c>
+      <c r="W641" s="9">
+        <v>5</v>
+      </c>
+      <c r="X641" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y641" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z641" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA641" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB641" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC641" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD641" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE641" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF641" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG641" s="9">
+        <v>4</v>
+      </c>
+      <c r="AH641" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI641" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ641" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="642" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A642" s="4">
+        <v>45599.763537152779</v>
+      </c>
+      <c r="B642" s="5" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C642" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D642" s="5">
+        <v>20243622</v>
+      </c>
+      <c r="E642" s="5" t="s">
+        <v>1438</v>
+      </c>
+      <c r="F642" s="6">
+        <v>0.75694444444525288</v>
+      </c>
+      <c r="G642" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H642" s="5">
+        <v>2</v>
+      </c>
+      <c r="I642" s="5">
+        <v>4</v>
+      </c>
+      <c r="J642" s="5">
+        <v>4</v>
+      </c>
+      <c r="K642" s="5">
+        <v>3</v>
+      </c>
+      <c r="L642" s="5">
+        <v>3</v>
+      </c>
+      <c r="M642" s="5">
+        <v>4</v>
+      </c>
+      <c r="N642" s="5">
+        <v>3</v>
+      </c>
+      <c r="O642" s="5">
+        <v>2</v>
+      </c>
+      <c r="P642" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q642" s="5">
+        <v>2</v>
+      </c>
+      <c r="R642" s="5">
+        <v>4</v>
+      </c>
+      <c r="S642" s="5">
+        <v>5</v>
+      </c>
+      <c r="T642" s="5">
+        <v>2</v>
+      </c>
+      <c r="U642" s="5">
+        <v>2</v>
+      </c>
+      <c r="V642" s="5">
+        <v>5</v>
+      </c>
+      <c r="W642" s="5">
+        <v>5</v>
+      </c>
+      <c r="X642" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y642" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z642" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA642" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB642" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC642" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD642" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE642" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF642" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG642" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH642" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI642" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ642" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="643" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A643" s="8">
+        <v>45599.763545925925</v>
+      </c>
+      <c r="B643" s="9" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C643" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D643" s="9">
+        <v>20232210</v>
+      </c>
+      <c r="E643" s="9" t="s">
+        <v>1440</v>
+      </c>
+      <c r="F643" s="10">
+        <v>0.76249999999708962</v>
+      </c>
+      <c r="G643" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AL643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AT643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AW643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AX643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY643" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BB643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BE643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL643" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM643" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="644" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A644" s="15">
+        <v>45599.765390011569</v>
+      </c>
+      <c r="B644" s="16" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C644" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D644" s="16">
+        <v>20217096</v>
+      </c>
+      <c r="E644" s="16" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F644" s="17">
+        <v>0.76458333333721384</v>
+      </c>
+      <c r="G644" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H644" s="26"/>
+      <c r="I644" s="26"/>
+      <c r="J644" s="26"/>
+      <c r="K644" s="26"/>
+      <c r="L644" s="26"/>
+      <c r="M644" s="26"/>
+      <c r="N644" s="26"/>
+      <c r="O644" s="26"/>
+      <c r="P644" s="26"/>
+      <c r="Q644" s="26"/>
+      <c r="R644" s="26"/>
+      <c r="S644" s="26"/>
+      <c r="T644" s="26"/>
+      <c r="U644" s="26"/>
+      <c r="V644" s="26"/>
+      <c r="W644" s="26"/>
+      <c r="X644" s="26"/>
+      <c r="Y644" s="26"/>
+      <c r="Z644" s="26"/>
+      <c r="AA644" s="26"/>
+      <c r="AB644" s="26"/>
+      <c r="AC644" s="26"/>
+      <c r="AD644" s="26"/>
+      <c r="AE644" s="26"/>
+      <c r="AF644" s="26"/>
+      <c r="AG644" s="26"/>
+      <c r="AH644" s="26"/>
+      <c r="AI644" s="26"/>
+      <c r="AJ644" s="26"/>
+      <c r="AK644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AL644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AM644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AN644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AO644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AP644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AQ644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AR644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AS644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AT644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AU644" s="16">
+        <v>5</v>
+      </c>
+      <c r="AV644" s="16">
+        <v>5</v>
+      </c>
+      <c r="AW644" s="16">
+        <v>5</v>
+      </c>
+      <c r="AX644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AY644" s="16">
+        <v>3</v>
+      </c>
+      <c r="AZ644" s="16">
+        <v>3</v>
+      </c>
+      <c r="BA644" s="16">
+        <v>4</v>
+      </c>
+      <c r="BB644" s="16">
+        <v>3</v>
+      </c>
+      <c r="BC644" s="16">
+        <v>4</v>
+      </c>
+      <c r="BD644" s="16">
+        <v>3</v>
+      </c>
+      <c r="BE644" s="16">
+        <v>3</v>
+      </c>
+      <c r="BF644" s="16">
+        <v>4</v>
+      </c>
+      <c r="BG644" s="16">
+        <v>3</v>
+      </c>
+      <c r="BH644" s="16">
+        <v>3</v>
+      </c>
+      <c r="BI644" s="16">
+        <v>4</v>
+      </c>
+      <c r="BJ644" s="16">
+        <v>3</v>
+      </c>
+      <c r="BK644" s="16">
+        <v>3</v>
+      </c>
+      <c r="BL644" s="16">
+        <v>3</v>
+      </c>
+      <c r="BM644" s="21">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
241021, oxford modified sunday 19:40
</commit_message>
<xml_diff>
--- a/R/data/oxford_241021.xlsx
+++ b/R/data/oxford_241021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Dropbox/내 Mac (Kee-Won의 MacBook Air)/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC0840B-FAD4-0D43-AE20-C04CE2B60FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F46DF6-F843-BF4D-AC58-D975DD1D362F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42920" yWindow="1420" windowWidth="37080" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="1442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2751" uniqueCount="1501">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -4349,6 +4349,183 @@
   </si>
   <si>
     <t>20217096@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>rlatldbs124@naver.com</t>
+  </si>
+  <si>
+    <t>김시윤</t>
+  </si>
+  <si>
+    <t>saycom816@gmail.com</t>
+  </si>
+  <si>
+    <t>김영빈</t>
+  </si>
+  <si>
+    <t>skyflight0656@gmail.com</t>
+  </si>
+  <si>
+    <t>한충서</t>
+  </si>
+  <si>
+    <t>dhpark25678@naver.com</t>
+  </si>
+  <si>
+    <t>박도현</t>
+  </si>
+  <si>
+    <t>lgc01040089921@gmail.com</t>
+  </si>
+  <si>
+    <t>이감찬</t>
+  </si>
+  <si>
+    <t>kimw0707@naver.com</t>
+  </si>
+  <si>
+    <t>김원영</t>
+  </si>
+  <si>
+    <t>20182346@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>이용재</t>
+  </si>
+  <si>
+    <t>osmokroyal1@gmail.com</t>
+  </si>
+  <si>
+    <t>오성민</t>
+  </si>
+  <si>
+    <t>kmu2916@naver.com</t>
+  </si>
+  <si>
+    <t>강민욱</t>
+  </si>
+  <si>
+    <t>hshljy7@gmail.com</t>
+  </si>
+  <si>
+    <t>디지털 미디어 콘텐츠</t>
+  </si>
+  <si>
+    <t>황성훈</t>
+  </si>
+  <si>
+    <t>bcy1976@naver.com</t>
+  </si>
+  <si>
+    <t>변치윤</t>
+  </si>
+  <si>
+    <t>20235263@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>wjswlals789@naver.com</t>
+  </si>
+  <si>
+    <t>전지민</t>
+  </si>
+  <si>
+    <t>yeonh990@naver.com</t>
+  </si>
+  <si>
+    <t>언어병리학전공</t>
+  </si>
+  <si>
+    <t>박현아</t>
+  </si>
+  <si>
+    <t>jseunghun411@gmail.com</t>
+  </si>
+  <si>
+    <t>정성훈</t>
+  </si>
+  <si>
+    <t>bottom0406@gmail.com</t>
+  </si>
+  <si>
+    <t>박문형</t>
+  </si>
+  <si>
+    <t>junyeong@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>소프트웨어</t>
+  </si>
+  <si>
+    <t>박준영</t>
+  </si>
+  <si>
+    <t>hose0303@gmail.com</t>
+  </si>
+  <si>
+    <t>유정현</t>
+  </si>
+  <si>
+    <t>a01091830132@gmail.com</t>
+  </si>
+  <si>
+    <t>황유민</t>
+  </si>
+  <si>
+    <t>wlghd2352@naver.com</t>
+  </si>
+  <si>
+    <t>안지홍</t>
+  </si>
+  <si>
+    <t>wpghks1145@gmail.com</t>
+  </si>
+  <si>
+    <t>박제환</t>
+  </si>
+  <si>
+    <t>1202kge@naver.com</t>
+  </si>
+  <si>
+    <t>김가은</t>
+  </si>
+  <si>
+    <t>haeun_ob@naver.com</t>
+  </si>
+  <si>
+    <t>박하은</t>
+  </si>
+  <si>
+    <t>eunsoljj@naver.com</t>
+  </si>
+  <si>
+    <t>권은솔</t>
+  </si>
+  <si>
+    <t>skaskgus@gmail.com</t>
+  </si>
+  <si>
+    <t>남나현</t>
+  </si>
+  <si>
+    <t>jongjongsook@naver.com</t>
+  </si>
+  <si>
+    <t>김종숙</t>
+  </si>
+  <si>
+    <t>mkjk1227@naver.com</t>
+  </si>
+  <si>
+    <t>정민기</t>
+  </si>
+  <si>
+    <t>coreykang3@naver.com</t>
+  </si>
+  <si>
+    <t>반도체공학</t>
+  </si>
+  <si>
+    <t>강동훈</t>
   </si>
 </sst>
 </file>
@@ -4792,7 +4969,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM644">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:BM673">
   <tableColumns count="65">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="타임스탬프"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="이메일 주소"/>
@@ -5065,11 +5242,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM644"/>
+  <dimension ref="A1:BM673"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A613" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G650" sqref="G650"/>
+      <pane ySplit="1" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D678" sqref="D678"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -76813,35 +76990,6 @@
       <c r="G644" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H644" s="26"/>
-      <c r="I644" s="26"/>
-      <c r="J644" s="26"/>
-      <c r="K644" s="26"/>
-      <c r="L644" s="26"/>
-      <c r="M644" s="26"/>
-      <c r="N644" s="26"/>
-      <c r="O644" s="26"/>
-      <c r="P644" s="26"/>
-      <c r="Q644" s="26"/>
-      <c r="R644" s="26"/>
-      <c r="S644" s="26"/>
-      <c r="T644" s="26"/>
-      <c r="U644" s="26"/>
-      <c r="V644" s="26"/>
-      <c r="W644" s="26"/>
-      <c r="X644" s="26"/>
-      <c r="Y644" s="26"/>
-      <c r="Z644" s="26"/>
-      <c r="AA644" s="26"/>
-      <c r="AB644" s="26"/>
-      <c r="AC644" s="26"/>
-      <c r="AD644" s="26"/>
-      <c r="AE644" s="26"/>
-      <c r="AF644" s="26"/>
-      <c r="AG644" s="26"/>
-      <c r="AH644" s="26"/>
-      <c r="AI644" s="26"/>
-      <c r="AJ644" s="26"/>
       <c r="AK644" s="16">
         <v>3</v>
       </c>
@@ -76927,6 +77075,3225 @@
         <v>3</v>
       </c>
       <c r="BM644" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="645" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A645" s="8">
+        <v>45599.769991863424</v>
+      </c>
+      <c r="B645" s="9" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C645" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D645" s="9">
+        <v>20203807</v>
+      </c>
+      <c r="E645" s="9" t="s">
+        <v>1443</v>
+      </c>
+      <c r="F645" s="10">
+        <v>0.76736111110949423</v>
+      </c>
+      <c r="G645" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK645" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL645" s="9">
+        <v>4</v>
+      </c>
+      <c r="AM645" s="9">
+        <v>2</v>
+      </c>
+      <c r="AN645" s="9">
+        <v>2</v>
+      </c>
+      <c r="AO645" s="9">
+        <v>2</v>
+      </c>
+      <c r="AP645" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ645" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR645" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS645" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT645" s="9">
+        <v>4</v>
+      </c>
+      <c r="AU645" s="9">
+        <v>3</v>
+      </c>
+      <c r="AV645" s="9">
+        <v>2</v>
+      </c>
+      <c r="AW645" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX645" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY645" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ645" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA645" s="9">
+        <v>2</v>
+      </c>
+      <c r="BB645" s="9">
+        <v>3</v>
+      </c>
+      <c r="BC645" s="9">
+        <v>3</v>
+      </c>
+      <c r="BD645" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE645" s="9">
+        <v>4</v>
+      </c>
+      <c r="BF645" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG645" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH645" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI645" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ645" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK645" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL645" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM645" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="646" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A646" s="4">
+        <v>45599.771998854165</v>
+      </c>
+      <c r="B646" s="5" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C646" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D646" s="5">
+        <v>20242930</v>
+      </c>
+      <c r="E646" s="5" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F646" s="6">
+        <v>0.7694444444423425</v>
+      </c>
+      <c r="G646" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H646" s="5">
+        <v>3</v>
+      </c>
+      <c r="I646" s="5">
+        <v>2</v>
+      </c>
+      <c r="J646" s="5">
+        <v>3</v>
+      </c>
+      <c r="K646" s="5">
+        <v>3</v>
+      </c>
+      <c r="L646" s="5">
+        <v>3</v>
+      </c>
+      <c r="M646" s="5">
+        <v>1</v>
+      </c>
+      <c r="N646" s="5">
+        <v>3</v>
+      </c>
+      <c r="O646" s="5">
+        <v>5</v>
+      </c>
+      <c r="P646" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q646" s="5">
+        <v>3</v>
+      </c>
+      <c r="R646" s="5">
+        <v>4</v>
+      </c>
+      <c r="S646" s="5">
+        <v>3</v>
+      </c>
+      <c r="T646" s="5">
+        <v>1</v>
+      </c>
+      <c r="U646" s="5">
+        <v>5</v>
+      </c>
+      <c r="V646" s="5">
+        <v>4</v>
+      </c>
+      <c r="W646" s="5">
+        <v>4</v>
+      </c>
+      <c r="X646" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y646" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z646" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA646" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB646" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC646" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD646" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE646" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF646" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG646" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH646" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI646" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ646" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="647" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A647" s="8">
+        <v>45599.780275162033</v>
+      </c>
+      <c r="B647" s="9" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C647" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D647" s="9">
+        <v>20215269</v>
+      </c>
+      <c r="E647" s="9" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F647" s="10">
+        <v>0.77847222222044365</v>
+      </c>
+      <c r="G647" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H647" s="9">
+        <v>2</v>
+      </c>
+      <c r="I647" s="9">
+        <v>4</v>
+      </c>
+      <c r="J647" s="9">
+        <v>4</v>
+      </c>
+      <c r="K647" s="9">
+        <v>4</v>
+      </c>
+      <c r="L647" s="9">
+        <v>2</v>
+      </c>
+      <c r="M647" s="9">
+        <v>2</v>
+      </c>
+      <c r="N647" s="9">
+        <v>5</v>
+      </c>
+      <c r="O647" s="9">
+        <v>5</v>
+      </c>
+      <c r="P647" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q647" s="9">
+        <v>2</v>
+      </c>
+      <c r="R647" s="9">
+        <v>5</v>
+      </c>
+      <c r="S647" s="9">
+        <v>5</v>
+      </c>
+      <c r="T647" s="9">
+        <v>2</v>
+      </c>
+      <c r="U647" s="9">
+        <v>2</v>
+      </c>
+      <c r="V647" s="9">
+        <v>5</v>
+      </c>
+      <c r="W647" s="9">
+        <v>5</v>
+      </c>
+      <c r="X647" s="9">
+        <v>5</v>
+      </c>
+      <c r="Y647" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z647" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA647" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB647" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC647" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD647" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE647" s="9">
+        <v>2</v>
+      </c>
+      <c r="AF647" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG647" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH647" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI647" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ647" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="648" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A648" s="4">
+        <v>45599.782656840282</v>
+      </c>
+      <c r="B648" s="5" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C648" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D648" s="5">
+        <v>20223224</v>
+      </c>
+      <c r="E648" s="5" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F648" s="6">
+        <v>0.78194444444670808</v>
+      </c>
+      <c r="G648" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H648" s="5">
+        <v>1</v>
+      </c>
+      <c r="I648" s="5">
+        <v>2</v>
+      </c>
+      <c r="J648" s="5">
+        <v>2</v>
+      </c>
+      <c r="K648" s="5">
+        <v>2</v>
+      </c>
+      <c r="L648" s="5">
+        <v>2</v>
+      </c>
+      <c r="M648" s="5">
+        <v>3</v>
+      </c>
+      <c r="N648" s="5">
+        <v>3</v>
+      </c>
+      <c r="O648" s="5">
+        <v>3</v>
+      </c>
+      <c r="P648" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q648" s="5">
+        <v>3</v>
+      </c>
+      <c r="R648" s="5">
+        <v>3</v>
+      </c>
+      <c r="S648" s="5">
+        <v>3</v>
+      </c>
+      <c r="T648" s="5">
+        <v>3</v>
+      </c>
+      <c r="U648" s="5">
+        <v>2</v>
+      </c>
+      <c r="V648" s="5">
+        <v>2</v>
+      </c>
+      <c r="W648" s="5">
+        <v>2</v>
+      </c>
+      <c r="X648" s="5">
+        <v>2</v>
+      </c>
+      <c r="Y648" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z648" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA648" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB648" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC648" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD648" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE648" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF648" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG648" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH648" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI648" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ648" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="649" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A649" s="8">
+        <v>45599.787776354162</v>
+      </c>
+      <c r="B649" s="9" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C649" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D649" s="9">
+        <v>20242995</v>
+      </c>
+      <c r="E649" s="9" t="s">
+        <v>1451</v>
+      </c>
+      <c r="F649" s="10">
+        <v>0.78611111111240461</v>
+      </c>
+      <c r="G649" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H649" s="9">
+        <v>2</v>
+      </c>
+      <c r="I649" s="9">
+        <v>5</v>
+      </c>
+      <c r="J649" s="9">
+        <v>6</v>
+      </c>
+      <c r="K649" s="9">
+        <v>5</v>
+      </c>
+      <c r="L649" s="9">
+        <v>1</v>
+      </c>
+      <c r="M649" s="9">
+        <v>1</v>
+      </c>
+      <c r="N649" s="9">
+        <v>3</v>
+      </c>
+      <c r="O649" s="9">
+        <v>2</v>
+      </c>
+      <c r="P649" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q649" s="9">
+        <v>1</v>
+      </c>
+      <c r="R649" s="9">
+        <v>2</v>
+      </c>
+      <c r="S649" s="9">
+        <v>1</v>
+      </c>
+      <c r="T649" s="9">
+        <v>2</v>
+      </c>
+      <c r="U649" s="9">
+        <v>2</v>
+      </c>
+      <c r="V649" s="9">
+        <v>3</v>
+      </c>
+      <c r="W649" s="9">
+        <v>3</v>
+      </c>
+      <c r="X649" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y649" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z649" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA649" s="9">
+        <v>2</v>
+      </c>
+      <c r="AB649" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC649" s="9">
+        <v>2</v>
+      </c>
+      <c r="AD649" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE649" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF649" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG649" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH649" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI649" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ649" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="650" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A650" s="4">
+        <v>45599.789923993056</v>
+      </c>
+      <c r="B650" s="5" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C650" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D650" s="5">
+        <v>20245138</v>
+      </c>
+      <c r="E650" s="5" t="s">
+        <v>1453</v>
+      </c>
+      <c r="F650" s="6">
+        <v>0.78611111111240461</v>
+      </c>
+      <c r="G650" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H650" s="5">
+        <v>1</v>
+      </c>
+      <c r="I650" s="5">
+        <v>5</v>
+      </c>
+      <c r="J650" s="5">
+        <v>5</v>
+      </c>
+      <c r="K650" s="5">
+        <v>4</v>
+      </c>
+      <c r="L650" s="5">
+        <v>2</v>
+      </c>
+      <c r="M650" s="5">
+        <v>2</v>
+      </c>
+      <c r="N650" s="5">
+        <v>4</v>
+      </c>
+      <c r="O650" s="5">
+        <v>3</v>
+      </c>
+      <c r="P650" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q650" s="5">
+        <v>2</v>
+      </c>
+      <c r="R650" s="5">
+        <v>2</v>
+      </c>
+      <c r="S650" s="5">
+        <v>4</v>
+      </c>
+      <c r="T650" s="5">
+        <v>3</v>
+      </c>
+      <c r="U650" s="5">
+        <v>2</v>
+      </c>
+      <c r="V650" s="5">
+        <v>4</v>
+      </c>
+      <c r="W650" s="5">
+        <v>4</v>
+      </c>
+      <c r="X650" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y650" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z650" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA650" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB650" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC650" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD650" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE650" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF650" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG650" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH650" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI650" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ650" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="651" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A651" s="8">
+        <v>45599.793084050922</v>
+      </c>
+      <c r="B651" s="9" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C651" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="D651" s="9">
+        <v>20182346</v>
+      </c>
+      <c r="E651" s="9" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F651" s="10">
+        <v>0.79166666666424135</v>
+      </c>
+      <c r="G651" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H651" s="9">
+        <v>4</v>
+      </c>
+      <c r="I651" s="9">
+        <v>3</v>
+      </c>
+      <c r="J651" s="9">
+        <v>2</v>
+      </c>
+      <c r="K651" s="9">
+        <v>2</v>
+      </c>
+      <c r="L651" s="9">
+        <v>4</v>
+      </c>
+      <c r="M651" s="9">
+        <v>5</v>
+      </c>
+      <c r="N651" s="9">
+        <v>3</v>
+      </c>
+      <c r="O651" s="9">
+        <v>3</v>
+      </c>
+      <c r="P651" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q651" s="9">
+        <v>5</v>
+      </c>
+      <c r="R651" s="9">
+        <v>4</v>
+      </c>
+      <c r="S651" s="9">
+        <v>3</v>
+      </c>
+      <c r="T651" s="9">
+        <v>6</v>
+      </c>
+      <c r="U651" s="9">
+        <v>4</v>
+      </c>
+      <c r="V651" s="9">
+        <v>2</v>
+      </c>
+      <c r="W651" s="9">
+        <v>4</v>
+      </c>
+      <c r="X651" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y651" s="9">
+        <v>2</v>
+      </c>
+      <c r="Z651" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA651" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB651" s="9">
+        <v>2</v>
+      </c>
+      <c r="AC651" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD651" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE651" s="9">
+        <v>5</v>
+      </c>
+      <c r="AF651" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG651" s="9">
+        <v>2</v>
+      </c>
+      <c r="AH651" s="9">
+        <v>3</v>
+      </c>
+      <c r="AI651" s="9">
+        <v>5</v>
+      </c>
+      <c r="AJ651" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="652" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A652" s="4">
+        <v>45599.793304467588</v>
+      </c>
+      <c r="B652" s="5" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C652" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D652" s="5">
+        <v>20241526</v>
+      </c>
+      <c r="E652" s="5" t="s">
+        <v>1457</v>
+      </c>
+      <c r="F652" s="6">
+        <v>0.29166666666424135</v>
+      </c>
+      <c r="G652" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H652" s="5">
+        <v>2</v>
+      </c>
+      <c r="I652" s="5">
+        <v>2</v>
+      </c>
+      <c r="J652" s="5">
+        <v>5</v>
+      </c>
+      <c r="K652" s="5">
+        <v>2</v>
+      </c>
+      <c r="L652" s="5">
+        <v>4</v>
+      </c>
+      <c r="M652" s="5">
+        <v>3</v>
+      </c>
+      <c r="N652" s="5">
+        <v>4</v>
+      </c>
+      <c r="O652" s="5">
+        <v>5</v>
+      </c>
+      <c r="P652" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q652" s="5">
+        <v>5</v>
+      </c>
+      <c r="R652" s="5">
+        <v>5</v>
+      </c>
+      <c r="S652" s="5">
+        <v>4</v>
+      </c>
+      <c r="T652" s="5">
+        <v>2</v>
+      </c>
+      <c r="U652" s="5">
+        <v>3</v>
+      </c>
+      <c r="V652" s="5">
+        <v>5</v>
+      </c>
+      <c r="W652" s="5">
+        <v>5</v>
+      </c>
+      <c r="X652" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y652" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z652" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA652" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB652" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC652" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD652" s="5">
+        <v>5</v>
+      </c>
+      <c r="AE652" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF652" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG652" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH652" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI652" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ652" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="653" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A653" s="8">
+        <v>45599.79347469908</v>
+      </c>
+      <c r="B653" s="9" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C653" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D653" s="9">
+        <v>20222902</v>
+      </c>
+      <c r="E653" s="9" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F653" s="10">
+        <v>0.78958333333139308</v>
+      </c>
+      <c r="G653" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK653" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO653" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP653" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AR653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AS653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT653" s="9">
+        <v>1</v>
+      </c>
+      <c r="AU653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AX653" s="9">
+        <v>5</v>
+      </c>
+      <c r="AY653" s="9">
+        <v>6</v>
+      </c>
+      <c r="AZ653" s="9">
+        <v>6</v>
+      </c>
+      <c r="BA653" s="9">
+        <v>6</v>
+      </c>
+      <c r="BB653" s="9">
+        <v>6</v>
+      </c>
+      <c r="BC653" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD653" s="9">
+        <v>5</v>
+      </c>
+      <c r="BE653" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF653" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG653" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH653" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI653" s="9">
+        <v>5</v>
+      </c>
+      <c r="BJ653" s="9">
+        <v>5</v>
+      </c>
+      <c r="BK653" s="9">
+        <v>1</v>
+      </c>
+      <c r="BL653" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM653" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="654" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A654" s="4">
+        <v>45599.79563925926</v>
+      </c>
+      <c r="B654" s="5" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C654" s="5" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D654" s="5">
+        <v>20193017</v>
+      </c>
+      <c r="E654" s="5" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F654" s="6">
+        <v>0.7930555555576575</v>
+      </c>
+      <c r="G654" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H654" s="5">
+        <v>4</v>
+      </c>
+      <c r="I654" s="5">
+        <v>5</v>
+      </c>
+      <c r="J654" s="5">
+        <v>4</v>
+      </c>
+      <c r="K654" s="5">
+        <v>1</v>
+      </c>
+      <c r="L654" s="5">
+        <v>5</v>
+      </c>
+      <c r="M654" s="5">
+        <v>2</v>
+      </c>
+      <c r="N654" s="5">
+        <v>2</v>
+      </c>
+      <c r="O654" s="5">
+        <v>3</v>
+      </c>
+      <c r="P654" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q654" s="5">
+        <v>5</v>
+      </c>
+      <c r="R654" s="5">
+        <v>3</v>
+      </c>
+      <c r="S654" s="5">
+        <v>3</v>
+      </c>
+      <c r="T654" s="5">
+        <v>3</v>
+      </c>
+      <c r="U654" s="5">
+        <v>3</v>
+      </c>
+      <c r="V654" s="5">
+        <v>4</v>
+      </c>
+      <c r="W654" s="5">
+        <v>3</v>
+      </c>
+      <c r="X654" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y654" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z654" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA654" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB654" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC654" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD654" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE654" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF654" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG654" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH654" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI654" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ654" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="655" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A655" s="8">
+        <v>45599.796520300923</v>
+      </c>
+      <c r="B655" s="9" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C655" s="9" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D655" s="9">
+        <v>20235180</v>
+      </c>
+      <c r="E655" s="9" t="s">
+        <v>1464</v>
+      </c>
+      <c r="F655" s="10">
+        <v>0.79513888889050577</v>
+      </c>
+      <c r="G655" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK655" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL655" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM655" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN655" s="9">
+        <v>2</v>
+      </c>
+      <c r="AO655" s="9">
+        <v>1</v>
+      </c>
+      <c r="AP655" s="9">
+        <v>1</v>
+      </c>
+      <c r="AQ655" s="9">
+        <v>2</v>
+      </c>
+      <c r="AR655" s="9">
+        <v>1</v>
+      </c>
+      <c r="AS655" s="9">
+        <v>1</v>
+      </c>
+      <c r="AT655" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU655" s="9">
+        <v>1</v>
+      </c>
+      <c r="AV655" s="9">
+        <v>2</v>
+      </c>
+      <c r="AW655" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX655" s="9">
+        <v>1</v>
+      </c>
+      <c r="AY655" s="9">
+        <v>2</v>
+      </c>
+      <c r="AZ655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BA655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BB655" s="9">
+        <v>2</v>
+      </c>
+      <c r="BC655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BD655" s="9">
+        <v>2</v>
+      </c>
+      <c r="BE655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BF655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BG655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BH655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BI655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BJ655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BK655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BL655" s="9">
+        <v>1</v>
+      </c>
+      <c r="BM655" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="656" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A656" s="4">
+        <v>45599.796633391205</v>
+      </c>
+      <c r="B656" s="5" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C656" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="D656" s="5">
+        <v>20235263</v>
+      </c>
+      <c r="E656" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="F656" s="6">
+        <v>0.78680555555911269</v>
+      </c>
+      <c r="G656" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H656" s="5">
+        <v>4</v>
+      </c>
+      <c r="I656" s="5">
+        <v>3</v>
+      </c>
+      <c r="J656" s="5">
+        <v>3</v>
+      </c>
+      <c r="K656" s="5">
+        <v>3</v>
+      </c>
+      <c r="L656" s="5">
+        <v>2</v>
+      </c>
+      <c r="M656" s="5">
+        <v>4</v>
+      </c>
+      <c r="N656" s="5">
+        <v>3</v>
+      </c>
+      <c r="O656" s="5">
+        <v>3</v>
+      </c>
+      <c r="P656" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q656" s="5">
+        <v>4</v>
+      </c>
+      <c r="R656" s="5">
+        <v>5</v>
+      </c>
+      <c r="S656" s="5">
+        <v>3</v>
+      </c>
+      <c r="T656" s="5">
+        <v>4</v>
+      </c>
+      <c r="U656" s="5">
+        <v>4</v>
+      </c>
+      <c r="V656" s="5">
+        <v>3</v>
+      </c>
+      <c r="W656" s="5">
+        <v>3</v>
+      </c>
+      <c r="X656" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y656" s="5">
+        <v>3</v>
+      </c>
+      <c r="Z656" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA656" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB656" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC656" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD656" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE656" s="5">
+        <v>3</v>
+      </c>
+      <c r="AF656" s="5">
+        <v>4</v>
+      </c>
+      <c r="AG656" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH656" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI656" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ656" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="657" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A657" s="8">
+        <v>45599.799634837967</v>
+      </c>
+      <c r="B657" s="9" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C657" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D657" s="9">
+        <v>20213731</v>
+      </c>
+      <c r="E657" s="9" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F657" s="10">
+        <v>0.77847222222044365</v>
+      </c>
+      <c r="G657" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H657" s="9">
+        <v>2</v>
+      </c>
+      <c r="I657" s="9">
+        <v>3</v>
+      </c>
+      <c r="J657" s="9">
+        <v>3</v>
+      </c>
+      <c r="K657" s="9">
+        <v>3</v>
+      </c>
+      <c r="L657" s="9">
+        <v>4</v>
+      </c>
+      <c r="M657" s="9">
+        <v>4</v>
+      </c>
+      <c r="N657" s="9">
+        <v>4</v>
+      </c>
+      <c r="O657" s="9">
+        <v>4</v>
+      </c>
+      <c r="P657" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q657" s="9">
+        <v>4</v>
+      </c>
+      <c r="R657" s="9">
+        <v>4</v>
+      </c>
+      <c r="S657" s="9">
+        <v>4</v>
+      </c>
+      <c r="T657" s="9">
+        <v>4</v>
+      </c>
+      <c r="U657" s="9">
+        <v>4</v>
+      </c>
+      <c r="V657" s="9">
+        <v>4</v>
+      </c>
+      <c r="W657" s="9">
+        <v>3</v>
+      </c>
+      <c r="X657" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y657" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z657" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA657" s="9">
+        <v>4</v>
+      </c>
+      <c r="AB657" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC657" s="9">
+        <v>4</v>
+      </c>
+      <c r="AD657" s="9">
+        <v>2</v>
+      </c>
+      <c r="AE657" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF657" s="9">
+        <v>3</v>
+      </c>
+      <c r="AG657" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH657" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI657" s="9">
+        <v>4</v>
+      </c>
+      <c r="AJ657" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="658" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A658" s="4">
+        <v>45599.800890138889</v>
+      </c>
+      <c r="B658" s="5" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C658" s="5" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D658" s="5">
+        <v>20233930</v>
+      </c>
+      <c r="E658" s="5" t="s">
+        <v>1470</v>
+      </c>
+      <c r="F658" s="6">
+        <v>0.79930555555620231</v>
+      </c>
+      <c r="G658" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK658" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AM658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AN658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AO658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP658" s="5">
+        <v>2</v>
+      </c>
+      <c r="AQ658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AS658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AT658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AU658" s="5">
+        <v>6</v>
+      </c>
+      <c r="AV658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AW658" s="5">
+        <v>3</v>
+      </c>
+      <c r="AX658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AY658" s="5">
+        <v>5</v>
+      </c>
+      <c r="AZ658" s="5">
+        <v>5</v>
+      </c>
+      <c r="BA658" s="5">
+        <v>5</v>
+      </c>
+      <c r="BB658" s="5">
+        <v>5</v>
+      </c>
+      <c r="BC658" s="5">
+        <v>2</v>
+      </c>
+      <c r="BD658" s="5">
+        <v>5</v>
+      </c>
+      <c r="BE658" s="5">
+        <v>5</v>
+      </c>
+      <c r="BF658" s="5">
+        <v>6</v>
+      </c>
+      <c r="BG658" s="5">
+        <v>5</v>
+      </c>
+      <c r="BH658" s="5">
+        <v>2</v>
+      </c>
+      <c r="BI658" s="5">
+        <v>5</v>
+      </c>
+      <c r="BJ658" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK658" s="5">
+        <v>2</v>
+      </c>
+      <c r="BL658" s="5">
+        <v>1</v>
+      </c>
+      <c r="BM658" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="659" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A659" s="8">
+        <v>45599.801996736111</v>
+      </c>
+      <c r="B659" s="9" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C659" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="D659" s="9">
+        <v>20243031</v>
+      </c>
+      <c r="E659" s="9" t="s">
+        <v>1472</v>
+      </c>
+      <c r="F659" s="10">
+        <v>0.79861111110949423</v>
+      </c>
+      <c r="G659" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H659" s="9">
+        <v>4</v>
+      </c>
+      <c r="I659" s="9">
+        <v>4</v>
+      </c>
+      <c r="J659" s="9">
+        <v>2</v>
+      </c>
+      <c r="K659" s="9">
+        <v>2</v>
+      </c>
+      <c r="L659" s="9">
+        <v>3</v>
+      </c>
+      <c r="M659" s="9">
+        <v>5</v>
+      </c>
+      <c r="N659" s="9">
+        <v>2</v>
+      </c>
+      <c r="O659" s="9">
+        <v>3</v>
+      </c>
+      <c r="P659" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q659" s="9">
+        <v>4</v>
+      </c>
+      <c r="R659" s="9">
+        <v>3</v>
+      </c>
+      <c r="S659" s="9">
+        <v>3</v>
+      </c>
+      <c r="T659" s="9">
+        <v>4</v>
+      </c>
+      <c r="U659" s="9">
+        <v>3</v>
+      </c>
+      <c r="V659" s="9">
+        <v>3</v>
+      </c>
+      <c r="W659" s="9">
+        <v>4</v>
+      </c>
+      <c r="X659" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y659" s="9">
+        <v>3</v>
+      </c>
+      <c r="Z659" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA659" s="9">
+        <v>3</v>
+      </c>
+      <c r="AB659" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC659" s="9">
+        <v>3</v>
+      </c>
+      <c r="AD659" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE659" s="9">
+        <v>5</v>
+      </c>
+      <c r="AF659" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG659" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH659" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI659" s="9">
+        <v>4</v>
+      </c>
+      <c r="AJ659" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="660" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A660" s="4">
+        <v>45599.80208040509</v>
+      </c>
+      <c r="B660" s="5" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C660" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D660" s="5">
+        <v>20242616</v>
+      </c>
+      <c r="E660" s="5" t="s">
+        <v>1474</v>
+      </c>
+      <c r="F660" s="6">
+        <v>0.79166666666424135</v>
+      </c>
+      <c r="G660" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H660" s="5">
+        <v>5</v>
+      </c>
+      <c r="I660" s="5">
+        <v>6</v>
+      </c>
+      <c r="J660" s="5">
+        <v>3</v>
+      </c>
+      <c r="K660" s="5">
+        <v>5</v>
+      </c>
+      <c r="L660" s="5">
+        <v>3</v>
+      </c>
+      <c r="M660" s="5">
+        <v>4</v>
+      </c>
+      <c r="N660" s="5">
+        <v>4</v>
+      </c>
+      <c r="O660" s="5">
+        <v>5</v>
+      </c>
+      <c r="P660" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q660" s="5">
+        <v>1</v>
+      </c>
+      <c r="R660" s="5">
+        <v>5</v>
+      </c>
+      <c r="S660" s="5">
+        <v>6</v>
+      </c>
+      <c r="T660" s="5">
+        <v>5</v>
+      </c>
+      <c r="U660" s="5">
+        <v>4</v>
+      </c>
+      <c r="V660" s="5">
+        <v>5</v>
+      </c>
+      <c r="W660" s="5">
+        <v>5</v>
+      </c>
+      <c r="X660" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y660" s="5">
+        <v>2</v>
+      </c>
+      <c r="Z660" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA660" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB660" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC660" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD660" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE660" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF660" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG660" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH660" s="5">
+        <v>4</v>
+      </c>
+      <c r="AI660" s="5">
+        <v>3</v>
+      </c>
+      <c r="AJ660" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="661" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A661" s="8">
+        <v>45599.802872349537</v>
+      </c>
+      <c r="B661" s="9" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C661" s="9" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D661" s="9">
+        <v>20245169</v>
+      </c>
+      <c r="E661" s="9" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F661" s="10">
+        <v>0.79861111110949423</v>
+      </c>
+      <c r="G661" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK661" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL661" s="9">
+        <v>4</v>
+      </c>
+      <c r="AM661" s="9">
+        <v>5</v>
+      </c>
+      <c r="AN661" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO661" s="9">
+        <v>4</v>
+      </c>
+      <c r="AP661" s="9">
+        <v>4</v>
+      </c>
+      <c r="AQ661" s="9">
+        <v>4</v>
+      </c>
+      <c r="AR661" s="9">
+        <v>5</v>
+      </c>
+      <c r="AS661" s="9">
+        <v>5</v>
+      </c>
+      <c r="AT661" s="9">
+        <v>2</v>
+      </c>
+      <c r="AU661" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV661" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW661" s="9">
+        <v>2</v>
+      </c>
+      <c r="AX661" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY661" s="9">
+        <v>4</v>
+      </c>
+      <c r="AZ661" s="9">
+        <v>4</v>
+      </c>
+      <c r="BA661" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB661" s="9">
+        <v>4</v>
+      </c>
+      <c r="BC661" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD661" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE661" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF661" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG661" s="9">
+        <v>5</v>
+      </c>
+      <c r="BH661" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI661" s="9">
+        <v>4</v>
+      </c>
+      <c r="BJ661" s="9">
+        <v>4</v>
+      </c>
+      <c r="BK661" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL661" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM661" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="662" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A662" s="4">
+        <v>45599.80305962963</v>
+      </c>
+      <c r="B662" s="5" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C662" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="D662" s="5">
+        <v>20223523</v>
+      </c>
+      <c r="E662" s="5" t="s">
+        <v>1479</v>
+      </c>
+      <c r="F662" s="6">
+        <v>0.8006944444423425</v>
+      </c>
+      <c r="G662" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H662" s="5">
+        <v>3</v>
+      </c>
+      <c r="I662" s="5">
+        <v>2</v>
+      </c>
+      <c r="J662" s="5">
+        <v>4</v>
+      </c>
+      <c r="K662" s="5">
+        <v>2</v>
+      </c>
+      <c r="L662" s="5">
+        <v>1</v>
+      </c>
+      <c r="M662" s="5">
+        <v>2</v>
+      </c>
+      <c r="N662" s="5">
+        <v>2</v>
+      </c>
+      <c r="O662" s="5">
+        <v>4</v>
+      </c>
+      <c r="P662" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q662" s="5">
+        <v>1</v>
+      </c>
+      <c r="R662" s="5">
+        <v>5</v>
+      </c>
+      <c r="S662" s="5">
+        <v>4</v>
+      </c>
+      <c r="T662" s="5">
+        <v>4</v>
+      </c>
+      <c r="U662" s="5">
+        <v>3</v>
+      </c>
+      <c r="V662" s="5">
+        <v>4</v>
+      </c>
+      <c r="W662" s="5">
+        <v>4</v>
+      </c>
+      <c r="X662" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y662" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z662" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA662" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB662" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC662" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD662" s="5">
+        <v>3</v>
+      </c>
+      <c r="AE662" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF662" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG662" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH662" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI662" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ662" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="663" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A663" s="8">
+        <v>45599.804565034719</v>
+      </c>
+      <c r="B663" s="9" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C663" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="D663" s="9">
+        <v>20243368</v>
+      </c>
+      <c r="E663" s="9" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F663" s="10">
+        <v>0.80347222222189885</v>
+      </c>
+      <c r="G663" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H663" s="9">
+        <v>4</v>
+      </c>
+      <c r="I663" s="9">
+        <v>2</v>
+      </c>
+      <c r="J663" s="9">
+        <v>4</v>
+      </c>
+      <c r="K663" s="9">
+        <v>2</v>
+      </c>
+      <c r="L663" s="9">
+        <v>2</v>
+      </c>
+      <c r="M663" s="9">
+        <v>2</v>
+      </c>
+      <c r="N663" s="9">
+        <v>3</v>
+      </c>
+      <c r="O663" s="9">
+        <v>5</v>
+      </c>
+      <c r="P663" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q663" s="9">
+        <v>4</v>
+      </c>
+      <c r="R663" s="9">
+        <v>3</v>
+      </c>
+      <c r="S663" s="9">
+        <v>4</v>
+      </c>
+      <c r="T663" s="9">
+        <v>3</v>
+      </c>
+      <c r="U663" s="9">
+        <v>3</v>
+      </c>
+      <c r="V663" s="9">
+        <v>4</v>
+      </c>
+      <c r="W663" s="9">
+        <v>4</v>
+      </c>
+      <c r="X663" s="9">
+        <v>4</v>
+      </c>
+      <c r="Y663" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z663" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA663" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB663" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC663" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD663" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE663" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF663" s="9">
+        <v>4</v>
+      </c>
+      <c r="AG663" s="9">
+        <v>3</v>
+      </c>
+      <c r="AH663" s="9">
+        <v>4</v>
+      </c>
+      <c r="AI663" s="9">
+        <v>5</v>
+      </c>
+      <c r="AJ663" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="664" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A664" s="4">
+        <v>45599.804772430551</v>
+      </c>
+      <c r="B664" s="5" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C664" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D664" s="5">
+        <v>20202418</v>
+      </c>
+      <c r="E664" s="5" t="s">
+        <v>1483</v>
+      </c>
+      <c r="F664" s="6">
+        <v>0.80347222222189885</v>
+      </c>
+      <c r="G664" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H664" s="5">
+        <v>2</v>
+      </c>
+      <c r="I664" s="5">
+        <v>5</v>
+      </c>
+      <c r="J664" s="5">
+        <v>5</v>
+      </c>
+      <c r="K664" s="5">
+        <v>4</v>
+      </c>
+      <c r="L664" s="5">
+        <v>2</v>
+      </c>
+      <c r="M664" s="5">
+        <v>2</v>
+      </c>
+      <c r="N664" s="5">
+        <v>5</v>
+      </c>
+      <c r="O664" s="5">
+        <v>5</v>
+      </c>
+      <c r="P664" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q664" s="5">
+        <v>2</v>
+      </c>
+      <c r="R664" s="5">
+        <v>5</v>
+      </c>
+      <c r="S664" s="5">
+        <v>5</v>
+      </c>
+      <c r="T664" s="5">
+        <v>2</v>
+      </c>
+      <c r="U664" s="5">
+        <v>2</v>
+      </c>
+      <c r="V664" s="5">
+        <v>5</v>
+      </c>
+      <c r="W664" s="5">
+        <v>5</v>
+      </c>
+      <c r="X664" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y664" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z664" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA664" s="5">
+        <v>5</v>
+      </c>
+      <c r="AB664" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC664" s="5">
+        <v>5</v>
+      </c>
+      <c r="AD664" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE664" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF664" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG664" s="5">
+        <v>5</v>
+      </c>
+      <c r="AH664" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI664" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ664" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="665" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A665" s="8">
+        <v>45599.806643460644</v>
+      </c>
+      <c r="B665" s="9" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C665" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D665" s="9">
+        <v>20201046</v>
+      </c>
+      <c r="E665" s="9" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F665" s="10">
+        <v>0.80138888888905058</v>
+      </c>
+      <c r="G665" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H665" s="9">
+        <v>1</v>
+      </c>
+      <c r="I665" s="9">
+        <v>6</v>
+      </c>
+      <c r="J665" s="9">
+        <v>4</v>
+      </c>
+      <c r="K665" s="9">
+        <v>6</v>
+      </c>
+      <c r="L665" s="9">
+        <v>2</v>
+      </c>
+      <c r="M665" s="9">
+        <v>2</v>
+      </c>
+      <c r="N665" s="9">
+        <v>5</v>
+      </c>
+      <c r="O665" s="9">
+        <v>6</v>
+      </c>
+      <c r="P665" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q665" s="9">
+        <v>1</v>
+      </c>
+      <c r="R665" s="9">
+        <v>6</v>
+      </c>
+      <c r="S665" s="9">
+        <v>6</v>
+      </c>
+      <c r="T665" s="9">
+        <v>1</v>
+      </c>
+      <c r="U665" s="9">
+        <v>3</v>
+      </c>
+      <c r="V665" s="9">
+        <v>6</v>
+      </c>
+      <c r="W665" s="9">
+        <v>6</v>
+      </c>
+      <c r="X665" s="9">
+        <v>6</v>
+      </c>
+      <c r="Y665" s="9">
+        <v>6</v>
+      </c>
+      <c r="Z665" s="9">
+        <v>3</v>
+      </c>
+      <c r="AA665" s="9">
+        <v>6</v>
+      </c>
+      <c r="AB665" s="9">
+        <v>6</v>
+      </c>
+      <c r="AC665" s="9">
+        <v>6</v>
+      </c>
+      <c r="AD665" s="9">
+        <v>4</v>
+      </c>
+      <c r="AE665" s="9">
+        <v>2</v>
+      </c>
+      <c r="AF665" s="9">
+        <v>6</v>
+      </c>
+      <c r="AG665" s="9">
+        <v>6</v>
+      </c>
+      <c r="AH665" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI665" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ665" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="666" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A666" s="4">
+        <v>45599.807292546291</v>
+      </c>
+      <c r="B666" s="5" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C666" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D666" s="5">
+        <v>20242205</v>
+      </c>
+      <c r="E666" s="5" t="s">
+        <v>1487</v>
+      </c>
+      <c r="F666" s="6">
+        <v>0.804861111115315</v>
+      </c>
+      <c r="G666" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H666" s="5">
+        <v>2</v>
+      </c>
+      <c r="I666" s="5">
+        <v>5</v>
+      </c>
+      <c r="J666" s="5">
+        <v>2</v>
+      </c>
+      <c r="K666" s="5">
+        <v>1</v>
+      </c>
+      <c r="L666" s="5">
+        <v>5</v>
+      </c>
+      <c r="M666" s="5">
+        <v>4</v>
+      </c>
+      <c r="N666" s="5">
+        <v>3</v>
+      </c>
+      <c r="O666" s="5">
+        <v>2</v>
+      </c>
+      <c r="P666" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q666" s="5">
+        <v>5</v>
+      </c>
+      <c r="R666" s="5">
+        <v>3</v>
+      </c>
+      <c r="S666" s="5">
+        <v>2</v>
+      </c>
+      <c r="T666" s="5">
+        <v>3</v>
+      </c>
+      <c r="U666" s="5">
+        <v>4</v>
+      </c>
+      <c r="V666" s="5">
+        <v>3</v>
+      </c>
+      <c r="W666" s="5">
+        <v>4</v>
+      </c>
+      <c r="X666" s="5">
+        <v>4</v>
+      </c>
+      <c r="Y666" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z666" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA666" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB666" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC666" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD666" s="5">
+        <v>2</v>
+      </c>
+      <c r="AE666" s="5">
+        <v>2</v>
+      </c>
+      <c r="AF666" s="5">
+        <v>2</v>
+      </c>
+      <c r="AG666" s="5">
+        <v>2</v>
+      </c>
+      <c r="AH666" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI666" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ666" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="667" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A667" s="8">
+        <v>45599.809763124998</v>
+      </c>
+      <c r="B667" s="9" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C667" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D667" s="9">
+        <v>20222327</v>
+      </c>
+      <c r="E667" s="9" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F667" s="10">
+        <v>0.80555555555474712</v>
+      </c>
+      <c r="G667" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK667" s="9">
+        <v>4</v>
+      </c>
+      <c r="AL667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AM667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AO667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AP667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AR667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AS667" s="9">
+        <v>4</v>
+      </c>
+      <c r="AT667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AU667" s="9">
+        <v>4</v>
+      </c>
+      <c r="AV667" s="9">
+        <v>4</v>
+      </c>
+      <c r="AW667" s="9">
+        <v>4</v>
+      </c>
+      <c r="AX667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AY667" s="9">
+        <v>3</v>
+      </c>
+      <c r="AZ667" s="9">
+        <v>3</v>
+      </c>
+      <c r="BA667" s="9">
+        <v>2</v>
+      </c>
+      <c r="BB667" s="9">
+        <v>1</v>
+      </c>
+      <c r="BC667" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD667" s="9">
+        <v>2</v>
+      </c>
+      <c r="BE667" s="9">
+        <v>3</v>
+      </c>
+      <c r="BF667" s="9">
+        <v>3</v>
+      </c>
+      <c r="BG667" s="9">
+        <v>3</v>
+      </c>
+      <c r="BH667" s="9">
+        <v>3</v>
+      </c>
+      <c r="BI667" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ667" s="9">
+        <v>3</v>
+      </c>
+      <c r="BK667" s="9">
+        <v>3</v>
+      </c>
+      <c r="BL667" s="9">
+        <v>3</v>
+      </c>
+      <c r="BM667" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="668" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A668" s="4">
+        <v>45599.810346921295</v>
+      </c>
+      <c r="B668" s="5" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C668" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D668" s="5">
+        <v>20245113</v>
+      </c>
+      <c r="E668" s="5" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F668" s="6">
+        <v>0.80833333333430346</v>
+      </c>
+      <c r="G668" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK668" s="5">
+        <v>3</v>
+      </c>
+      <c r="AL668" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM668" s="5">
+        <v>3</v>
+      </c>
+      <c r="AN668" s="5">
+        <v>3</v>
+      </c>
+      <c r="AO668" s="5">
+        <v>2</v>
+      </c>
+      <c r="AP668" s="5">
+        <v>4</v>
+      </c>
+      <c r="AQ668" s="5">
+        <v>3</v>
+      </c>
+      <c r="AR668" s="5">
+        <v>3</v>
+      </c>
+      <c r="AS668" s="5">
+        <v>4</v>
+      </c>
+      <c r="AT668" s="5">
+        <v>4</v>
+      </c>
+      <c r="AU668" s="5">
+        <v>2</v>
+      </c>
+      <c r="AV668" s="5">
+        <v>3</v>
+      </c>
+      <c r="AW668" s="5">
+        <v>4</v>
+      </c>
+      <c r="AX668" s="5">
+        <v>4</v>
+      </c>
+      <c r="AY668" s="5">
+        <v>3</v>
+      </c>
+      <c r="AZ668" s="5">
+        <v>4</v>
+      </c>
+      <c r="BA668" s="5">
+        <v>3</v>
+      </c>
+      <c r="BB668" s="5">
+        <v>3</v>
+      </c>
+      <c r="BC668" s="5">
+        <v>3</v>
+      </c>
+      <c r="BD668" s="5">
+        <v>3</v>
+      </c>
+      <c r="BE668" s="5">
+        <v>3</v>
+      </c>
+      <c r="BF668" s="5">
+        <v>4</v>
+      </c>
+      <c r="BG668" s="5">
+        <v>4</v>
+      </c>
+      <c r="BH668" s="5">
+        <v>4</v>
+      </c>
+      <c r="BI668" s="5">
+        <v>2</v>
+      </c>
+      <c r="BJ668" s="5">
+        <v>3</v>
+      </c>
+      <c r="BK668" s="5">
+        <v>3</v>
+      </c>
+      <c r="BL668" s="5">
+        <v>3</v>
+      </c>
+      <c r="BM668" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="669" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A669" s="8">
+        <v>45599.810631608794</v>
+      </c>
+      <c r="B669" s="9" t="s">
+        <v>872</v>
+      </c>
+      <c r="C669" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D669" s="9">
+        <v>20197126</v>
+      </c>
+      <c r="E669" s="9" t="s">
+        <v>873</v>
+      </c>
+      <c r="F669" s="10">
+        <v>0.80902777778101154</v>
+      </c>
+      <c r="G669" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H669" s="9">
+        <v>2</v>
+      </c>
+      <c r="I669" s="9">
+        <v>5</v>
+      </c>
+      <c r="J669" s="9">
+        <v>5</v>
+      </c>
+      <c r="K669" s="9">
+        <v>5</v>
+      </c>
+      <c r="L669" s="9">
+        <v>1</v>
+      </c>
+      <c r="M669" s="9">
+        <v>2</v>
+      </c>
+      <c r="N669" s="9">
+        <v>4</v>
+      </c>
+      <c r="O669" s="9">
+        <v>5</v>
+      </c>
+      <c r="P669" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q669" s="9">
+        <v>4</v>
+      </c>
+      <c r="R669" s="9">
+        <v>6</v>
+      </c>
+      <c r="S669" s="9">
+        <v>6</v>
+      </c>
+      <c r="T669" s="9">
+        <v>4</v>
+      </c>
+      <c r="U669" s="9">
+        <v>4</v>
+      </c>
+      <c r="V669" s="9">
+        <v>6</v>
+      </c>
+      <c r="W669" s="9">
+        <v>5</v>
+      </c>
+      <c r="X669" s="9">
+        <v>6</v>
+      </c>
+      <c r="Y669" s="9">
+        <v>5</v>
+      </c>
+      <c r="Z669" s="9">
+        <v>4</v>
+      </c>
+      <c r="AA669" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB669" s="9">
+        <v>6</v>
+      </c>
+      <c r="AC669" s="9">
+        <v>5</v>
+      </c>
+      <c r="AD669" s="9">
+        <v>3</v>
+      </c>
+      <c r="AE669" s="9">
+        <v>3</v>
+      </c>
+      <c r="AF669" s="9">
+        <v>5</v>
+      </c>
+      <c r="AG669" s="9">
+        <v>5</v>
+      </c>
+      <c r="AH669" s="9">
+        <v>2</v>
+      </c>
+      <c r="AI669" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ669" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="670" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A670" s="4">
+        <v>45599.812439965273</v>
+      </c>
+      <c r="B670" s="5" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C670" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D670" s="5">
+        <v>20202324</v>
+      </c>
+      <c r="E670" s="5" t="s">
+        <v>1493</v>
+      </c>
+      <c r="F670" s="6">
+        <v>0.81041666666715173</v>
+      </c>
+      <c r="G670" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H670" s="5">
+        <v>1</v>
+      </c>
+      <c r="I670" s="5">
+        <v>6</v>
+      </c>
+      <c r="J670" s="5">
+        <v>6</v>
+      </c>
+      <c r="K670" s="5">
+        <v>2</v>
+      </c>
+      <c r="L670" s="5">
+        <v>3</v>
+      </c>
+      <c r="M670" s="5">
+        <v>5</v>
+      </c>
+      <c r="N670" s="5">
+        <v>3</v>
+      </c>
+      <c r="O670" s="5">
+        <v>4</v>
+      </c>
+      <c r="P670" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q670" s="5">
+        <v>3</v>
+      </c>
+      <c r="R670" s="5">
+        <v>3</v>
+      </c>
+      <c r="S670" s="5">
+        <v>3</v>
+      </c>
+      <c r="T670" s="5">
+        <v>4</v>
+      </c>
+      <c r="U670" s="5">
+        <v>4</v>
+      </c>
+      <c r="V670" s="5">
+        <v>3</v>
+      </c>
+      <c r="W670" s="5">
+        <v>4</v>
+      </c>
+      <c r="X670" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y670" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z670" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA670" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB670" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC670" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD670" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE670" s="5">
+        <v>4</v>
+      </c>
+      <c r="AF670" s="5">
+        <v>3</v>
+      </c>
+      <c r="AG670" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH670" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI670" s="5">
+        <v>4</v>
+      </c>
+      <c r="AJ670" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="671" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A671" s="8">
+        <v>45599.812822870372</v>
+      </c>
+      <c r="B671" s="9" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C671" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D671" s="9">
+        <v>20243613</v>
+      </c>
+      <c r="E671" s="9" t="s">
+        <v>1495</v>
+      </c>
+      <c r="F671" s="10">
+        <v>0.80763888888759539</v>
+      </c>
+      <c r="G671" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK671" s="9">
+        <v>2</v>
+      </c>
+      <c r="AL671" s="9">
+        <v>5</v>
+      </c>
+      <c r="AM671" s="9">
+        <v>4</v>
+      </c>
+      <c r="AN671" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO671" s="9">
+        <v>2</v>
+      </c>
+      <c r="AP671" s="9">
+        <v>3</v>
+      </c>
+      <c r="AQ671" s="9">
+        <v>5</v>
+      </c>
+      <c r="AR671" s="9">
+        <v>4</v>
+      </c>
+      <c r="AS671" s="9">
+        <v>6</v>
+      </c>
+      <c r="AT671" s="9">
+        <v>1</v>
+      </c>
+      <c r="AU671" s="9">
+        <v>5</v>
+      </c>
+      <c r="AV671" s="9">
+        <v>5</v>
+      </c>
+      <c r="AW671" s="9">
+        <v>1</v>
+      </c>
+      <c r="AX671" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY671" s="9">
+        <v>5</v>
+      </c>
+      <c r="AZ671" s="9">
+        <v>5</v>
+      </c>
+      <c r="BA671" s="9">
+        <v>4</v>
+      </c>
+      <c r="BB671" s="9">
+        <v>5</v>
+      </c>
+      <c r="BC671" s="9">
+        <v>2</v>
+      </c>
+      <c r="BD671" s="9">
+        <v>4</v>
+      </c>
+      <c r="BE671" s="9">
+        <v>2</v>
+      </c>
+      <c r="BF671" s="9">
+        <v>4</v>
+      </c>
+      <c r="BG671" s="9">
+        <v>2</v>
+      </c>
+      <c r="BH671" s="9">
+        <v>2</v>
+      </c>
+      <c r="BI671" s="9">
+        <v>3</v>
+      </c>
+      <c r="BJ671" s="9">
+        <v>5</v>
+      </c>
+      <c r="BK671" s="9">
+        <v>2</v>
+      </c>
+      <c r="BL671" s="9">
+        <v>2</v>
+      </c>
+      <c r="BM671" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="672" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A672" s="4">
+        <v>45599.813596817126</v>
+      </c>
+      <c r="B672" s="5" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C672" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D672" s="5">
+        <v>20212840</v>
+      </c>
+      <c r="E672" s="5" t="s">
+        <v>1497</v>
+      </c>
+      <c r="F672" s="6">
+        <v>0.3125</v>
+      </c>
+      <c r="G672" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H672" s="5">
+        <v>3</v>
+      </c>
+      <c r="I672" s="5">
+        <v>3</v>
+      </c>
+      <c r="J672" s="5">
+        <v>4</v>
+      </c>
+      <c r="K672" s="5">
+        <v>4</v>
+      </c>
+      <c r="L672" s="5">
+        <v>3</v>
+      </c>
+      <c r="M672" s="5">
+        <v>2</v>
+      </c>
+      <c r="N672" s="5">
+        <v>4</v>
+      </c>
+      <c r="O672" s="5">
+        <v>4</v>
+      </c>
+      <c r="P672" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q672" s="5">
+        <v>3</v>
+      </c>
+      <c r="R672" s="5">
+        <v>3</v>
+      </c>
+      <c r="S672" s="5">
+        <v>3</v>
+      </c>
+      <c r="T672" s="5">
+        <v>4</v>
+      </c>
+      <c r="U672" s="5">
+        <v>4</v>
+      </c>
+      <c r="V672" s="5">
+        <v>3</v>
+      </c>
+      <c r="W672" s="5">
+        <v>3</v>
+      </c>
+      <c r="X672" s="5">
+        <v>3</v>
+      </c>
+      <c r="Y672" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z672" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA672" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB672" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC672" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD672" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE672" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF672" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG672" s="5">
+        <v>3</v>
+      </c>
+      <c r="AH672" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI672" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ672" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="673" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A673" s="18">
+        <v>45599.814953530091</v>
+      </c>
+      <c r="B673" s="19" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C673" s="19" t="s">
+        <v>1499</v>
+      </c>
+      <c r="D673" s="19">
+        <v>20233301</v>
+      </c>
+      <c r="E673" s="19" t="s">
+        <v>1500</v>
+      </c>
+      <c r="F673" s="20">
+        <v>0.8125</v>
+      </c>
+      <c r="G673" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H673" s="26"/>
+      <c r="I673" s="26"/>
+      <c r="J673" s="26"/>
+      <c r="K673" s="26"/>
+      <c r="L673" s="26"/>
+      <c r="M673" s="26"/>
+      <c r="N673" s="26"/>
+      <c r="O673" s="26"/>
+      <c r="P673" s="26"/>
+      <c r="Q673" s="26"/>
+      <c r="R673" s="26"/>
+      <c r="S673" s="26"/>
+      <c r="T673" s="26"/>
+      <c r="U673" s="26"/>
+      <c r="V673" s="26"/>
+      <c r="W673" s="26"/>
+      <c r="X673" s="26"/>
+      <c r="Y673" s="26"/>
+      <c r="Z673" s="26"/>
+      <c r="AA673" s="26"/>
+      <c r="AB673" s="26"/>
+      <c r="AC673" s="26"/>
+      <c r="AD673" s="26"/>
+      <c r="AE673" s="26"/>
+      <c r="AF673" s="26"/>
+      <c r="AG673" s="26"/>
+      <c r="AH673" s="26"/>
+      <c r="AI673" s="26"/>
+      <c r="AJ673" s="26"/>
+      <c r="AK673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AL673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AM673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AN673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AO673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AP673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AQ673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AR673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AS673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AT673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AU673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AV673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AW673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AX673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AY673" s="19">
+        <v>4</v>
+      </c>
+      <c r="AZ673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BA673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BB673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BC673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BD673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BE673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BF673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BG673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BH673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BI673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BJ673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BK673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BL673" s="19">
+        <v>4</v>
+      </c>
+      <c r="BM673" s="22">
         <v>4</v>
       </c>
     </row>

</xml_diff>